<commit_message>
Alteração nos requisitos do sistema.
</commit_message>
<xml_diff>
--- a/documentacao/requisitos.xlsx
+++ b/documentacao/requisitos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rocha\Desktop\Data-Source\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71345AE6-C924-410E-A8FA-CA1E9FEBFDDE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE926D00-4368-426A-933C-F3973D3B1531}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="101">
   <si>
     <t>Histórico de alterações do documento</t>
   </si>
@@ -351,9 +351,6 @@
     <t>O software deverá ter níveis de acesso</t>
   </si>
   <si>
-    <t>O software deverá ter autenticação de usuários</t>
-  </si>
-  <si>
     <t>6.1</t>
   </si>
   <si>
@@ -372,15 +369,9 @@
     <t>O software deverá kickar do servidor users com softwares possivelmente maliosos instalados em seu device</t>
   </si>
   <si>
-    <t>O software deverá bloquear no servidor a entrada de users que anteriormente tentaram acessá-lo com softwares possivelmente maliosos instalados em seu device</t>
-  </si>
-  <si>
     <t>O software deverá permitir a exibição de usuários</t>
   </si>
   <si>
-    <t>7.1</t>
-  </si>
-  <si>
     <t>O software deverá permitir ao administrador a exclusão de um ou mais usuários</t>
   </si>
   <si>
@@ -391,6 +382,54 @@
   </si>
   <si>
     <t>O sofware deverá guardar o log</t>
+  </si>
+  <si>
+    <t>Essencial</t>
+  </si>
+  <si>
+    <t>Importante</t>
+  </si>
+  <si>
+    <t>Desejável</t>
+  </si>
+  <si>
+    <t>O software deverá bloquear no servidor a entrada de users que anteriormente tentaram acessá-lo com softwares possivelmente maliosos</t>
+  </si>
+  <si>
+    <t>O software deverá ter autenticação de usuários para a entrada no sistema</t>
+  </si>
+  <si>
+    <t>Não Funcional</t>
+  </si>
+  <si>
+    <t>Funcional</t>
+  </si>
+  <si>
+    <t>Gerson Santos</t>
+  </si>
+  <si>
+    <t>Proposto</t>
+  </si>
+  <si>
+    <t>Mínima</t>
+  </si>
+  <si>
+    <t>Alta</t>
+  </si>
+  <si>
+    <t>Baixa</t>
+  </si>
+  <si>
+    <t>Média</t>
+  </si>
+  <si>
+    <t>Máxima</t>
+  </si>
+  <si>
+    <t>O software deverá permitir ao administrador a alteração de um ou mais usuários</t>
+  </si>
+  <si>
+    <t>8.1</t>
   </si>
 </sst>
 </file>
@@ -663,36 +702,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -726,6 +735,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -748,8 +787,19 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="medium">
+          <color theme="0"/>
+        </top>
+        <bottom style="medium">
+          <color theme="0"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -769,6 +819,581 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color theme="0"/>
+        </left>
+        <right style="medium">
+          <color theme="0"/>
+        </right>
+        <top style="medium">
+          <color theme="0"/>
+        </top>
+        <bottom style="medium">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color theme="0"/>
+        </left>
+        <right style="medium">
+          <color theme="0"/>
+        </right>
+        <top style="medium">
+          <color theme="0"/>
+        </top>
+        <bottom style="medium">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color theme="0"/>
+        </left>
+        <right style="medium">
+          <color theme="0"/>
+        </right>
+        <top style="medium">
+          <color theme="0"/>
+        </top>
+        <bottom style="medium">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color theme="0"/>
+        </left>
+        <right style="medium">
+          <color theme="0"/>
+        </right>
+        <top style="medium">
+          <color theme="0"/>
+        </top>
+        <bottom style="medium">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color theme="0"/>
+        </left>
+        <right style="medium">
+          <color theme="0"/>
+        </right>
+        <top style="medium">
+          <color theme="0"/>
+        </top>
+        <bottom style="medium">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color theme="0"/>
+        </left>
+        <right style="medium">
+          <color theme="0"/>
+        </right>
+        <top style="medium">
+          <color theme="0"/>
+        </top>
+        <bottom style="medium">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color theme="0"/>
+        </left>
+        <right style="medium">
+          <color theme="0"/>
+        </right>
+        <top style="medium">
+          <color theme="0"/>
+        </top>
+        <bottom style="medium">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color theme="0"/>
+        </left>
+        <right style="medium">
+          <color theme="0"/>
+        </right>
+        <top style="medium">
+          <color theme="0"/>
+        </top>
+        <bottom style="medium">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color theme="0"/>
+        </left>
+        <right style="medium">
+          <color theme="0"/>
+        </right>
+        <top style="medium">
+          <color theme="0"/>
+        </top>
+        <bottom style="medium">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color theme="0"/>
+        </left>
+        <right style="medium">
+          <color theme="0"/>
+        </right>
+        <top style="medium">
+          <color theme="0"/>
+        </top>
+        <bottom style="medium">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color theme="0"/>
+        </left>
+        <right style="medium">
+          <color theme="0"/>
+        </right>
+        <top style="medium">
+          <color theme="0"/>
+        </top>
+        <bottom style="medium">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color theme="0"/>
+        </left>
+        <right style="medium">
+          <color theme="0"/>
+        </right>
+        <top style="medium">
+          <color theme="0"/>
+        </top>
+        <bottom style="medium">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color theme="0"/>
+        </left>
+        <right style="medium">
+          <color theme="0"/>
+        </right>
+        <top style="medium">
+          <color theme="0"/>
+        </top>
+        <bottom style="medium">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color theme="0"/>
+        </left>
+        <right style="medium">
+          <color theme="0"/>
+        </right>
+        <top style="medium">
+          <color theme="0"/>
+        </top>
+        <bottom style="medium">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color theme="0"/>
+        </left>
+        <right style="medium">
+          <color theme="0"/>
+        </right>
+        <top style="medium">
+          <color theme="0"/>
+        </top>
+        <bottom style="medium">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color theme="0"/>
+        </left>
+        <right style="medium">
+          <color theme="0"/>
+        </right>
+        <top style="medium">
+          <color theme="0"/>
+        </top>
+        <bottom style="medium">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color theme="0"/>
+        </right>
+        <top style="medium">
+          <color theme="0"/>
+        </top>
+        <bottom style="medium">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -822,594 +1447,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color theme="0"/>
-        </left>
-        <right/>
-        <top style="medium">
-          <color theme="0"/>
-        </top>
-        <bottom style="medium">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color theme="0"/>
-        </left>
-        <right style="medium">
-          <color theme="0"/>
-        </right>
-        <top style="medium">
-          <color theme="0"/>
-        </top>
-        <bottom style="medium">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color theme="0"/>
-        </left>
-        <right style="medium">
-          <color theme="0"/>
-        </right>
-        <top style="medium">
-          <color theme="0"/>
-        </top>
-        <bottom style="medium">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color theme="0"/>
-        </left>
-        <right style="medium">
-          <color theme="0"/>
-        </right>
-        <top style="medium">
-          <color theme="0"/>
-        </top>
-        <bottom style="medium">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color theme="0"/>
-        </left>
-        <right style="medium">
-          <color theme="0"/>
-        </right>
-        <top style="medium">
-          <color theme="0"/>
-        </top>
-        <bottom style="medium">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color theme="0"/>
-        </left>
-        <right style="medium">
-          <color theme="0"/>
-        </right>
-        <top style="medium">
-          <color theme="0"/>
-        </top>
-        <bottom style="medium">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color theme="0"/>
-        </left>
-        <right style="medium">
-          <color theme="0"/>
-        </right>
-        <top style="medium">
-          <color theme="0"/>
-        </top>
-        <bottom style="medium">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color theme="0"/>
-        </left>
-        <right style="medium">
-          <color theme="0"/>
-        </right>
-        <top style="medium">
-          <color theme="0"/>
-        </top>
-        <bottom style="medium">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color theme="0"/>
-        </left>
-        <right style="medium">
-          <color theme="0"/>
-        </right>
-        <top style="medium">
-          <color theme="0"/>
-        </top>
-        <bottom style="medium">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color theme="0"/>
-        </left>
-        <right style="medium">
-          <color theme="0"/>
-        </right>
-        <top style="medium">
-          <color theme="0"/>
-        </top>
-        <bottom style="medium">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color theme="0"/>
-        </left>
-        <right style="medium">
-          <color theme="0"/>
-        </right>
-        <top style="medium">
-          <color theme="0"/>
-        </top>
-        <bottom style="medium">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color theme="0"/>
-        </left>
-        <right style="medium">
-          <color theme="0"/>
-        </right>
-        <top style="medium">
-          <color theme="0"/>
-        </top>
-        <bottom style="medium">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color theme="0"/>
-        </left>
-        <right style="medium">
-          <color theme="0"/>
-        </right>
-        <top style="medium">
-          <color theme="0"/>
-        </top>
-        <bottom style="medium">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color theme="0"/>
-        </left>
-        <right style="medium">
-          <color theme="0"/>
-        </right>
-        <top style="medium">
-          <color theme="0"/>
-        </top>
-        <bottom style="medium">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color theme="0"/>
-        </left>
-        <right style="medium">
-          <color theme="0"/>
-        </right>
-        <top style="medium">
-          <color theme="0"/>
-        </top>
-        <bottom style="medium">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color theme="0"/>
-        </left>
-        <right style="medium">
-          <color theme="0"/>
-        </right>
-        <top style="medium">
-          <color theme="0"/>
-        </top>
-        <bottom style="medium">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color theme="0"/>
-        </left>
-        <right style="medium">
-          <color theme="0"/>
-        </right>
-        <top style="medium">
-          <color theme="0"/>
-        </top>
-        <bottom style="medium">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color theme="0"/>
-        </right>
-        <top style="medium">
-          <color theme="0"/>
-        </top>
-        <bottom style="medium">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1622,7 +1661,7 @@
     <tableColumn id="1" xr3:uid="{3254B635-2323-4E75-BB71-FDB8433D84AA}" name="Versão" dataDxfId="25"/>
     <tableColumn id="2" xr3:uid="{C2D5BAAF-DA6E-4E32-A4FB-784A019C5633}" name="Alteração efetuada" dataDxfId="24"/>
     <tableColumn id="3" xr3:uid="{1592629F-8DF0-4B3E-A0F2-8634A8164A2A}" name="Responsável " dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{EEFC847D-DD1C-4AAA-9864-5127AFD71971}" name="Data " dataDxfId="0">
+    <tableColumn id="4" xr3:uid="{EEFC847D-DD1C-4AAA-9864-5127AFD71971}" name="Data " dataDxfId="22">
       <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1631,27 +1670,27 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="requisitos" displayName="requisitos" ref="D4:U71" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1" headerRowBorderDxfId="22" tableBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="requisitos" displayName="requisitos" ref="D4:U71" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18">
   <autoFilter ref="D4:U71" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Descrição do Requisito" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Objetivo / Estratégia de Negócio" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Prioridade" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Versão do Requisito" dataDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Tipo Requisito " dataDxfId="16"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Complexidade" dataDxfId="15"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Solicitante" dataDxfId="14"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Responsável" dataDxfId="13"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Validador" dataDxfId="12"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Critérios de Aceitação" dataDxfId="11"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Dependência Internas entre Requisitos  (Rastreabilidade)" dataDxfId="10"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Dependências Externas entre Requisitos (Rastreabilidade)" dataDxfId="9"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Data da Criação" dataDxfId="8"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Data Última Alteração" dataDxfId="7"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Responsável pela última alteração" dataDxfId="6"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Motivo Última Alteração" dataDxfId="5"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Documentação de Apoio" dataDxfId="4"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Situação do Requisito" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Descrição do Requisito" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Objetivo / Estratégia de Negócio" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Prioridade" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Versão do Requisito" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Tipo Requisito " dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Complexidade" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Solicitante" dataDxfId="11"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Responsável" dataDxfId="10"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Validador" dataDxfId="9"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Critérios de Aceitação" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Dependência Internas entre Requisitos  (Rastreabilidade)" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Dependências Externas entre Requisitos (Rastreabilidade)" dataDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Data da Criação" dataDxfId="5"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Data Última Alteração" dataDxfId="4"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Responsável pela última alteração" dataDxfId="3"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Motivo Última Alteração" dataDxfId="2"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Documentação de Apoio" dataDxfId="1"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Situação do Requisito" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1998,12 +2037,12 @@
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2"/>
     <row r="4" spans="2:5" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -2031,7 +2070,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
@@ -2161,28 +2200,28 @@
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2"/>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="25"/>
     </row>
     <row r="36" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="14" t="s">
+      <c r="B36" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
+      <c r="C36" s="25"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="25"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2"/>
     <row r="38" spans="2:5" hidden="1" x14ac:dyDescent="0.2"/>
@@ -2213,94 +2252,94 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V73"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E30" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="4" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="D35" sqref="D35"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="3.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="49.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" style="1" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="21.28515625" style="1" customWidth="1"/>
     <col min="8" max="8" width="18.85546875" style="1" customWidth="1"/>
     <col min="9" max="9" width="16.7109375" style="7" customWidth="1"/>
     <col min="10" max="10" width="25.42578125" style="7" customWidth="1"/>
-    <col min="11" max="11" width="20.5703125" style="7" customWidth="1"/>
+    <col min="11" max="11" width="20.5703125" style="7" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="16.28515625" style="7" customWidth="1"/>
-    <col min="13" max="13" width="26.140625" style="7" customWidth="1"/>
+    <col min="13" max="13" width="26.140625" style="7" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="22.42578125" style="1" customWidth="1"/>
     <col min="15" max="15" width="30.5703125" style="7" customWidth="1"/>
     <col min="16" max="16" width="16" style="7" customWidth="1"/>
     <col min="17" max="17" width="14.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16" style="1" customWidth="1"/>
-    <col min="20" max="20" width="16.140625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="17" style="1" customWidth="1"/>
+    <col min="20" max="20" width="16.140625" style="1" hidden="1" customWidth="1"/>
     <col min="21" max="21" width="25.42578125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="14.42578125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="3.7109375" style="1" customWidth="1"/>
     <col min="23" max="16384" width="9.140625" style="1" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" s="24" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="28"/>
+    <row r="1" spans="2:21" s="14" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="18"/>
       <c r="R1" s="10"/>
-      <c r="U1" s="28"/>
-    </row>
-    <row r="2" spans="2:21" s="24" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E2" s="21"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15" t="s">
+      <c r="U1" s="18"/>
+    </row>
+    <row r="2" spans="2:21" s="14" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E2" s="32"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="17" t="s">
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="19">
+      <c r="P2" s="30">
         <f ca="1">TODAY()</f>
         <v>43716</v>
       </c>
-      <c r="R2" s="29"/>
-      <c r="U2" s="28"/>
-    </row>
-    <row r="3" spans="2:21" s="24" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E3" s="22"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="18"/>
-      <c r="P3" s="20"/>
-      <c r="U3" s="30"/>
+      <c r="R2" s="19"/>
+      <c r="U2" s="18"/>
+    </row>
+    <row r="3" spans="2:21" s="14" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="33"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="31"/>
+      <c r="U3" s="20"/>
     </row>
     <row r="4" spans="2:21" s="2" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="13" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -2361,22 +2400,34 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="31">
+    <row r="5" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="21">
         <v>1</v>
       </c>
-      <c r="C5" s="31"/>
+      <c r="C5" s="21"/>
       <c r="D5" s="11" t="s">
         <v>38</v>
       </c>
       <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
+      <c r="L5" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
@@ -2389,26 +2440,43 @@
       <c r="R5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S5" s="4"/>
+      <c r="S5" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
       <c r="T5" s="4"/>
-      <c r="U5" s="4"/>
-    </row>
-    <row r="6" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="31"/>
-      <c r="C6" s="31" t="s">
+      <c r="U5" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="21"/>
+      <c r="C6" s="21" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>39</v>
       </c>
       <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
+      <c r="F6" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
+      <c r="L6" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -2421,26 +2489,43 @@
       <c r="R6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S6" s="4"/>
+      <c r="S6" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
       <c r="T6" s="4"/>
-      <c r="U6" s="4"/>
-    </row>
-    <row r="7" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="31"/>
-      <c r="C7" s="31" t="s">
+      <c r="U6" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="21"/>
+      <c r="C7" s="21" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>40</v>
       </c>
       <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
+      <c r="F7" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
+      <c r="L7" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
@@ -2453,26 +2538,43 @@
       <c r="R7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S7" s="4"/>
+      <c r="S7" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>Adequação ao escopo do projeto</v>
+      </c>
       <c r="T7" s="4"/>
-      <c r="U7" s="4"/>
-    </row>
-    <row r="8" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="31"/>
-      <c r="C8" s="31" t="s">
+      <c r="U7" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="21"/>
+      <c r="C8" s="21" t="s">
         <v>41</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>59</v>
       </c>
       <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
+      <c r="F8" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
+      <c r="L8" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
@@ -2485,26 +2587,43 @@
       <c r="R8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S8" s="4"/>
+      <c r="S8" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
       <c r="T8" s="4"/>
-      <c r="U8" s="4"/>
-    </row>
-    <row r="9" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="31">
+      <c r="U8" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="21">
         <v>2</v>
       </c>
-      <c r="C9" s="31"/>
+      <c r="C9" s="21"/>
       <c r="D9" s="11" t="s">
         <v>42</v>
       </c>
       <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
+      <c r="F9" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
+      <c r="L9" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
@@ -2517,26 +2636,43 @@
       <c r="R9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S9" s="4"/>
+      <c r="S9" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
       <c r="T9" s="4"/>
-      <c r="U9" s="4"/>
-    </row>
-    <row r="10" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="31"/>
-      <c r="C10" s="31" t="s">
+      <c r="U9" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="21"/>
+      <c r="C10" s="21" t="s">
         <v>43</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>44</v>
       </c>
       <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
+      <c r="F10" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
+      <c r="L10" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
@@ -2549,26 +2685,43 @@
       <c r="R10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S10" s="4"/>
+      <c r="S10" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
       <c r="T10" s="4"/>
-      <c r="U10" s="4"/>
-    </row>
-    <row r="11" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="31"/>
-      <c r="C11" s="31" t="s">
+      <c r="U10" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="21"/>
+      <c r="C11" s="21" t="s">
         <v>45</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>46</v>
       </c>
       <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
+      <c r="F11" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
+      <c r="L11" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
@@ -2581,26 +2734,43 @@
       <c r="R11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S11" s="4"/>
+      <c r="S11" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
       <c r="T11" s="4"/>
-      <c r="U11" s="4"/>
-    </row>
-    <row r="12" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="31">
+      <c r="U11" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="21">
         <v>3</v>
       </c>
-      <c r="C12" s="31"/>
+      <c r="C12" s="21"/>
       <c r="D12" s="11" t="s">
         <v>58</v>
       </c>
       <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
+      <c r="F12" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
+      <c r="L12" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
@@ -2613,26 +2783,43 @@
       <c r="R12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S12" s="4"/>
+      <c r="S12" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
       <c r="T12" s="4"/>
-      <c r="U12" s="4"/>
-    </row>
-    <row r="13" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="31"/>
-      <c r="C13" s="31" t="s">
+      <c r="U12" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="21"/>
+      <c r="C13" s="21" t="s">
         <v>48</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>47</v>
       </c>
       <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
+      <c r="F13" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
+      <c r="L13" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
@@ -2645,26 +2832,43 @@
       <c r="R13" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S13" s="4"/>
+      <c r="S13" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
       <c r="T13" s="4"/>
-      <c r="U13" s="4"/>
-    </row>
-    <row r="14" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="31"/>
-      <c r="C14" s="31" t="s">
+      <c r="U13" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="21"/>
+      <c r="C14" s="21" t="s">
         <v>50</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
+      <c r="F14" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
+      <c r="L14" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
@@ -2677,26 +2881,43 @@
       <c r="R14" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S14" s="4"/>
+      <c r="S14" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
       <c r="T14" s="4"/>
-      <c r="U14" s="4"/>
-    </row>
-    <row r="15" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="31"/>
-      <c r="C15" s="31" t="s">
+      <c r="U14" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="21"/>
+      <c r="C15" s="21" t="s">
         <v>52</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
+      <c r="F15" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
+      <c r="L15" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
@@ -2709,26 +2930,43 @@
       <c r="R15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S15" s="4"/>
+      <c r="S15" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
       <c r="T15" s="4"/>
-      <c r="U15" s="4"/>
-    </row>
-    <row r="16" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="31"/>
-      <c r="C16" s="31" t="s">
+      <c r="U15" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="21"/>
+      <c r="C16" s="21" t="s">
         <v>54</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>53</v>
       </c>
       <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
+      <c r="F16" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
+      <c r="L16" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
@@ -2741,26 +2979,43 @@
       <c r="R16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S16" s="4"/>
+      <c r="S16" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
       <c r="T16" s="4"/>
-      <c r="U16" s="4"/>
-    </row>
-    <row r="17" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="31"/>
-      <c r="C17" s="31" t="s">
+      <c r="U16" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="21"/>
+      <c r="C17" s="21" t="s">
         <v>55</v>
       </c>
       <c r="D17" s="12" t="s">
         <v>60</v>
       </c>
       <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
+      <c r="F17" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
+      <c r="L17" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
@@ -2773,26 +3028,43 @@
       <c r="R17" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S17" s="4"/>
+      <c r="S17" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>Adequação ao escopo do projeto</v>
+      </c>
       <c r="T17" s="4"/>
-      <c r="U17" s="4"/>
-    </row>
-    <row r="18" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="31"/>
-      <c r="C18" s="31" t="s">
+      <c r="U17" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="21"/>
+      <c r="C18" s="21" t="s">
         <v>62</v>
       </c>
       <c r="D18" s="12" t="s">
         <v>56</v>
       </c>
       <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
+      <c r="F18" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
+      <c r="L18" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
@@ -2805,26 +3077,43 @@
       <c r="R18" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S18" s="4"/>
+      <c r="S18" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
       <c r="T18" s="4"/>
-      <c r="U18" s="4"/>
-    </row>
-    <row r="19" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="31"/>
-      <c r="C19" s="31" t="s">
+      <c r="U18" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="21"/>
+      <c r="C19" s="21" t="s">
         <v>63</v>
       </c>
       <c r="D19" s="12" t="s">
         <v>61</v>
       </c>
       <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
+      <c r="F19" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
+      <c r="L19" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
@@ -2837,26 +3126,43 @@
       <c r="R19" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S19" s="4"/>
+      <c r="S19" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
       <c r="T19" s="4"/>
-      <c r="U19" s="4"/>
-    </row>
-    <row r="20" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="31"/>
-      <c r="C20" s="31" t="s">
+      <c r="U19" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="21"/>
+      <c r="C20" s="21" t="s">
         <v>64</v>
       </c>
       <c r="D20" s="12" t="s">
         <v>57</v>
       </c>
       <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
+      <c r="F20" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
+      <c r="L20" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
@@ -2869,26 +3175,43 @@
       <c r="R20" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S20" s="4"/>
+      <c r="S20" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
       <c r="T20" s="4"/>
-      <c r="U20" s="4"/>
-    </row>
-    <row r="21" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="31">
+      <c r="U20" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="21">
         <v>4</v>
       </c>
-      <c r="C21" s="31"/>
+      <c r="C21" s="21"/>
       <c r="D21" s="11" t="s">
         <v>67</v>
       </c>
       <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
+      <c r="F21" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
+      <c r="L21" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
@@ -2901,26 +3224,43 @@
       <c r="R21" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S21" s="4"/>
+      <c r="S21" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
       <c r="T21" s="4"/>
-      <c r="U21" s="4"/>
-    </row>
-    <row r="22" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="31"/>
-      <c r="C22" s="31" t="s">
+      <c r="U21" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="21"/>
+      <c r="C22" s="21" t="s">
         <v>68</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>69</v>
       </c>
       <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
+      <c r="F22" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
+      <c r="L22" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
@@ -2933,26 +3273,43 @@
       <c r="R22" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S22" s="4"/>
+      <c r="S22" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
       <c r="T22" s="4"/>
-      <c r="U22" s="4"/>
-    </row>
-    <row r="23" spans="2:21" s="32" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="31"/>
-      <c r="C23" s="31" t="s">
+      <c r="U22" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="2:21" s="22" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="21"/>
+      <c r="C23" s="21" t="s">
         <v>70</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
+      <c r="F23" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
+      <c r="L23" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
@@ -2965,26 +3322,43 @@
       <c r="R23" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S23" s="4"/>
+      <c r="S23" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
       <c r="T23" s="4"/>
-      <c r="U23" s="4"/>
-    </row>
-    <row r="24" spans="2:21" s="32" customFormat="1" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="31"/>
-      <c r="C24" s="31" t="s">
-        <v>79</v>
+      <c r="U23" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="2:21" s="22" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="21"/>
+      <c r="C24" s="21" t="s">
+        <v>78</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
+      <c r="F24" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
+      <c r="L24" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
@@ -2997,26 +3371,43 @@
       <c r="R24" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S24" s="4"/>
+      <c r="S24" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
       <c r="T24" s="4"/>
-      <c r="U24" s="4"/>
-    </row>
-    <row r="25" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="31">
+      <c r="U24" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="21">
         <v>5</v>
       </c>
-      <c r="C25" s="31"/>
+      <c r="C25" s="21"/>
       <c r="D25" s="11" t="s">
         <v>71</v>
       </c>
       <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
+      <c r="F25" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
+      <c r="L25" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
@@ -3029,26 +3420,43 @@
       <c r="R25" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S25" s="4"/>
+      <c r="S25" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
       <c r="T25" s="4"/>
-      <c r="U25" s="4"/>
-    </row>
-    <row r="26" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="31"/>
-      <c r="C26" s="31" t="s">
+      <c r="U25" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="21"/>
+      <c r="C26" s="21" t="s">
         <v>72</v>
       </c>
       <c r="D26" s="11" t="s">
         <v>73</v>
       </c>
       <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
+      <c r="F26" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
+      <c r="L26" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="M26" s="4"/>
       <c r="N26" s="4"/>
       <c r="O26" s="4"/>
@@ -3061,26 +3469,43 @@
       <c r="R26" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S26" s="4"/>
+      <c r="S26" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
       <c r="T26" s="4"/>
-      <c r="U26" s="4"/>
-    </row>
-    <row r="27" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="31">
+      <c r="U26" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="21">
         <v>6</v>
       </c>
-      <c r="C27" s="31"/>
-      <c r="D27" s="32" t="s">
-        <v>74</v>
+      <c r="C27" s="21"/>
+      <c r="D27" s="22" t="s">
+        <v>89</v>
       </c>
       <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
+      <c r="F27" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
+      <c r="L27" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
@@ -3093,26 +3518,43 @@
       <c r="R27" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S27" s="4"/>
+      <c r="S27" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
       <c r="T27" s="4"/>
-      <c r="U27" s="4"/>
-    </row>
-    <row r="28" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="31"/>
-      <c r="C28" s="31" t="s">
+      <c r="U27" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="21"/>
+      <c r="C28" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="D28" s="32" t="s">
-        <v>76</v>
-      </c>
       <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
+      <c r="F28" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
+      <c r="L28" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
@@ -3125,26 +3567,43 @@
       <c r="R28" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S28" s="4"/>
+      <c r="S28" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
       <c r="T28" s="4"/>
-      <c r="U28" s="4"/>
-    </row>
-    <row r="29" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="31"/>
-      <c r="C29" s="31" t="s">
+      <c r="U28" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="21"/>
+      <c r="C29" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="D29" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="D29" s="11" t="s">
-        <v>78</v>
-      </c>
       <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
+      <c r="F29" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
+      <c r="L29" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
@@ -3157,24 +3616,43 @@
       <c r="R29" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S29" s="4"/>
+      <c r="S29" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
       <c r="T29" s="4"/>
-      <c r="U29" s="4"/>
-    </row>
-    <row r="30" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
+      <c r="U29" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="21">
+        <v>7</v>
+      </c>
+      <c r="C30" s="21"/>
       <c r="D30" s="11" t="s">
         <v>65</v>
       </c>
       <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
+      <c r="F30" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
+      <c r="L30" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
@@ -3187,26 +3665,43 @@
       <c r="R30" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S30" s="4"/>
+      <c r="S30" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
       <c r="T30" s="4"/>
-      <c r="U30" s="4"/>
-    </row>
-    <row r="31" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="31">
-        <v>7</v>
-      </c>
-      <c r="C31" s="31"/>
+      <c r="U30" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="21">
+        <v>8</v>
+      </c>
+      <c r="C31" s="21"/>
       <c r="D31" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
+      <c r="F31" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
+      <c r="L31" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="M31" s="4"/>
       <c r="N31" s="4"/>
       <c r="O31" s="4"/>
@@ -3219,26 +3714,43 @@
       <c r="R31" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S31" s="4"/>
+      <c r="S31" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
       <c r="T31" s="4"/>
-      <c r="U31" s="4"/>
-    </row>
-    <row r="32" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="31"/>
-      <c r="C32" s="31" t="s">
-        <v>83</v>
+      <c r="U31" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="21"/>
+      <c r="C32" s="21" t="s">
+        <v>100</v>
       </c>
       <c r="D32" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
+      <c r="G32" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
+      <c r="L32" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
       <c r="O32" s="4"/>
@@ -3251,26 +3763,43 @@
       <c r="R32" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S32" s="4"/>
+      <c r="S32" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
       <c r="T32" s="4"/>
-      <c r="U32" s="4"/>
-    </row>
-    <row r="33" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="31">
-        <v>8</v>
-      </c>
-      <c r="C33" s="31"/>
+      <c r="U32" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="21">
+        <v>9</v>
+      </c>
+      <c r="C33" s="21"/>
       <c r="D33" s="11" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
+      <c r="F33" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
+      <c r="L33" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
@@ -3283,31 +3812,48 @@
       <c r="R33" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S33" s="4"/>
+      <c r="S33" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
       <c r="T33" s="4"/>
-      <c r="U33" s="4"/>
-    </row>
-    <row r="34" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="31">
-        <v>9</v>
-      </c>
-      <c r="C34" s="31"/>
-      <c r="D34" s="32" t="s">
-        <v>87</v>
+      <c r="U33" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="34" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="21">
+        <v>10</v>
+      </c>
+      <c r="C34" s="21"/>
+      <c r="D34" s="11" t="s">
+        <v>99</v>
       </c>
       <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
+      <c r="F34" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
+      <c r="L34" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
       <c r="P34" s="5">
-        <v>43714</v>
+        <v>43716</v>
       </c>
       <c r="Q34" s="5">
         <v>43716</v>
@@ -3315,35 +3861,67 @@
       <c r="R34" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="S34" s="4"/>
+      <c r="S34" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
       <c r="T34" s="4"/>
-      <c r="U34" s="4"/>
-    </row>
-    <row r="35" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="31"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="11"/>
+      <c r="U34" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="21">
+        <v>11</v>
+      </c>
+      <c r="C35" s="21"/>
+      <c r="D35" s="22" t="s">
+        <v>84</v>
+      </c>
       <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
+      <c r="F35" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
+      <c r="L35" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="M35" s="4"/>
       <c r="N35" s="4"/>
       <c r="O35" s="4"/>
-      <c r="P35" s="5"/>
-      <c r="Q35" s="4"/>
-      <c r="R35" s="4"/>
-      <c r="S35" s="4"/>
+      <c r="P35" s="5">
+        <v>43714</v>
+      </c>
+      <c r="Q35" s="5">
+        <v>43716</v>
+      </c>
+      <c r="R35" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="S35" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>Adequação ao escopo do projeto</v>
+      </c>
       <c r="T35" s="4"/>
-      <c r="U35" s="4"/>
-    </row>
-    <row r="36" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="31"/>
-      <c r="C36" s="31"/>
+      <c r="U35" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="36" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
       <c r="D36" s="11"/>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
@@ -3363,9 +3941,9 @@
       <c r="T36" s="4"/>
       <c r="U36" s="4"/>
     </row>
-    <row r="37" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="31"/>
-      <c r="C37" s="31"/>
+    <row r="37" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="21"/>
+      <c r="C37" s="21"/>
       <c r="D37" s="11"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
@@ -3385,9 +3963,9 @@
       <c r="T37" s="4"/>
       <c r="U37" s="4"/>
     </row>
-    <row r="38" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="31"/>
-      <c r="C38" s="31"/>
+    <row r="38" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="21"/>
+      <c r="C38" s="21"/>
       <c r="D38" s="11"/>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
@@ -3407,9 +3985,9 @@
       <c r="T38" s="4"/>
       <c r="U38" s="4"/>
     </row>
-    <row r="39" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="31"/>
-      <c r="C39" s="31"/>
+    <row r="39" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="21"/>
+      <c r="C39" s="21"/>
       <c r="D39" s="11"/>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
@@ -3429,9 +4007,9 @@
       <c r="T39" s="4"/>
       <c r="U39" s="4"/>
     </row>
-    <row r="40" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="31"/>
-      <c r="C40" s="31"/>
+    <row r="40" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="21"/>
+      <c r="C40" s="21"/>
       <c r="D40" s="11"/>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
@@ -3451,9 +4029,9 @@
       <c r="T40" s="4"/>
       <c r="U40" s="4"/>
     </row>
-    <row r="41" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="31"/>
-      <c r="C41" s="31"/>
+    <row r="41" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="21"/>
+      <c r="C41" s="21"/>
       <c r="D41" s="11"/>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
@@ -3473,9 +4051,9 @@
       <c r="T41" s="4"/>
       <c r="U41" s="4"/>
     </row>
-    <row r="42" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="31"/>
-      <c r="C42" s="31"/>
+    <row r="42" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="21"/>
+      <c r="C42" s="21"/>
       <c r="D42" s="11"/>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
@@ -3495,9 +4073,9 @@
       <c r="T42" s="4"/>
       <c r="U42" s="4"/>
     </row>
-    <row r="43" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="31"/>
-      <c r="C43" s="31"/>
+    <row r="43" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="21"/>
+      <c r="C43" s="21"/>
       <c r="D43" s="11"/>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
@@ -3517,9 +4095,9 @@
       <c r="T43" s="4"/>
       <c r="U43" s="4"/>
     </row>
-    <row r="44" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="31"/>
-      <c r="C44" s="31"/>
+    <row r="44" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="21"/>
+      <c r="C44" s="21"/>
       <c r="D44" s="11"/>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
@@ -3539,9 +4117,9 @@
       <c r="T44" s="4"/>
       <c r="U44" s="4"/>
     </row>
-    <row r="45" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="31"/>
-      <c r="C45" s="31"/>
+    <row r="45" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="21"/>
+      <c r="C45" s="21"/>
       <c r="D45" s="11"/>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
@@ -3561,9 +4139,9 @@
       <c r="T45" s="4"/>
       <c r="U45" s="4"/>
     </row>
-    <row r="46" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="31"/>
-      <c r="C46" s="31"/>
+    <row r="46" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="21"/>
+      <c r="C46" s="21"/>
       <c r="D46" s="11"/>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
@@ -3583,9 +4161,9 @@
       <c r="T46" s="4"/>
       <c r="U46" s="4"/>
     </row>
-    <row r="47" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="31"/>
-      <c r="C47" s="31"/>
+    <row r="47" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="21"/>
+      <c r="C47" s="21"/>
       <c r="D47" s="11"/>
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
@@ -3605,9 +4183,9 @@
       <c r="T47" s="4"/>
       <c r="U47" s="4"/>
     </row>
-    <row r="48" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="31"/>
-      <c r="C48" s="31"/>
+    <row r="48" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="21"/>
+      <c r="C48" s="21"/>
       <c r="D48" s="11"/>
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
@@ -3627,9 +4205,9 @@
       <c r="T48" s="4"/>
       <c r="U48" s="4"/>
     </row>
-    <row r="49" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="31"/>
-      <c r="C49" s="31"/>
+    <row r="49" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="21"/>
+      <c r="C49" s="21"/>
       <c r="D49" s="11"/>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
@@ -3649,9 +4227,9 @@
       <c r="T49" s="4"/>
       <c r="U49" s="4"/>
     </row>
-    <row r="50" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="31"/>
-      <c r="C50" s="31"/>
+    <row r="50" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="21"/>
+      <c r="C50" s="21"/>
       <c r="D50" s="11"/>
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
@@ -3671,9 +4249,9 @@
       <c r="T50" s="4"/>
       <c r="U50" s="4"/>
     </row>
-    <row r="51" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="31"/>
-      <c r="C51" s="31"/>
+    <row r="51" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="21"/>
+      <c r="C51" s="21"/>
       <c r="D51" s="11"/>
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
@@ -3693,9 +4271,9 @@
       <c r="T51" s="4"/>
       <c r="U51" s="4"/>
     </row>
-    <row r="52" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="31"/>
-      <c r="C52" s="31"/>
+    <row r="52" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="21"/>
+      <c r="C52" s="21"/>
       <c r="D52" s="11"/>
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
@@ -3715,9 +4293,9 @@
       <c r="T52" s="4"/>
       <c r="U52" s="4"/>
     </row>
-    <row r="53" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="31"/>
-      <c r="C53" s="31"/>
+    <row r="53" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="21"/>
+      <c r="C53" s="21"/>
       <c r="D53" s="11"/>
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
@@ -3737,9 +4315,9 @@
       <c r="T53" s="4"/>
       <c r="U53" s="4"/>
     </row>
-    <row r="54" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="31"/>
-      <c r="C54" s="31"/>
+    <row r="54" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="21"/>
+      <c r="C54" s="21"/>
       <c r="D54" s="11"/>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
@@ -3759,9 +4337,9 @@
       <c r="T54" s="4"/>
       <c r="U54" s="4"/>
     </row>
-    <row r="55" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="31"/>
-      <c r="C55" s="31"/>
+    <row r="55" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="21"/>
+      <c r="C55" s="21"/>
       <c r="D55" s="11"/>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
@@ -3781,9 +4359,9 @@
       <c r="T55" s="4"/>
       <c r="U55" s="4"/>
     </row>
-    <row r="56" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="31"/>
-      <c r="C56" s="31"/>
+    <row r="56" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="21"/>
+      <c r="C56" s="21"/>
       <c r="D56" s="11"/>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
@@ -3803,9 +4381,9 @@
       <c r="T56" s="4"/>
       <c r="U56" s="4"/>
     </row>
-    <row r="57" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="31"/>
-      <c r="C57" s="31"/>
+    <row r="57" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="21"/>
+      <c r="C57" s="21"/>
       <c r="D57" s="11"/>
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
@@ -3825,9 +4403,9 @@
       <c r="T57" s="4"/>
       <c r="U57" s="4"/>
     </row>
-    <row r="58" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="31"/>
-      <c r="C58" s="31"/>
+    <row r="58" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="21"/>
+      <c r="C58" s="21"/>
       <c r="D58" s="11"/>
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
@@ -3847,9 +4425,9 @@
       <c r="T58" s="4"/>
       <c r="U58" s="4"/>
     </row>
-    <row r="59" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="31"/>
-      <c r="C59" s="31"/>
+    <row r="59" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="21"/>
+      <c r="C59" s="21"/>
       <c r="D59" s="11"/>
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
@@ -3869,9 +4447,9 @@
       <c r="T59" s="4"/>
       <c r="U59" s="4"/>
     </row>
-    <row r="60" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="31"/>
-      <c r="C60" s="31"/>
+    <row r="60" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="21"/>
+      <c r="C60" s="21"/>
       <c r="D60" s="11"/>
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
@@ -3891,9 +4469,9 @@
       <c r="T60" s="4"/>
       <c r="U60" s="4"/>
     </row>
-    <row r="61" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="31"/>
-      <c r="C61" s="31"/>
+    <row r="61" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="21"/>
+      <c r="C61" s="21"/>
       <c r="D61" s="11"/>
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
@@ -3913,9 +4491,9 @@
       <c r="T61" s="4"/>
       <c r="U61" s="4"/>
     </row>
-    <row r="62" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="31"/>
-      <c r="C62" s="31"/>
+    <row r="62" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="21"/>
+      <c r="C62" s="21"/>
       <c r="D62" s="11"/>
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
@@ -3935,9 +4513,9 @@
       <c r="T62" s="4"/>
       <c r="U62" s="4"/>
     </row>
-    <row r="63" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="31"/>
-      <c r="C63" s="31"/>
+    <row r="63" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="21"/>
+      <c r="C63" s="21"/>
       <c r="D63" s="11"/>
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
@@ -3957,9 +4535,9 @@
       <c r="T63" s="4"/>
       <c r="U63" s="4"/>
     </row>
-    <row r="64" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="31"/>
-      <c r="C64" s="31"/>
+    <row r="64" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="21"/>
+      <c r="C64" s="21"/>
       <c r="D64" s="11"/>
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
@@ -3979,9 +4557,9 @@
       <c r="T64" s="4"/>
       <c r="U64" s="4"/>
     </row>
-    <row r="65" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="31"/>
-      <c r="C65" s="31"/>
+    <row r="65" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="21"/>
+      <c r="C65" s="21"/>
       <c r="D65" s="11"/>
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
@@ -4001,9 +4579,9 @@
       <c r="T65" s="4"/>
       <c r="U65" s="4"/>
     </row>
-    <row r="66" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="31"/>
-      <c r="C66" s="31"/>
+    <row r="66" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="21"/>
+      <c r="C66" s="21"/>
       <c r="D66" s="11"/>
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
@@ -4023,9 +4601,9 @@
       <c r="T66" s="4"/>
       <c r="U66" s="4"/>
     </row>
-    <row r="67" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="31"/>
-      <c r="C67" s="31"/>
+    <row r="67" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="21"/>
+      <c r="C67" s="21"/>
       <c r="D67" s="11"/>
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
@@ -4045,9 +4623,9 @@
       <c r="T67" s="4"/>
       <c r="U67" s="4"/>
     </row>
-    <row r="68" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="31"/>
-      <c r="C68" s="31"/>
+    <row r="68" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="21"/>
+      <c r="C68" s="21"/>
       <c r="D68" s="11"/>
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
@@ -4067,9 +4645,9 @@
       <c r="T68" s="4"/>
       <c r="U68" s="4"/>
     </row>
-    <row r="69" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="31"/>
-      <c r="C69" s="31"/>
+    <row r="69" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="21"/>
+      <c r="C69" s="21"/>
       <c r="D69" s="11"/>
       <c r="E69" s="4"/>
       <c r="F69" s="4"/>
@@ -4089,9 +4667,9 @@
       <c r="T69" s="4"/>
       <c r="U69" s="4"/>
     </row>
-    <row r="70" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="31"/>
-      <c r="C70" s="31"/>
+    <row r="70" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="21"/>
+      <c r="C70" s="21"/>
       <c r="D70" s="11"/>
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
@@ -4111,9 +4689,9 @@
       <c r="T70" s="4"/>
       <c r="U70" s="4"/>
     </row>
-    <row r="71" spans="2:21" s="32" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="31"/>
-      <c r="C71" s="31"/>
+    <row r="71" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="21"/>
+      <c r="C71" s="21"/>
       <c r="D71" s="11"/>
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
@@ -4134,7 +4712,7 @@
       <c r="U71" s="4"/>
     </row>
     <row r="72" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="N72" s="33"/>
+      <c r="N72" s="23"/>
     </row>
     <row r="73" spans="2:21" hidden="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -4164,7 +4742,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J71" xr:uid="{27F19A6C-524E-45E8-ABAC-AFD7E242F75B}">
       <formula1>"Gerson Santos,Célia Taniwaki,José Yoshihiro,Alex Barreira"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K5:K71 R5:R71" xr:uid="{08414707-FD34-4214-AC27-E0609CF58BB6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R5:R71 K5:K71" xr:uid="{08414707-FD34-4214-AC27-E0609CF58BB6}">
       <formula1>"Fernando Abreu,João Vinícius,Kessi Santana,Thalita Igwe,Vitoria Ferreira"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5:L71" xr:uid="{7BE54147-1A46-412A-BF1D-8B94526A2CB5}">

</xml_diff>

<commit_message>
Alteração nos Requisitos e projeto Yoshi.
</commit_message>
<xml_diff>
--- a/documentacao/requisitos.xlsx
+++ b/documentacao/requisitos.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rocha\Desktop\Data-Source\documentacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Data-Source\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE926D00-4368-426A-933C-F3973D3B1531}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Histórico de Alterações" sheetId="4" r:id="rId1"/>
     <sheet name="Documentação e Matriz" sheetId="1" r:id="rId2"/>
+    <sheet name="Product Backlog" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="113">
   <si>
     <t>Histórico de alterações do documento</t>
   </si>
@@ -54,6 +55,9 @@
     <t>Vitoria Ferreira</t>
   </si>
   <si>
+    <t>08/30/2019</t>
+  </si>
+  <si>
     <t>1.1</t>
   </si>
   <si>
@@ -66,7 +70,13 @@
     <t>Revisão de requisitos</t>
   </si>
   <si>
+    <t>1.3</t>
+  </si>
+  <si>
     <t>Revisão e inclusão de requisitos</t>
+  </si>
+  <si>
+    <t>1.4</t>
   </si>
   <si>
     <t>Documentação e Matriz de Rastreabilidade dos Requisitos - Versão 5.0</t>
@@ -246,75 +256,195 @@
     <t>O sotware deverá ter conexão com um banco de dados</t>
   </si>
   <si>
+    <t>Essencial</t>
+  </si>
+  <si>
+    <t>Funcional</t>
+  </si>
+  <si>
+    <t>Mínima</t>
+  </si>
+  <si>
+    <t>Gerson Santos</t>
+  </si>
+  <si>
+    <t>Fernando Abreu</t>
+  </si>
+  <si>
+    <t>Exemplo executado em até 5 seg</t>
+  </si>
+  <si>
+    <t>Proposto</t>
+  </si>
+  <si>
     <t>O banco de dados deverá ser MS SQL Server</t>
   </si>
   <si>
+    <t>Importante</t>
+  </si>
+  <si>
     <t>O banco de dados deverá estar hospedado na Cloud</t>
   </si>
   <si>
-    <t>1.3</t>
+    <t>A cloud de hospedagem do banco de dados será o Azure</t>
+  </si>
+  <si>
+    <t>Não Funcional</t>
   </si>
   <si>
     <t>O sotware deverá ser desenvolvido na linguagem de programação Java</t>
   </si>
   <si>
+    <t>Alta</t>
+  </si>
+  <si>
+    <t>O cliente deverá ter a JVM instalada em seu computador</t>
+  </si>
+  <si>
+    <t>Baixa</t>
+  </si>
+  <si>
+    <t>O cliente deverá ter o JRE instalado em seu computador</t>
+  </si>
+  <si>
+    <t>O sofware deverá ter um dashboard com as informações do hardware do device</t>
+  </si>
+  <si>
+    <t>Média</t>
+  </si>
+  <si>
+    <t>O software deverá coletar as informações de hardware do device</t>
+  </si>
+  <si>
+    <t>O software deverá coletar os processos em execução do sistema operacional</t>
+  </si>
+  <si>
+    <t>O software deverá coletar o consumo de memória do device</t>
+  </si>
+  <si>
+    <t>O software deverá coletar o consumo do disco do device</t>
+  </si>
+  <si>
+    <t>O software deverá coletar o desempenho da placa de vídeo</t>
+  </si>
+  <si>
+    <t>O software deverá coletar informações sobre a conexão com a internet</t>
+  </si>
+  <si>
+    <t>O software deverá coletar o consumo do processador</t>
+  </si>
+  <si>
+    <t>O software deverá encerrar processos "desnecessários" do sistema operacional</t>
+  </si>
+  <si>
+    <t>Máxima</t>
+  </si>
+  <si>
+    <t>O software deverá agir na proteção do servidor</t>
+  </si>
+  <si>
+    <t>O software deverá ter uma lista de softwares possivelmente maliciosos</t>
+  </si>
+  <si>
+    <t>O software deverá kickar do servidor users com softwares possivelmente maliosos instalados em seu device</t>
+  </si>
+  <si>
+    <t>O software deverá bloquear no servidor a entrada de users que anteriormente tentaram acessá-lo com softwares possivelmente maliosos</t>
+  </si>
+  <si>
+    <t>O software deverá ter uma tela de cadastro em que os próprios usuários se cadastram</t>
+  </si>
+  <si>
+    <t>O software deverá ter níveis de acesso</t>
+  </si>
+  <si>
+    <t>O software deverá ter autenticação de usuários para a entrada no sistema</t>
+  </si>
+  <si>
+    <t>O software deverá ter uma tela de login</t>
+  </si>
+  <si>
+    <t>O software deverá emitir um alerta visual, caso os dados de login sejam inválidos</t>
+  </si>
+  <si>
+    <t>O software deverá fazer integração com o PowerBI</t>
+  </si>
+  <si>
+    <t>O software deverá permitir a exibição de usuários</t>
+  </si>
+  <si>
+    <t>O software deverá permitir ao administrador a exibição de usuários em cada servidor</t>
+  </si>
+  <si>
+    <t>O software deverá permitir ao administrador a exclusão de um ou mais usuários</t>
+  </si>
+  <si>
+    <t>O software deverá permitir ao administrador a alteração de um ou mais usuários</t>
+  </si>
+  <si>
+    <t>O sofware deverá guardar o log</t>
+  </si>
+  <si>
+    <t>https://github.com/oshi/oshi</t>
+  </si>
+  <si>
+    <t>Projetado</t>
+  </si>
+  <si>
+    <t>O software deverá ter uma API que capta as informações do usuário</t>
+  </si>
+  <si>
+    <t>O software deverá uma tela com os dados do usuário e do seu device</t>
+  </si>
+  <si>
+    <t>O software deverá permitir que o usuário encerre a sessão que está logado</t>
+  </si>
+  <si>
+    <t>O software deverá permitir ao administrador o bloqueio de usuários aos servidores de jogos</t>
+  </si>
+  <si>
+    <t>O software deverá ter uma tela de cadastro em que o administrador possa cadastrar outros usuários (NOC)</t>
+  </si>
+  <si>
+    <t>O software deverá permitir aos usuários (jogadores) o reset de senha</t>
+  </si>
+  <si>
+    <t>O software deverá ter uma sala de espera, para os jogadores que não conseguiram se conectar em nenhum servidor</t>
+  </si>
+  <si>
+    <t>O software deverá permitir ao administrador o reset de senha dos usuários do NOC</t>
+  </si>
+  <si>
+    <t>O software deverá permitir ao administrador o bloqueio de usuários NOC</t>
+  </si>
+  <si>
+    <t>O software deverá permitir ao administrador o desbloqueio de usuários NOC</t>
+  </si>
+  <si>
+    <t>O software deverá ter salas de jogos</t>
+  </si>
+  <si>
     <t>2.1</t>
   </si>
   <si>
-    <t>O cliente deverá ter a JVM instalada em seu computador</t>
-  </si>
-  <si>
     <t>2.2</t>
   </si>
   <si>
-    <t>O cliente deverá ter o JRE instalado em seu computador</t>
-  </si>
-  <si>
-    <t>O software deverá coletar as informações de hardware do device</t>
-  </si>
-  <si>
     <t>3.1</t>
   </si>
   <si>
-    <t>O software deverá coletar os processos em execução do sistema operacional</t>
-  </si>
-  <si>
     <t>3.2</t>
   </si>
   <si>
-    <t>O software deverá coletar o consumo de memória do device</t>
-  </si>
-  <si>
     <t>3.3</t>
   </si>
   <si>
-    <t>O software deverá coletar o consumo do disco do device</t>
-  </si>
-  <si>
     <t>3.4</t>
   </si>
   <si>
     <t>3.5</t>
   </si>
   <si>
-    <t>O software deverá coletar informações sobre a conexão com a internet</t>
-  </si>
-  <si>
-    <t>O software deverá encerrar processos "desnecessários" do sistema operacional</t>
-  </si>
-  <si>
-    <t>O sofware deverá ter um dashboard com as informações do hardware do device</t>
-  </si>
-  <si>
-    <t>A cloud de hospedagem do banco de dados será o Azure</t>
-  </si>
-  <si>
-    <t>O software deverá coletar o desempenho da placa de vídeo</t>
-  </si>
-  <si>
-    <t>O software deverá coletar o consumo do processador</t>
-  </si>
-  <si>
     <t>3.6</t>
   </si>
   <si>
@@ -324,119 +454,26 @@
     <t>3.8</t>
   </si>
   <si>
-    <t>O software deverá fazer integração com o PowerBI</t>
-  </si>
-  <si>
-    <t>1.4</t>
-  </si>
-  <si>
-    <t>O software deverá agir na proteção do servidor</t>
-  </si>
-  <si>
-    <t>4.1</t>
-  </si>
-  <si>
-    <t>O software deverá ter uma lista de softwares possivelmente maliciosos</t>
-  </si>
-  <si>
-    <t>4.2</t>
-  </si>
-  <si>
-    <t>O software deverá ter uma tela de cadastro de usuários</t>
+    <t>Desejável</t>
+  </si>
+  <si>
+    <t>A API OSHI deverá ser usada para captar os dados de hardware do device</t>
   </si>
   <si>
     <t>5.1</t>
   </si>
   <si>
-    <t>O software deverá ter níveis de acesso</t>
-  </si>
-  <si>
-    <t>6.1</t>
-  </si>
-  <si>
-    <t>O software deverá ter uma tela de login</t>
-  </si>
-  <si>
-    <t>6.2</t>
-  </si>
-  <si>
-    <t>O software deverá emitir um alerta visual, caso os dados de login sejam inválidos</t>
-  </si>
-  <si>
-    <t>4.3</t>
-  </si>
-  <si>
-    <t>O software deverá kickar do servidor users com softwares possivelmente maliosos instalados em seu device</t>
-  </si>
-  <si>
-    <t>O software deverá permitir a exibição de usuários</t>
-  </si>
-  <si>
-    <t>O software deverá permitir ao administrador a exclusão de um ou mais usuários</t>
-  </si>
-  <si>
-    <t>O software deverá permitir ao administrador a exibição de usuários em cada servidor</t>
-  </si>
-  <si>
-    <t>08/30/2019</t>
-  </si>
-  <si>
-    <t>O sofware deverá guardar o log</t>
-  </si>
-  <si>
-    <t>Essencial</t>
-  </si>
-  <si>
-    <t>Importante</t>
-  </si>
-  <si>
-    <t>Desejável</t>
-  </si>
-  <si>
-    <t>O software deverá bloquear no servidor a entrada de users que anteriormente tentaram acessá-lo com softwares possivelmente maliosos</t>
-  </si>
-  <si>
-    <t>O software deverá ter autenticação de usuários para a entrada no sistema</t>
-  </si>
-  <si>
-    <t>Não Funcional</t>
-  </si>
-  <si>
-    <t>Funcional</t>
-  </si>
-  <si>
-    <t>Gerson Santos</t>
-  </si>
-  <si>
-    <t>Proposto</t>
-  </si>
-  <si>
-    <t>Mínima</t>
-  </si>
-  <si>
-    <t>Alta</t>
-  </si>
-  <si>
-    <t>Baixa</t>
-  </si>
-  <si>
-    <t>Média</t>
-  </si>
-  <si>
-    <t>Máxima</t>
-  </si>
-  <si>
-    <t>O software deverá permitir ao administrador a alteração de um ou mais usuários</t>
-  </si>
-  <si>
-    <t>8.1</t>
+    <t>5.2</t>
+  </si>
+  <si>
+    <t>5.3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -498,6 +535,25 @@
       <b/>
       <sz val="10"/>
       <color indexed="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -661,10 +717,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -688,9 +745,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -738,6 +792,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -765,8 +823,24 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="30">
@@ -784,7 +858,6 @@
         <sz val="10"/>
         <color auto="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -815,7 +888,6 @@
         <sz val="10"/>
         <color auto="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -848,7 +920,6 @@
         <sz val="10"/>
         <color auto="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -881,7 +952,6 @@
         <sz val="10"/>
         <color auto="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -914,7 +984,6 @@
         <sz val="10"/>
         <color auto="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -947,7 +1016,6 @@
         <sz val="10"/>
         <color auto="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
@@ -981,7 +1049,6 @@
         <sz val="10"/>
         <color auto="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1014,7 +1081,6 @@
         <sz val="10"/>
         <color auto="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1047,7 +1113,6 @@
         <sz val="10"/>
         <color auto="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1080,7 +1145,6 @@
         <sz val="10"/>
         <color auto="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1113,7 +1177,6 @@
         <sz val="10"/>
         <color auto="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1146,7 +1209,6 @@
         <sz val="10"/>
         <color auto="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1179,7 +1241,6 @@
         <sz val="10"/>
         <color auto="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1213,7 +1274,6 @@
         <sz val="10"/>
         <color auto="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1246,7 +1306,6 @@
         <sz val="10"/>
         <color auto="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1279,7 +1338,6 @@
         <sz val="10"/>
         <color auto="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1312,7 +1370,6 @@
         <sz val="10"/>
         <color auto="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1345,7 +1402,6 @@
         <sz val="10"/>
         <color auto="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1383,7 +1439,6 @@
         <sz val="10"/>
         <color auto="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1409,7 +1464,6 @@
         <sz val="10"/>
         <color theme="0"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -1444,7 +1498,6 @@
         <sz val="10"/>
         <color auto="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
@@ -1464,7 +1517,6 @@
         <sz val="10"/>
         <color auto="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1483,7 +1535,6 @@
         <sz val="10"/>
         <color auto="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1502,7 +1553,6 @@
         <sz val="10"/>
         <color auto="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1528,7 +1578,6 @@
         <sz val="10"/>
         <color auto="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1554,7 +1603,6 @@
         <sz val="10"/>
         <color auto="1"/>
         <name val="Arial"/>
-        <family val="2"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -1655,13 +1703,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E1B1CD77-BAD2-4A02-9F6B-581F7C363EAE}" name="Tabela1" displayName="Tabela1" ref="B4:E32" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26">
-  <autoFilter ref="B4:E32" xr:uid="{5D10ECB7-FA14-4DC2-88A3-4C35A84FE31F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B4:E32" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26">
+  <autoFilter ref="B4:E32"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{3254B635-2323-4E75-BB71-FDB8433D84AA}" name="Versão" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{C2D5BAAF-DA6E-4E32-A4FB-784A019C5633}" name="Alteração efetuada" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{1592629F-8DF0-4B3E-A0F2-8634A8164A2A}" name="Responsável " dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{EEFC847D-DD1C-4AAA-9864-5127AFD71971}" name="Data " dataDxfId="22">
+    <tableColumn id="1" name="Versão" dataDxfId="25"/>
+    <tableColumn id="2" name="Alteração efetuada" dataDxfId="24"/>
+    <tableColumn id="3" name="Responsável " dataDxfId="23"/>
+    <tableColumn id="4" name="Data " dataDxfId="22">
       <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1670,27 +1718,27 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="requisitos" displayName="requisitos" ref="D4:U71" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18">
-  <autoFilter ref="D4:U71" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="requisitos" displayName="requisitos" ref="D4:U71" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18">
+  <autoFilter ref="D4:U71"/>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Descrição do Requisito" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Objetivo / Estratégia de Negócio" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Prioridade" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Versão do Requisito" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Tipo Requisito " dataDxfId="13"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Complexidade" dataDxfId="12"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Solicitante" dataDxfId="11"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Responsável" dataDxfId="10"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Validador" dataDxfId="9"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Critérios de Aceitação" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Dependência Internas entre Requisitos  (Rastreabilidade)" dataDxfId="7"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Dependências Externas entre Requisitos (Rastreabilidade)" dataDxfId="6"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Data da Criação" dataDxfId="5"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Data Última Alteração" dataDxfId="4"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Responsável pela última alteração" dataDxfId="3"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Motivo Última Alteração" dataDxfId="2"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Documentação de Apoio" dataDxfId="1"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Situação do Requisito" dataDxfId="0"/>
+    <tableColumn id="1" name="Descrição do Requisito" dataDxfId="17"/>
+    <tableColumn id="2" name="Objetivo / Estratégia de Negócio" dataDxfId="16"/>
+    <tableColumn id="3" name="Prioridade" dataDxfId="15"/>
+    <tableColumn id="4" name="Versão do Requisito" dataDxfId="14"/>
+    <tableColumn id="7" name="Tipo Requisito " dataDxfId="13"/>
+    <tableColumn id="8" name="Complexidade" dataDxfId="12"/>
+    <tableColumn id="9" name="Solicitante" dataDxfId="11"/>
+    <tableColumn id="10" name="Responsável" dataDxfId="10"/>
+    <tableColumn id="11" name="Validador" dataDxfId="9"/>
+    <tableColumn id="12" name="Critérios de Aceitação" dataDxfId="8"/>
+    <tableColumn id="13" name="Dependência Internas entre Requisitos  (Rastreabilidade)" dataDxfId="7"/>
+    <tableColumn id="14" name="Dependências Externas entre Requisitos (Rastreabilidade)" dataDxfId="6"/>
+    <tableColumn id="15" name="Data da Criação" dataDxfId="5"/>
+    <tableColumn id="16" name="Data Última Alteração" dataDxfId="4"/>
+    <tableColumn id="17" name="Responsável pela última alteração" dataDxfId="3"/>
+    <tableColumn id="18" name="Motivo Última Alteração" dataDxfId="2"/>
+    <tableColumn id="19" name="Documentação de Apoio" dataDxfId="1"/>
+    <tableColumn id="20" name="Situação do Requisito" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1772,23 +1820,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1824,23 +1855,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2016,7 +2030,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2037,25 +2051,25 @@
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2"/>
     <row r="4" spans="2:5" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="23" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2070,15 +2084,15 @@
         <v>7</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>83</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>7</v>
@@ -2089,10 +2103,10 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>7</v>
@@ -2103,10 +2117,10 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" s="7" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>7</v>
@@ -2117,10 +2131,10 @@
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B9" s="7" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>7</v>
@@ -2200,28 +2214,28 @@
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2"/>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B34" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
+      <c r="B34" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B35" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
+      <c r="B35" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
     </row>
     <row r="36" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
+      <c r="B36" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="26"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2"/>
     <row r="38" spans="2:5" hidden="1" x14ac:dyDescent="0.2"/>
@@ -2236,7 +2250,7 @@
     <mergeCell ref="B36:E36"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D32" xr:uid="{0B960ABE-A90C-4B02-B2D8-DC98F26688EB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D32">
       <formula1>"Fernando Abreu,João Vinícius,Kessi Santana,Thalita Igwe,Vitoria Ferreira"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2249,11 +2263,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V73"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
       <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
@@ -2265,170 +2279,174 @@
     <col min="2" max="2" width="3.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="49.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="21.28515625" style="1" customWidth="1"/>
     <col min="8" max="8" width="18.85546875" style="1" customWidth="1"/>
     <col min="9" max="9" width="16.7109375" style="7" customWidth="1"/>
     <col min="10" max="10" width="25.42578125" style="7" customWidth="1"/>
-    <col min="11" max="11" width="20.5703125" style="7" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="20.5703125" style="7" customWidth="1"/>
     <col min="12" max="12" width="16.28515625" style="7" customWidth="1"/>
-    <col min="13" max="13" width="26.140625" style="7" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="26.140625" style="7" customWidth="1"/>
     <col min="14" max="14" width="22.42578125" style="1" customWidth="1"/>
     <col min="15" max="15" width="30.5703125" style="7" customWidth="1"/>
     <col min="16" max="16" width="16" style="7" customWidth="1"/>
     <col min="17" max="17" width="14.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="17" style="1" customWidth="1"/>
-    <col min="20" max="20" width="16.140625" style="1" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="16.140625" style="1" customWidth="1"/>
     <col min="21" max="21" width="25.42578125" style="1" customWidth="1"/>
     <col min="22" max="22" width="3.7109375" style="1" customWidth="1"/>
     <col min="23" max="16384" width="9.140625" style="1" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" s="14" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="10"/>
-      <c r="U1" s="18"/>
-    </row>
-    <row r="2" spans="2:21" s="14" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E2" s="32"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="P2" s="30">
+    <row r="1" spans="2:21" s="13" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="9"/>
+      <c r="U1" s="17"/>
+    </row>
+    <row r="2" spans="2:21" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E2" s="33"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" s="31">
         <f ca="1">TODAY()</f>
-        <v>43716</v>
-      </c>
-      <c r="R2" s="19"/>
-      <c r="U2" s="18"/>
-    </row>
-    <row r="3" spans="2:21" s="14" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E3" s="33"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="31"/>
-      <c r="U3" s="20"/>
+        <v>43719</v>
+      </c>
+      <c r="R2" s="18"/>
+      <c r="U2" s="17"/>
+    </row>
+    <row r="3" spans="2:21" s="13" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="34"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="30"/>
+      <c r="P3" s="32"/>
+      <c r="U3" s="19"/>
     </row>
     <row r="4" spans="2:21" s="2" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="13" t="s">
-        <v>18</v>
+      <c r="B4" s="12" t="s">
+        <v>21</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="21">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="20">
         <v>1</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="11" t="s">
-        <v>38</v>
+      <c r="C5" s="20"/>
+      <c r="D5" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
-        <v>85</v>
+        <v>42</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>90</v>
+        <v>43</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>94</v>
+        <v>44</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="K5" s="4"/>
+        <v>45</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="L5" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="M5" s="4"/>
+        <v>45</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
       <c r="P5" s="5">
@@ -2446,36 +2464,38 @@
       </c>
       <c r="T5" s="4"/>
       <c r="U5" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="6" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="21"/>
-      <c r="C6" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>39</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="20"/>
+      <c r="C6" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>90</v>
+        <v>43</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>94</v>
+        <v>44</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="K6" s="4"/>
+        <v>45</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="L6" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
@@ -2495,36 +2515,34 @@
       </c>
       <c r="T6" s="4"/>
       <c r="U6" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="7" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="21"/>
-      <c r="C7" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>40</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="20"/>
+      <c r="C7" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>51</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4" t="s">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="4" t="s">
-        <v>90</v>
-      </c>
+      <c r="H7" s="4"/>
       <c r="I7" s="4" t="s">
-        <v>94</v>
+        <v>44</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
@@ -2544,36 +2562,38 @@
       </c>
       <c r="T7" s="4"/>
       <c r="U7" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="8" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="21"/>
-      <c r="C8" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>59</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="20"/>
+      <c r="C8" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4" t="s">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>90</v>
+        <v>53</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>94</v>
+        <v>44</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="K8" s="4"/>
+        <v>45</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="L8" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
@@ -2593,36 +2613,38 @@
       </c>
       <c r="T8" s="4"/>
       <c r="U8" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="9" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="21">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="20">
         <v>2</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="11" t="s">
-        <v>42</v>
+      <c r="C9" s="20"/>
+      <c r="D9" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4" t="s">
-        <v>85</v>
+        <v>42</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>90</v>
+        <v>53</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>95</v>
+        <v>55</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="K9" s="4"/>
+        <v>45</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="L9" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
@@ -2642,36 +2664,36 @@
       </c>
       <c r="T9" s="4"/>
       <c r="U9" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="10" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="21"/>
-      <c r="C10" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>44</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="20"/>
+      <c r="C10" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>56</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4" t="s">
-        <v>85</v>
+        <v>42</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>90</v>
+        <v>53</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>96</v>
+        <v>57</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="K10" s="4"/>
       <c r="L10" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
@@ -2691,36 +2713,36 @@
       </c>
       <c r="T10" s="4"/>
       <c r="U10" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="11" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="21"/>
-      <c r="C11" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>46</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="20"/>
+      <c r="C11" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>58</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4" t="s">
-        <v>85</v>
+        <v>42</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>90</v>
+        <v>53</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>96</v>
+        <v>57</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="K11" s="4"/>
       <c r="L11" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
@@ -2740,36 +2762,36 @@
       </c>
       <c r="T11" s="4"/>
       <c r="U11" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="12" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="21">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="20">
         <v>3</v>
       </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="11" t="s">
-        <v>58</v>
+      <c r="C12" s="20"/>
+      <c r="D12" s="10" t="s">
+        <v>59</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4" t="s">
-        <v>85</v>
+        <v>42</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>90</v>
+        <v>43</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="K12" s="4"/>
       <c r="L12" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
@@ -2789,85 +2811,85 @@
       </c>
       <c r="T12" s="4"/>
       <c r="U12" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="13" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="21"/>
-      <c r="C13" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="12" t="s">
-        <v>47</v>
+    </row>
+    <row r="13" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="20"/>
+      <c r="C13" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>61</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
-        <v>85</v>
+        <v>42</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>90</v>
+        <v>43</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>97</v>
+        <v>55</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="K13" s="4"/>
+        <v>45</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="L13" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
       <c r="P13" s="5">
-        <v>43711</v>
+        <v>43718</v>
       </c>
       <c r="Q13" s="5">
-        <v>43711</v>
+        <v>43718</v>
       </c>
       <c r="R13" s="4" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="S13" s="4" t="str">
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T13" s="4"/>
+      <c r="T13" s="24" t="s">
+        <v>85</v>
+      </c>
       <c r="U13" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="14" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="21"/>
-      <c r="C14" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>49</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="20"/>
+      <c r="C14" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>109</v>
       </c>
       <c r="E14" s="4"/>
-      <c r="F14" s="4" t="s">
-        <v>85</v>
-      </c>
+      <c r="F14" s="4"/>
       <c r="G14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H14" s="4" t="s">
-        <v>90</v>
-      </c>
+      <c r="H14" s="4"/>
       <c r="I14" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="K14" s="4"/>
       <c r="L14" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
@@ -2887,36 +2909,32 @@
       </c>
       <c r="T14" s="4"/>
       <c r="U14" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="15" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="21"/>
-      <c r="C15" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>51</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="20"/>
+      <c r="C15" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="E15" s="4"/>
-      <c r="F15" s="4" t="s">
-        <v>85</v>
-      </c>
+      <c r="F15" s="4"/>
       <c r="G15" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H15" s="4" t="s">
-        <v>90</v>
-      </c>
+      <c r="H15" s="4"/>
       <c r="I15" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="K15" s="4"/>
       <c r="L15" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
@@ -2936,36 +2954,32 @@
       </c>
       <c r="T15" s="4"/>
       <c r="U15" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="21"/>
-      <c r="C16" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>53</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="20"/>
+      <c r="C16" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="E16" s="4"/>
-      <c r="F16" s="4" t="s">
-        <v>85</v>
-      </c>
+      <c r="F16" s="4"/>
       <c r="G16" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H16" s="4" t="s">
-        <v>90</v>
-      </c>
+      <c r="H16" s="4"/>
       <c r="I16" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="K16" s="4"/>
       <c r="L16" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
@@ -2985,36 +2999,32 @@
       </c>
       <c r="T16" s="4"/>
       <c r="U16" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="17" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="21"/>
-      <c r="C17" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>60</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="20"/>
+      <c r="C17" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>64</v>
       </c>
       <c r="E17" s="4"/>
-      <c r="F17" s="4" t="s">
-        <v>86</v>
-      </c>
+      <c r="F17" s="4"/>
       <c r="G17" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H17" s="4" t="s">
-        <v>90</v>
-      </c>
+      <c r="H17" s="4"/>
       <c r="I17" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="K17" s="4"/>
       <c r="L17" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
@@ -3023,47 +3033,45 @@
         <v>43711</v>
       </c>
       <c r="Q17" s="5">
-        <v>43713</v>
+        <v>43711</v>
       </c>
       <c r="R17" s="4" t="s">
         <v>7</v>
       </c>
       <c r="S17" s="4" t="str">
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
-        <v>Adequação ao escopo do projeto</v>
+        <v>N/A</v>
       </c>
       <c r="T17" s="4"/>
       <c r="U17" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="18" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="21"/>
-      <c r="C18" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>56</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="20"/>
+      <c r="C18" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>65</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4" t="s">
-        <v>86</v>
+        <v>50</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H18" s="4" t="s">
-        <v>90</v>
-      </c>
+      <c r="H18" s="4"/>
       <c r="I18" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="K18" s="4"/>
       <c r="L18" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
@@ -3072,56 +3080,54 @@
         <v>43711</v>
       </c>
       <c r="Q18" s="5">
-        <v>43711</v>
+        <v>43713</v>
       </c>
       <c r="R18" s="4" t="s">
         <v>7</v>
       </c>
       <c r="S18" s="4" t="str">
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
-        <v>N/A</v>
+        <v>Adequação ao escopo do projeto</v>
       </c>
       <c r="T18" s="4"/>
       <c r="U18" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="19" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="21"/>
-      <c r="C19" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>61</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="20"/>
+      <c r="C19" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>66</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4" t="s">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H19" s="4" t="s">
-        <v>90</v>
-      </c>
+      <c r="H19" s="4"/>
       <c r="I19" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="K19" s="4"/>
       <c r="L19" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
       <c r="P19" s="5">
-        <v>43716</v>
+        <v>43711</v>
       </c>
       <c r="Q19" s="5">
-        <v>43716</v>
+        <v>43711</v>
       </c>
       <c r="R19" s="4" t="s">
         <v>7</v>
@@ -3132,45 +3138,43 @@
       </c>
       <c r="T19" s="4"/>
       <c r="U19" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="20" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="21"/>
-      <c r="C20" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>57</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="20"/>
+      <c r="C20" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>67</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4" t="s">
-        <v>86</v>
+        <v>42</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H20" s="4" t="s">
-        <v>91</v>
-      </c>
+      <c r="H20" s="4"/>
       <c r="I20" s="4" t="s">
-        <v>98</v>
+        <v>60</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="K20" s="4"/>
       <c r="L20" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
       <c r="P20" s="5">
-        <v>43711</v>
+        <v>43716</v>
       </c>
       <c r="Q20" s="5">
-        <v>43711</v>
+        <v>43716</v>
       </c>
       <c r="R20" s="4" t="s">
         <v>7</v>
@@ -3181,45 +3185,43 @@
       </c>
       <c r="T20" s="4"/>
       <c r="U20" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="21" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="21">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="20">
         <v>4</v>
       </c>
-      <c r="C21" s="21"/>
+      <c r="C21" s="20"/>
       <c r="D21" s="11" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4" t="s">
-        <v>87</v>
+        <v>50</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H21" s="4" t="s">
-        <v>90</v>
-      </c>
+      <c r="H21" s="4"/>
       <c r="I21" s="4" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="K21" s="4"/>
       <c r="L21" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
       <c r="P21" s="5">
-        <v>43716</v>
+        <v>43711</v>
       </c>
       <c r="Q21" s="5">
-        <v>43716</v>
+        <v>43711</v>
       </c>
       <c r="R21" s="4" t="s">
         <v>7</v>
@@ -3230,36 +3232,34 @@
       </c>
       <c r="T21" s="4"/>
       <c r="U21" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="22" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="21"/>
-      <c r="C22" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>69</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="20">
+        <v>5</v>
+      </c>
+      <c r="C22" s="20"/>
+      <c r="D22" s="10" t="s">
+        <v>70</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H22" s="4" t="s">
-        <v>90</v>
-      </c>
+      <c r="H22" s="4"/>
       <c r="I22" s="4" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="K22" s="4"/>
       <c r="L22" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
@@ -3279,36 +3279,32 @@
       </c>
       <c r="T22" s="4"/>
       <c r="U22" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="23" spans="2:21" s="22" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="21"/>
-      <c r="C23" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>79</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="2:21" s="21" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="20"/>
+      <c r="C23" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>71</v>
       </c>
       <c r="E23" s="4"/>
-      <c r="F23" s="4" t="s">
-        <v>87</v>
-      </c>
+      <c r="F23" s="4"/>
       <c r="G23" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H23" s="4" t="s">
-        <v>90</v>
-      </c>
+      <c r="H23" s="4"/>
       <c r="I23" s="4" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="K23" s="4"/>
       <c r="L23" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
@@ -3328,36 +3324,32 @@
       </c>
       <c r="T23" s="4"/>
       <c r="U23" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="24" spans="2:21" s="22" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="21"/>
-      <c r="C24" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>88</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="2:21" s="21" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="20"/>
+      <c r="C24" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>72</v>
       </c>
       <c r="E24" s="4"/>
-      <c r="F24" s="4" t="s">
-        <v>87</v>
-      </c>
+      <c r="F24" s="4"/>
       <c r="G24" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H24" s="4" t="s">
-        <v>90</v>
-      </c>
+      <c r="H24" s="4"/>
       <c r="I24" s="4" t="s">
-        <v>95</v>
+        <v>55</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="K24" s="4"/>
       <c r="L24" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
@@ -3377,36 +3369,32 @@
       </c>
       <c r="T24" s="4"/>
       <c r="U24" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="25" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="21">
-        <v>5</v>
-      </c>
-      <c r="C25" s="21"/>
-      <c r="D25" s="11" t="s">
-        <v>71</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="2:21" s="21" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="20"/>
+      <c r="C25" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>73</v>
       </c>
       <c r="E25" s="4"/>
-      <c r="F25" s="4" t="s">
-        <v>85</v>
-      </c>
+      <c r="F25" s="4"/>
       <c r="G25" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H25" s="4" t="s">
-        <v>91</v>
-      </c>
+      <c r="H25" s="4"/>
       <c r="I25" s="4" t="s">
-        <v>97</v>
+        <v>55</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="K25" s="4"/>
       <c r="L25" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
@@ -3426,85 +3414,75 @@
       </c>
       <c r="T25" s="4"/>
       <c r="U25" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="26" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="21"/>
-      <c r="C26" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="G26" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="2:21" s="39" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="35">
+        <v>6</v>
+      </c>
+      <c r="C26" s="35"/>
+      <c r="D26" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="H26" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="J26" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
-      <c r="P26" s="5">
+      <c r="H26" s="37"/>
+      <c r="I26" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="J26" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="K26" s="37"/>
+      <c r="L26" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="M26" s="37"/>
+      <c r="N26" s="37"/>
+      <c r="O26" s="37"/>
+      <c r="P26" s="38">
         <v>43716</v>
       </c>
-      <c r="Q26" s="5">
+      <c r="Q26" s="38">
         <v>43716</v>
       </c>
-      <c r="R26" s="4" t="s">
+      <c r="R26" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="S26" s="4" t="str">
+      <c r="S26" s="37" t="str">
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T26" s="4"/>
-      <c r="U26" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="27" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="21">
-        <v>6</v>
-      </c>
-      <c r="C27" s="21"/>
-      <c r="D27" s="22" t="s">
-        <v>89</v>
+      <c r="T26" s="37"/>
+      <c r="U26" s="37" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="10" t="s">
+        <v>75</v>
       </c>
       <c r="E27" s="4"/>
-      <c r="F27" s="4" t="s">
-        <v>85</v>
-      </c>
+      <c r="F27" s="4"/>
       <c r="G27" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H27" s="4" t="s">
-        <v>91</v>
-      </c>
+      <c r="H27" s="4"/>
       <c r="I27" s="4" t="s">
-        <v>97</v>
+        <v>55</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="K27" s="4"/>
       <c r="L27" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
@@ -3524,36 +3502,30 @@
       </c>
       <c r="T27" s="4"/>
       <c r="U27" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="28" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="21"/>
-      <c r="C28" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="D28" s="22" t="s">
-        <v>75</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="21" t="s">
+        <v>76</v>
       </c>
       <c r="E28" s="4"/>
-      <c r="F28" s="4" t="s">
-        <v>85</v>
-      </c>
+      <c r="F28" s="4"/>
       <c r="G28" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H28" s="4" t="s">
-        <v>91</v>
-      </c>
+      <c r="H28" s="4"/>
       <c r="I28" s="4" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="K28" s="4"/>
       <c r="L28" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
@@ -3573,36 +3545,30 @@
       </c>
       <c r="T28" s="4"/>
       <c r="U28" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="29" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="21"/>
-      <c r="C29" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="D29" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="21" t="s">
         <v>77</v>
       </c>
       <c r="E29" s="4"/>
-      <c r="F29" s="4" t="s">
-        <v>85</v>
-      </c>
+      <c r="F29" s="4"/>
       <c r="G29" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H29" s="4" t="s">
-        <v>90</v>
-      </c>
+      <c r="H29" s="4"/>
       <c r="I29" s="4" t="s">
-        <v>96</v>
+        <v>57</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="K29" s="4"/>
       <c r="L29" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
@@ -3622,36 +3588,30 @@
       </c>
       <c r="T29" s="4"/>
       <c r="U29" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="30" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="21">
-        <v>7</v>
-      </c>
-      <c r="C30" s="21"/>
-      <c r="D30" s="11" t="s">
-        <v>65</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="10" t="s">
+        <v>78</v>
       </c>
       <c r="E30" s="4"/>
-      <c r="F30" s="4" t="s">
-        <v>87</v>
-      </c>
+      <c r="F30" s="4"/>
       <c r="G30" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H30" s="4" t="s">
-        <v>90</v>
-      </c>
+      <c r="H30" s="4"/>
       <c r="I30" s="4" t="s">
-        <v>95</v>
+        <v>57</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="K30" s="4"/>
       <c r="L30" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
@@ -3671,36 +3631,32 @@
       </c>
       <c r="T30" s="4"/>
       <c r="U30" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="31" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="21">
-        <v>8</v>
-      </c>
-      <c r="C31" s="21"/>
-      <c r="D31" s="11" t="s">
-        <v>80</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="10" t="s">
+        <v>79</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4" t="s">
-        <v>85</v>
+        <v>108</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H31" s="4" t="s">
-        <v>91</v>
-      </c>
+      <c r="H31" s="4"/>
       <c r="I31" s="4" t="s">
-        <v>97</v>
+        <v>55</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="K31" s="4"/>
       <c r="L31" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="M31" s="4"/>
       <c r="N31" s="4"/>
@@ -3720,36 +3676,30 @@
       </c>
       <c r="T31" s="4"/>
       <c r="U31" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="32" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="21"/>
-      <c r="C32" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>82</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="10" t="s">
+        <v>80</v>
       </c>
       <c r="E32" s="4"/>
-      <c r="F32" s="4" t="s">
-        <v>85</v>
-      </c>
+      <c r="F32" s="4"/>
       <c r="G32" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H32" s="4" t="s">
-        <v>91</v>
-      </c>
+      <c r="H32" s="4"/>
       <c r="I32" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="K32" s="4"/>
       <c r="L32" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
@@ -3769,36 +3719,30 @@
       </c>
       <c r="T32" s="4"/>
       <c r="U32" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="33" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="21">
-        <v>9</v>
-      </c>
-      <c r="C33" s="21"/>
-      <c r="D33" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="10" t="s">
         <v>81</v>
       </c>
       <c r="E33" s="4"/>
-      <c r="F33" s="4" t="s">
-        <v>86</v>
-      </c>
+      <c r="F33" s="4"/>
       <c r="G33" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H33" s="4" t="s">
-        <v>91</v>
-      </c>
+      <c r="H33" s="4"/>
       <c r="I33" s="4" t="s">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="K33" s="4"/>
       <c r="L33" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
@@ -3818,36 +3762,30 @@
       </c>
       <c r="T33" s="4"/>
       <c r="U33" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="34" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="21">
-        <v>10</v>
-      </c>
-      <c r="C34" s="21"/>
-      <c r="D34" s="11" t="s">
-        <v>99</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="10" t="s">
+        <v>82</v>
       </c>
       <c r="E34" s="4"/>
-      <c r="F34" s="4" t="s">
-        <v>86</v>
-      </c>
+      <c r="F34" s="4"/>
       <c r="G34" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H34" s="4" t="s">
-        <v>91</v>
-      </c>
+      <c r="H34" s="4"/>
       <c r="I34" s="4" t="s">
-        <v>95</v>
+        <v>55</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="K34" s="4"/>
       <c r="L34" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
@@ -3867,42 +3805,36 @@
       </c>
       <c r="T34" s="4"/>
       <c r="U34" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="35" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="21">
-        <v>11</v>
-      </c>
-      <c r="C35" s="21"/>
-      <c r="D35" s="22" t="s">
-        <v>84</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="20"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="10" t="s">
+        <v>83</v>
       </c>
       <c r="E35" s="4"/>
-      <c r="F35" s="4" t="s">
-        <v>85</v>
-      </c>
+      <c r="F35" s="4"/>
       <c r="G35" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H35" s="4" t="s">
-        <v>90</v>
-      </c>
+      <c r="H35" s="4"/>
       <c r="I35" s="4" t="s">
-        <v>97</v>
+        <v>55</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="K35" s="4"/>
       <c r="L35" s="4" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="M35" s="4"/>
       <c r="N35" s="4"/>
       <c r="O35" s="4"/>
       <c r="P35" s="5">
-        <v>43714</v>
+        <v>43716</v>
       </c>
       <c r="Q35" s="5">
         <v>43716</v>
@@ -3912,39 +3844,60 @@
       </c>
       <c r="S35" s="4" t="str">
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
-        <v>Adequação ao escopo do projeto</v>
+        <v>N/A</v>
       </c>
       <c r="T35" s="4"/>
       <c r="U35" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="36" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="21"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="11"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="20"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="21" t="s">
+        <v>84</v>
+      </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
+      <c r="G36" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
+      <c r="I36" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
+      <c r="L36" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="M36" s="4"/>
       <c r="N36" s="4"/>
       <c r="O36" s="4"/>
-      <c r="P36" s="5"/>
-      <c r="Q36" s="4"/>
-      <c r="R36" s="4"/>
-      <c r="S36" s="4"/>
+      <c r="P36" s="5">
+        <v>43714</v>
+      </c>
+      <c r="Q36" s="5">
+        <v>43716</v>
+      </c>
+      <c r="R36" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="S36" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>Adequação ao escopo do projeto</v>
+      </c>
       <c r="T36" s="4"/>
-      <c r="U36" s="4"/>
-    </row>
-    <row r="37" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="11"/>
+      <c r="U36" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="20"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="10"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
@@ -3957,258 +3910,465 @@
       <c r="N37" s="4"/>
       <c r="O37" s="4"/>
       <c r="P37" s="5"/>
-      <c r="Q37" s="4"/>
+      <c r="Q37" s="5"/>
       <c r="R37" s="4"/>
       <c r="S37" s="4"/>
-      <c r="T37" s="4"/>
+      <c r="T37" s="24"/>
       <c r="U37" s="4"/>
     </row>
-    <row r="38" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="21"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="11"/>
+    <row r="38" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="20"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="10" t="s">
+        <v>87</v>
+      </c>
       <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
-      <c r="L38" s="4"/>
+      <c r="F38" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="K38" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L38" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="M38" s="4"/>
       <c r="N38" s="4"/>
       <c r="O38" s="4"/>
-      <c r="P38" s="5"/>
-      <c r="Q38" s="4"/>
-      <c r="R38" s="4"/>
-      <c r="S38" s="4"/>
-      <c r="T38" s="4"/>
-      <c r="U38" s="4"/>
-    </row>
-    <row r="39" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="21"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="11"/>
+      <c r="P38" s="5">
+        <v>43718</v>
+      </c>
+      <c r="Q38" s="5">
+        <v>43718</v>
+      </c>
+      <c r="R38" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="S38" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
+      <c r="T38" s="24"/>
+      <c r="U38" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="20"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="10" t="s">
+        <v>88</v>
+      </c>
       <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
-      <c r="L39" s="4"/>
+      <c r="F39" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="K39" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L39" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="M39" s="4"/>
       <c r="N39" s="4"/>
       <c r="O39" s="4"/>
-      <c r="P39" s="5"/>
-      <c r="Q39" s="4"/>
-      <c r="R39" s="4"/>
-      <c r="S39" s="4"/>
-      <c r="T39" s="4"/>
-      <c r="U39" s="4"/>
-    </row>
-    <row r="40" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="21"/>
-      <c r="C40" s="21"/>
-      <c r="D40" s="11"/>
+      <c r="P39" s="5">
+        <v>43718</v>
+      </c>
+      <c r="Q39" s="5">
+        <v>43718</v>
+      </c>
+      <c r="R39" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="S39" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
+      <c r="T39" s="24"/>
+      <c r="U39" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="20"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="10" t="s">
+        <v>89</v>
+      </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
+      <c r="G40" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
-      <c r="J40" s="4"/>
+      <c r="J40" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="K40" s="4"/>
-      <c r="L40" s="4"/>
+      <c r="L40" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="M40" s="4"/>
       <c r="N40" s="4"/>
       <c r="O40" s="4"/>
-      <c r="P40" s="5"/>
-      <c r="Q40" s="4"/>
+      <c r="P40" s="5">
+        <v>43718</v>
+      </c>
+      <c r="Q40" s="5">
+        <v>43718</v>
+      </c>
       <c r="R40" s="4"/>
-      <c r="S40" s="4"/>
+      <c r="S40" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
       <c r="T40" s="4"/>
-      <c r="U40" s="4"/>
-    </row>
-    <row r="41" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="21"/>
-      <c r="C41" s="21"/>
-      <c r="D41" s="11"/>
+      <c r="U40" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="10" t="s">
+        <v>90</v>
+      </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
+      <c r="G41" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
-      <c r="J41" s="4"/>
+      <c r="J41" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="K41" s="4"/>
-      <c r="L41" s="4"/>
+      <c r="L41" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="M41" s="4"/>
       <c r="N41" s="4"/>
       <c r="O41" s="4"/>
-      <c r="P41" s="5"/>
-      <c r="Q41" s="4"/>
+      <c r="P41" s="5">
+        <v>43718</v>
+      </c>
+      <c r="Q41" s="5">
+        <v>43718</v>
+      </c>
       <c r="R41" s="4"/>
-      <c r="S41" s="4"/>
+      <c r="S41" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
       <c r="T41" s="4"/>
-      <c r="U41" s="4"/>
-    </row>
-    <row r="42" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="21"/>
-      <c r="C42" s="21"/>
-      <c r="D42" s="11"/>
+      <c r="U41" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="42" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="20"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
+      <c r="G42" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
-      <c r="J42" s="4"/>
+      <c r="J42" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="K42" s="4"/>
-      <c r="L42" s="4"/>
+      <c r="L42" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="M42" s="4"/>
       <c r="N42" s="4"/>
       <c r="O42" s="4"/>
-      <c r="P42" s="5"/>
-      <c r="Q42" s="4"/>
+      <c r="P42" s="5">
+        <v>43718</v>
+      </c>
+      <c r="Q42" s="5">
+        <v>43718</v>
+      </c>
       <c r="R42" s="4"/>
-      <c r="S42" s="4"/>
+      <c r="S42" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
       <c r="T42" s="4"/>
-      <c r="U42" s="4"/>
-    </row>
-    <row r="43" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="21"/>
-      <c r="C43" s="21"/>
-      <c r="D43" s="11"/>
+      <c r="U42" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="2:21" s="21" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="20"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="10" t="s">
+        <v>92</v>
+      </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
+      <c r="G43" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
+      <c r="J43" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="K43" s="4"/>
-      <c r="L43" s="4"/>
+      <c r="L43" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="M43" s="4"/>
       <c r="N43" s="4"/>
       <c r="O43" s="4"/>
-      <c r="P43" s="5"/>
-      <c r="Q43" s="4"/>
+      <c r="P43" s="5">
+        <v>43718</v>
+      </c>
+      <c r="Q43" s="5">
+        <v>43718</v>
+      </c>
       <c r="R43" s="4"/>
-      <c r="S43" s="4"/>
+      <c r="S43" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
       <c r="T43" s="4"/>
-      <c r="U43" s="4"/>
-    </row>
-    <row r="44" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="21"/>
-      <c r="C44" s="21"/>
-      <c r="D44" s="11"/>
+      <c r="U43" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="10" t="s">
+        <v>93</v>
+      </c>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
+      <c r="G44" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
-      <c r="J44" s="4"/>
+      <c r="J44" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="K44" s="4"/>
-      <c r="L44" s="4"/>
+      <c r="L44" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="M44" s="4"/>
       <c r="N44" s="4"/>
       <c r="O44" s="4"/>
-      <c r="P44" s="5"/>
-      <c r="Q44" s="4"/>
+      <c r="P44" s="5">
+        <v>43718</v>
+      </c>
+      <c r="Q44" s="5">
+        <v>43718</v>
+      </c>
       <c r="R44" s="4"/>
-      <c r="S44" s="4"/>
+      <c r="S44" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
       <c r="T44" s="4"/>
-      <c r="U44" s="4"/>
-    </row>
-    <row r="45" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="21"/>
-      <c r="C45" s="21"/>
-      <c r="D45" s="11"/>
+      <c r="U44" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="20"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="10" t="s">
+        <v>94</v>
+      </c>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
+      <c r="G45" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
-      <c r="J45" s="4"/>
+      <c r="J45" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="K45" s="4"/>
-      <c r="L45" s="4"/>
+      <c r="L45" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="M45" s="4"/>
       <c r="N45" s="4"/>
       <c r="O45" s="4"/>
-      <c r="P45" s="5"/>
-      <c r="Q45" s="4"/>
+      <c r="P45" s="5">
+        <v>43718</v>
+      </c>
+      <c r="Q45" s="5">
+        <v>43718</v>
+      </c>
       <c r="R45" s="4"/>
-      <c r="S45" s="4"/>
+      <c r="S45" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
       <c r="T45" s="4"/>
-      <c r="U45" s="4"/>
-    </row>
-    <row r="46" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="11"/>
+      <c r="U45" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="20"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="10" t="s">
+        <v>95</v>
+      </c>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
+      <c r="G46" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
-      <c r="J46" s="4"/>
+      <c r="J46" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="K46" s="4"/>
-      <c r="L46" s="4"/>
+      <c r="L46" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="M46" s="4"/>
       <c r="N46" s="4"/>
       <c r="O46" s="4"/>
-      <c r="P46" s="5"/>
-      <c r="Q46" s="4"/>
+      <c r="P46" s="5">
+        <v>43718</v>
+      </c>
+      <c r="Q46" s="5">
+        <v>43718</v>
+      </c>
       <c r="R46" s="4"/>
-      <c r="S46" s="4"/>
+      <c r="S46" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
       <c r="T46" s="4"/>
-      <c r="U46" s="4"/>
-    </row>
-    <row r="47" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="21"/>
-      <c r="C47" s="21"/>
-      <c r="D47" s="11"/>
+      <c r="U46" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="20"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="10" t="s">
+        <v>96</v>
+      </c>
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
+      <c r="G47" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
-      <c r="J47" s="4"/>
+      <c r="J47" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="K47" s="4"/>
-      <c r="L47" s="4"/>
+      <c r="L47" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="M47" s="4"/>
       <c r="N47" s="4"/>
       <c r="O47" s="4"/>
-      <c r="P47" s="5"/>
-      <c r="Q47" s="4"/>
+      <c r="P47" s="5">
+        <v>43718</v>
+      </c>
+      <c r="Q47" s="5">
+        <v>43718</v>
+      </c>
       <c r="R47" s="4"/>
-      <c r="S47" s="4"/>
+      <c r="S47" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
       <c r="T47" s="4"/>
-      <c r="U47" s="4"/>
-    </row>
-    <row r="48" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="21"/>
-      <c r="C48" s="21"/>
-      <c r="D48" s="11"/>
+      <c r="U47" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="20"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="10" t="s">
+        <v>97</v>
+      </c>
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
+      <c r="G48" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
-      <c r="J48" s="4"/>
+      <c r="J48" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="K48" s="4"/>
-      <c r="L48" s="4"/>
+      <c r="L48" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="M48" s="4"/>
       <c r="N48" s="4"/>
       <c r="O48" s="4"/>
-      <c r="P48" s="5"/>
-      <c r="Q48" s="4"/>
+      <c r="P48" s="5">
+        <v>43718</v>
+      </c>
+      <c r="Q48" s="5">
+        <v>43718</v>
+      </c>
       <c r="R48" s="4"/>
-      <c r="S48" s="4"/>
+      <c r="S48" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
       <c r="T48" s="4"/>
-      <c r="U48" s="4"/>
-    </row>
-    <row r="49" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="21"/>
-      <c r="C49" s="21"/>
-      <c r="D49" s="11"/>
+      <c r="U48" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="20"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="10"/>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
@@ -4227,10 +4387,10 @@
       <c r="T49" s="4"/>
       <c r="U49" s="4"/>
     </row>
-    <row r="50" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="21"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="11"/>
+    <row r="50" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="20"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="10"/>
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
       <c r="G50" s="4"/>
@@ -4249,10 +4409,10 @@
       <c r="T50" s="4"/>
       <c r="U50" s="4"/>
     </row>
-    <row r="51" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="21"/>
-      <c r="C51" s="21"/>
-      <c r="D51" s="11"/>
+    <row r="51" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="20"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="10"/>
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
       <c r="G51" s="4"/>
@@ -4271,10 +4431,10 @@
       <c r="T51" s="4"/>
       <c r="U51" s="4"/>
     </row>
-    <row r="52" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="21"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="11"/>
+    <row r="52" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="20"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="10"/>
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
@@ -4293,10 +4453,10 @@
       <c r="T52" s="4"/>
       <c r="U52" s="4"/>
     </row>
-    <row r="53" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="21"/>
-      <c r="C53" s="21"/>
-      <c r="D53" s="11"/>
+    <row r="53" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="20"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="10"/>
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
       <c r="G53" s="4"/>
@@ -4315,10 +4475,10 @@
       <c r="T53" s="4"/>
       <c r="U53" s="4"/>
     </row>
-    <row r="54" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="21"/>
-      <c r="C54" s="21"/>
-      <c r="D54" s="11"/>
+    <row r="54" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="20"/>
+      <c r="C54" s="20"/>
+      <c r="D54" s="10"/>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
@@ -4337,10 +4497,10 @@
       <c r="T54" s="4"/>
       <c r="U54" s="4"/>
     </row>
-    <row r="55" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="21"/>
-      <c r="C55" s="21"/>
-      <c r="D55" s="11"/>
+    <row r="55" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="20"/>
+      <c r="C55" s="20"/>
+      <c r="D55" s="10"/>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
@@ -4359,10 +4519,10 @@
       <c r="T55" s="4"/>
       <c r="U55" s="4"/>
     </row>
-    <row r="56" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="21"/>
-      <c r="C56" s="21"/>
-      <c r="D56" s="11"/>
+    <row r="56" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="20"/>
+      <c r="C56" s="20"/>
+      <c r="D56" s="10"/>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
       <c r="G56" s="4"/>
@@ -4381,10 +4541,10 @@
       <c r="T56" s="4"/>
       <c r="U56" s="4"/>
     </row>
-    <row r="57" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="21"/>
-      <c r="C57" s="21"/>
-      <c r="D57" s="11"/>
+    <row r="57" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="20"/>
+      <c r="C57" s="20"/>
+      <c r="D57" s="10"/>
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
       <c r="G57" s="4"/>
@@ -4403,10 +4563,10 @@
       <c r="T57" s="4"/>
       <c r="U57" s="4"/>
     </row>
-    <row r="58" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="21"/>
-      <c r="C58" s="21"/>
-      <c r="D58" s="11"/>
+    <row r="58" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="20"/>
+      <c r="C58" s="20"/>
+      <c r="D58" s="10"/>
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
       <c r="G58" s="4"/>
@@ -4425,10 +4585,10 @@
       <c r="T58" s="4"/>
       <c r="U58" s="4"/>
     </row>
-    <row r="59" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="21"/>
-      <c r="C59" s="21"/>
-      <c r="D59" s="11"/>
+    <row r="59" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="20"/>
+      <c r="C59" s="20"/>
+      <c r="D59" s="10"/>
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
       <c r="G59" s="4"/>
@@ -4447,10 +4607,10 @@
       <c r="T59" s="4"/>
       <c r="U59" s="4"/>
     </row>
-    <row r="60" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="21"/>
-      <c r="C60" s="21"/>
-      <c r="D60" s="11"/>
+    <row r="60" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="20"/>
+      <c r="C60" s="20"/>
+      <c r="D60" s="10"/>
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
       <c r="G60" s="4"/>
@@ -4469,10 +4629,10 @@
       <c r="T60" s="4"/>
       <c r="U60" s="4"/>
     </row>
-    <row r="61" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="21"/>
-      <c r="C61" s="21"/>
-      <c r="D61" s="11"/>
+    <row r="61" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="20"/>
+      <c r="C61" s="20"/>
+      <c r="D61" s="10"/>
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
       <c r="G61" s="4"/>
@@ -4491,10 +4651,10 @@
       <c r="T61" s="4"/>
       <c r="U61" s="4"/>
     </row>
-    <row r="62" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="21"/>
-      <c r="C62" s="21"/>
-      <c r="D62" s="11"/>
+    <row r="62" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="20"/>
+      <c r="C62" s="20"/>
+      <c r="D62" s="10"/>
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
       <c r="G62" s="4"/>
@@ -4513,10 +4673,10 @@
       <c r="T62" s="4"/>
       <c r="U62" s="4"/>
     </row>
-    <row r="63" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="21"/>
-      <c r="C63" s="21"/>
-      <c r="D63" s="11"/>
+    <row r="63" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="20"/>
+      <c r="C63" s="20"/>
+      <c r="D63" s="10"/>
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
       <c r="G63" s="4"/>
@@ -4535,10 +4695,10 @@
       <c r="T63" s="4"/>
       <c r="U63" s="4"/>
     </row>
-    <row r="64" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="21"/>
-      <c r="C64" s="21"/>
-      <c r="D64" s="11"/>
+    <row r="64" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="20"/>
+      <c r="C64" s="20"/>
+      <c r="D64" s="10"/>
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
@@ -4557,10 +4717,10 @@
       <c r="T64" s="4"/>
       <c r="U64" s="4"/>
     </row>
-    <row r="65" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="21"/>
-      <c r="C65" s="21"/>
-      <c r="D65" s="11"/>
+    <row r="65" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="20"/>
+      <c r="C65" s="20"/>
+      <c r="D65" s="10"/>
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
@@ -4579,10 +4739,10 @@
       <c r="T65" s="4"/>
       <c r="U65" s="4"/>
     </row>
-    <row r="66" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="21"/>
-      <c r="C66" s="21"/>
-      <c r="D66" s="11"/>
+    <row r="66" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="20"/>
+      <c r="C66" s="20"/>
+      <c r="D66" s="10"/>
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
       <c r="G66" s="4"/>
@@ -4601,10 +4761,10 @@
       <c r="T66" s="4"/>
       <c r="U66" s="4"/>
     </row>
-    <row r="67" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="21"/>
-      <c r="C67" s="21"/>
-      <c r="D67" s="11"/>
+    <row r="67" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="20"/>
+      <c r="C67" s="20"/>
+      <c r="D67" s="10"/>
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
       <c r="G67" s="4"/>
@@ -4623,10 +4783,10 @@
       <c r="T67" s="4"/>
       <c r="U67" s="4"/>
     </row>
-    <row r="68" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="21"/>
-      <c r="C68" s="21"/>
-      <c r="D68" s="11"/>
+    <row r="68" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="20"/>
+      <c r="C68" s="20"/>
+      <c r="D68" s="10"/>
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
       <c r="G68" s="4"/>
@@ -4645,10 +4805,10 @@
       <c r="T68" s="4"/>
       <c r="U68" s="4"/>
     </row>
-    <row r="69" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="21"/>
-      <c r="C69" s="21"/>
-      <c r="D69" s="11"/>
+    <row r="69" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="20"/>
+      <c r="C69" s="20"/>
+      <c r="D69" s="10"/>
       <c r="E69" s="4"/>
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>
@@ -4667,10 +4827,10 @@
       <c r="T69" s="4"/>
       <c r="U69" s="4"/>
     </row>
-    <row r="70" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="21"/>
-      <c r="C70" s="21"/>
-      <c r="D70" s="11"/>
+    <row r="70" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="20"/>
+      <c r="C70" s="20"/>
+      <c r="D70" s="10"/>
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
       <c r="G70" s="4"/>
@@ -4689,10 +4849,10 @@
       <c r="T70" s="4"/>
       <c r="U70" s="4"/>
     </row>
-    <row r="71" spans="2:21" s="22" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="21"/>
-      <c r="C71" s="21"/>
-      <c r="D71" s="11"/>
+    <row r="71" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="20"/>
+      <c r="C71" s="20"/>
+      <c r="D71" s="10"/>
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
       <c r="G71" s="4"/>
@@ -4712,7 +4872,7 @@
       <c r="U71" s="4"/>
     </row>
     <row r="72" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="N72" s="23"/>
+      <c r="N72" s="22"/>
     </row>
     <row r="73" spans="2:21" hidden="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -4730,25 +4890,25 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U5:U71" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U5:U71">
       <formula1>"Proposto,Aprovado,Projetado,Implementado,Verificado, Entregue, Eliminado, Rejeitado"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I71" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I71">
       <formula1>"Máxima,Alta,Média,Baixa,Mínima"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H71" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H71">
       <formula1>"Funcional,Não Funcional"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J71" xr:uid="{27F19A6C-524E-45E8-ABAC-AFD7E242F75B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L40:L48 J5:J71">
       <formula1>"Gerson Santos,Célia Taniwaki,José Yoshihiro,Alex Barreira"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R5:R71 K5:K71" xr:uid="{08414707-FD34-4214-AC27-E0609CF58BB6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R5:R71 K5:K71">
       <formula1>"Fernando Abreu,João Vinícius,Kessi Santana,Thalita Igwe,Vitoria Ferreira"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5:L71" xr:uid="{7BE54147-1A46-412A-BF1D-8B94526A2CB5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L49:L71 L5:L39">
       <formula1>"Gerson Santos,Fernando Abreu,João Vinícius,Kessi Santana,Thalita Igwe,Vitoria Ferreira,Célia Taniwaki,Alex Barreira,José Yoshihiro"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F71" xr:uid="{968C2421-7B57-4F57-8B60-603E777E75CC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F71">
       <formula1>"Essencial,Importante,Desejável"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4760,4 +4920,16 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Alteração requisitos, user stories e projeto do Yoshi.
</commit_message>
<xml_diff>
--- a/documentacao/requisitos.xlsx
+++ b/documentacao/requisitos.xlsx
@@ -9,12 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Histórico de Alterações" sheetId="4" r:id="rId1"/>
     <sheet name="Documentação e Matriz" sheetId="1" r:id="rId2"/>
-    <sheet name="Product Backlog" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="127">
   <si>
     <t>Histórico de alterações do documento</t>
   </si>
@@ -262,9 +261,6 @@
     <t>Funcional</t>
   </si>
   <si>
-    <t>Mínima</t>
-  </si>
-  <si>
     <t>Gerson Santos</t>
   </si>
   <si>
@@ -295,24 +291,15 @@
     <t>O sotware deverá ser desenvolvido na linguagem de programação Java</t>
   </si>
   <si>
-    <t>Alta</t>
-  </si>
-  <si>
     <t>O cliente deverá ter a JVM instalada em seu computador</t>
   </si>
   <si>
-    <t>Baixa</t>
-  </si>
-  <si>
     <t>O cliente deverá ter o JRE instalado em seu computador</t>
   </si>
   <si>
     <t>O sofware deverá ter um dashboard com as informações do hardware do device</t>
   </si>
   <si>
-    <t>Média</t>
-  </si>
-  <si>
     <t>O software deverá coletar as informações de hardware do device</t>
   </si>
   <si>
@@ -337,9 +324,6 @@
     <t>O software deverá encerrar processos "desnecessários" do sistema operacional</t>
   </si>
   <si>
-    <t>Máxima</t>
-  </si>
-  <si>
     <t>O software deverá agir na proteção do servidor</t>
   </si>
   <si>
@@ -352,9 +336,6 @@
     <t>O software deverá bloquear no servidor a entrada de users que anteriormente tentaram acessá-lo com softwares possivelmente maliosos</t>
   </si>
   <si>
-    <t>O software deverá ter uma tela de cadastro em que os próprios usuários se cadastram</t>
-  </si>
-  <si>
     <t>O software deverá ter níveis de acesso</t>
   </si>
   <si>
@@ -370,9 +351,6 @@
     <t>O software deverá fazer integração com o PowerBI</t>
   </si>
   <si>
-    <t>O software deverá permitir a exibição de usuários</t>
-  </si>
-  <si>
     <t>O software deverá permitir ao administrador a exibição de usuários em cada servidor</t>
   </si>
   <si>
@@ -391,9 +369,6 @@
     <t>Projetado</t>
   </si>
   <si>
-    <t>O software deverá ter uma API que capta as informações do usuário</t>
-  </si>
-  <si>
     <t>O software deverá uma tela com os dados do usuário e do seu device</t>
   </si>
   <si>
@@ -403,9 +378,6 @@
     <t>O software deverá permitir ao administrador o bloqueio de usuários aos servidores de jogos</t>
   </si>
   <si>
-    <t>O software deverá ter uma tela de cadastro em que o administrador possa cadastrar outros usuários (NOC)</t>
-  </si>
-  <si>
     <t>O software deverá permitir aos usuários (jogadores) o reset de senha</t>
   </si>
   <si>
@@ -467,13 +439,82 @@
   </si>
   <si>
     <t>5.3</t>
+  </si>
+  <si>
+    <t>O software deverá ter uma tela de cadastro em que os próprios usuários (jogadores) se cadastram</t>
+  </si>
+  <si>
+    <t>8.1</t>
+  </si>
+  <si>
+    <t>8.2</t>
+  </si>
+  <si>
+    <t>10.1</t>
+  </si>
+  <si>
+    <t>10.2</t>
+  </si>
+  <si>
+    <t>10.3</t>
+  </si>
+  <si>
+    <t>10.4</t>
+  </si>
+  <si>
+    <t>O software deverá permitir ao administrador a inclusão de um ou mais usuários</t>
+  </si>
+  <si>
+    <t>O software deverá ter uma API que capta as informações do device do usuário</t>
+  </si>
+  <si>
+    <t>12.1</t>
+  </si>
+  <si>
+    <t>8.3</t>
+  </si>
+  <si>
+    <t>10.5</t>
+  </si>
+  <si>
+    <t>10.6</t>
+  </si>
+  <si>
+    <t>10.7</t>
+  </si>
+  <si>
+    <t>10.8</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>https://docs.microsoft.com/pt-br/azure/sql-database/sql-database-connect-query-java</t>
+  </si>
+  <si>
+    <t>O software deverá permitir ao administrador a gestão de usuários (NOC)</t>
+  </si>
+  <si>
+    <t>https://www.java.com/pt_BR/download/</t>
+  </si>
+  <si>
+    <t>https://www.oracle.com/technetwork/pt/java/javase/downloads/jre8-downloads-2133155.html</t>
+  </si>
+  <si>
+    <t>https://docs.microsoft.com/pt-br/power-bi/developer/overview-of-power-bi-rest-api</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>USER PREMIUN E FREE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -532,27 +573,19 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color indexed="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u/>
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
       <sz val="10"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -578,7 +611,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -716,12 +749,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -780,9 +826,6 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -792,7 +835,33 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -823,20 +892,17 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -860,12 +926,14 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
           <color theme="0"/>
         </left>
-        <right/>
+        <right style="medium">
+          <color theme="0"/>
+        </right>
         <top style="medium">
           <color theme="0"/>
         </top>
@@ -895,9 +963,7 @@
         <left style="medium">
           <color theme="0"/>
         </left>
-        <right style="medium">
-          <color theme="0"/>
-        </right>
+        <right/>
         <top style="medium">
           <color theme="0"/>
         </top>
@@ -1737,8 +1803,8 @@
     <tableColumn id="16" name="Data Última Alteração" dataDxfId="4"/>
     <tableColumn id="17" name="Responsável pela última alteração" dataDxfId="3"/>
     <tableColumn id="18" name="Motivo Última Alteração" dataDxfId="2"/>
-    <tableColumn id="19" name="Documentação de Apoio" dataDxfId="1"/>
-    <tableColumn id="20" name="Situação do Requisito" dataDxfId="0"/>
+    <tableColumn id="19" name="Documentação de Apoio" dataDxfId="0"/>
+    <tableColumn id="20" name="Situação do Requisito" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2051,25 +2117,25 @@
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2"/>
     <row r="4" spans="2:5" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="22" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2144,7 +2210,18 @@
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E10" s="8"/>
+      <c r="B10" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="8">
+        <v>43747</v>
+      </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E11" s="8"/>
@@ -2214,28 +2291,28 @@
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2"/>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B34" s="26" t="s">
+      <c r="B34" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26"/>
+      <c r="C34" s="33"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="33"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B35" s="26" t="s">
+      <c r="B35" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="26"/>
+      <c r="C35" s="33"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="33"/>
     </row>
     <row r="36" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="26" t="s">
+      <c r="B36" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="C36" s="26"/>
-      <c r="D36" s="26"/>
-      <c r="E36" s="26"/>
+      <c r="C36" s="33"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="33"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2"/>
     <row r="38" spans="2:5" hidden="1" x14ac:dyDescent="0.2"/>
@@ -2267,7 +2344,7 @@
   <dimension ref="A1:V73"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="L5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
       <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
@@ -2276,8 +2353,8 @@
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="3.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.85546875" style="29" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="29" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="49.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
@@ -2294,13 +2371,15 @@
     <col min="17" max="17" width="14.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="17" style="1" customWidth="1"/>
-    <col min="20" max="20" width="16.140625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="16.140625" style="23" customWidth="1"/>
     <col min="21" max="21" width="25.42578125" style="1" customWidth="1"/>
     <col min="22" max="22" width="3.7109375" style="1" customWidth="1"/>
     <col min="23" max="16384" width="9.140625" style="1" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:21" s="13" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
       <c r="J1" s="14"/>
@@ -2312,47 +2391,57 @@
       <c r="P1" s="14"/>
       <c r="Q1" s="17"/>
       <c r="R1" s="9"/>
+      <c r="T1" s="42"/>
       <c r="U1" s="17"/>
     </row>
     <row r="2" spans="2:21" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E2" s="33"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27" t="s">
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="45" t="s">
+        <v>126</v>
+      </c>
+      <c r="E2" s="40"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="29" t="s">
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="31">
+      <c r="P2" s="38">
         <f ca="1">TODAY()</f>
         <v>43719</v>
       </c>
       <c r="R2" s="18"/>
+      <c r="T2" s="42"/>
       <c r="U2" s="17"/>
     </row>
     <row r="3" spans="2:21" s="13" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E3" s="34"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="30"/>
-      <c r="P3" s="32"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="39"/>
+      <c r="T3" s="42"/>
       <c r="U3" s="19"/>
     </row>
-    <row r="4" spans="2:21" s="2" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:21" s="2" customFormat="1" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="12" t="s">
         <v>21</v>
       </c>
@@ -2414,11 +2503,11 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="20">
+    <row r="5" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3">
         <v>1</v>
       </c>
-      <c r="C5" s="20"/>
+      <c r="C5" s="3"/>
       <c r="D5" s="10" t="s">
         <v>41</v>
       </c>
@@ -2432,20 +2521,18 @@
       <c r="H5" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>44</v>
-      </c>
+      <c r="I5" s="4"/>
       <c r="J5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="L5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="M5" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
@@ -2462,40 +2549,40 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T5" s="4"/>
+      <c r="T5" s="43" t="s">
+        <v>120</v>
+      </c>
       <c r="U5" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="20"/>
-      <c r="C6" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>49</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>44</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="I6" s="4"/>
       <c r="J6" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
@@ -2513,36 +2600,38 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T6" s="4"/>
+      <c r="T6" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="U6" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="20"/>
-      <c r="C7" s="20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4" t="s">
-        <v>44</v>
-      </c>
+      <c r="H7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I7" s="4"/>
       <c r="J7" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
@@ -2560,40 +2649,40 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>Adequação ao escopo do projeto</v>
       </c>
-      <c r="T7" s="4"/>
+      <c r="T7" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="U7" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="20"/>
-      <c r="C8" s="20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>44</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="I8" s="4"/>
       <c r="J8" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
@@ -2611,18 +2700,20 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T8" s="4"/>
+      <c r="T8" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="U8" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="20">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="3">
         <v>2</v>
       </c>
-      <c r="C9" s="20"/>
+      <c r="C9" s="3"/>
       <c r="D9" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4" t="s">
@@ -2632,19 +2723,17 @@
         <v>5</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>55</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="I9" s="4"/>
       <c r="J9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K9" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="K9" s="4" t="s">
-        <v>46</v>
-      </c>
       <c r="L9" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
@@ -2662,18 +2751,20 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T9" s="4"/>
+      <c r="T9" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="U9" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="20"/>
-      <c r="C10" s="20" t="s">
-        <v>98</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4" t="s">
@@ -2683,17 +2774,15 @@
         <v>5</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>57</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="I10" s="4"/>
       <c r="J10" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K10" s="4"/>
       <c r="L10" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
@@ -2711,18 +2800,20 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T10" s="4"/>
+      <c r="T10" s="43" t="s">
+        <v>122</v>
+      </c>
       <c r="U10" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="20"/>
-      <c r="C11" s="20" t="s">
-        <v>99</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>90</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4" t="s">
@@ -2732,17 +2823,15 @@
         <v>5</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>57</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="I11" s="4"/>
       <c r="J11" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K11" s="4"/>
       <c r="L11" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
@@ -2760,18 +2849,20 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T11" s="4"/>
+      <c r="T11" s="44" t="s">
+        <v>123</v>
+      </c>
       <c r="U11" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="20">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="3">
         <v>3</v>
       </c>
-      <c r="C12" s="20"/>
+      <c r="C12" s="3"/>
       <c r="D12" s="10" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4" t="s">
@@ -2783,15 +2874,13 @@
       <c r="H12" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I12" s="4" t="s">
-        <v>60</v>
-      </c>
+      <c r="I12" s="4"/>
       <c r="J12" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K12" s="4"/>
       <c r="L12" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
@@ -2809,18 +2898,20 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T12" s="4"/>
+      <c r="T12" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="U12" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="20"/>
-      <c r="C13" s="20" t="s">
-        <v>100</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3" t="s">
+        <v>91</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
@@ -2832,17 +2923,15 @@
       <c r="H13" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I13" s="4" t="s">
-        <v>55</v>
-      </c>
+      <c r="I13" s="4"/>
       <c r="J13" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K13" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="K13" s="4" t="s">
-        <v>46</v>
-      </c>
       <c r="L13" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
@@ -2854,42 +2943,44 @@
         <v>43718</v>
       </c>
       <c r="R13" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="S13" s="4" t="str">
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T13" s="24" t="s">
-        <v>85</v>
+      <c r="T13" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="U13" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="14" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="20"/>
-      <c r="C14" s="20" t="s">
-        <v>101</v>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
+      <c r="F14" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="G14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4" t="s">
-        <v>60</v>
-      </c>
+      <c r="H14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I14" s="4"/>
       <c r="J14" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K14" s="4"/>
       <c r="L14" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
@@ -2907,34 +2998,38 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T14" s="4"/>
+      <c r="T14" s="43" t="s">
+        <v>78</v>
+      </c>
       <c r="U14" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="20"/>
-      <c r="C15" s="20" t="s">
-        <v>102</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
+      <c r="F15" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="G15" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4" t="s">
-        <v>60</v>
-      </c>
+      <c r="H15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I15" s="4"/>
       <c r="J15" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K15" s="4"/>
       <c r="L15" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
@@ -2952,34 +3047,38 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T15" s="4"/>
+      <c r="T15" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="U15" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="20"/>
-      <c r="C16" s="20" t="s">
-        <v>103</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
+      <c r="F16" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="G16" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4" t="s">
-        <v>60</v>
-      </c>
+      <c r="H16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I16" s="4"/>
       <c r="J16" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K16" s="4"/>
       <c r="L16" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
@@ -2997,34 +3096,38 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T16" s="4"/>
+      <c r="T16" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="U16" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="20"/>
-      <c r="C17" s="20" t="s">
-        <v>104</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
+      <c r="F17" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="G17" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4" t="s">
-        <v>60</v>
-      </c>
+      <c r="H17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I17" s="4"/>
       <c r="J17" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K17" s="4"/>
       <c r="L17" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
@@ -3042,36 +3145,38 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T17" s="4"/>
+      <c r="T17" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="U17" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="20"/>
-      <c r="C18" s="20" t="s">
-        <v>105</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="3"/>
+      <c r="C18" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4" t="s">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4" t="s">
-        <v>60</v>
-      </c>
+      <c r="H18" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I18" s="4"/>
       <c r="J18" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K18" s="4"/>
       <c r="L18" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
@@ -3089,36 +3194,38 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>Adequação ao escopo do projeto</v>
       </c>
-      <c r="T18" s="4"/>
+      <c r="T18" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="U18" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="20"/>
-      <c r="C19" s="20" t="s">
-        <v>106</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3" t="s">
+        <v>97</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4" t="s">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4" t="s">
-        <v>60</v>
-      </c>
+      <c r="H19" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I19" s="4"/>
       <c r="J19" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K19" s="4"/>
       <c r="L19" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
@@ -3136,18 +3243,20 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T19" s="4"/>
+      <c r="T19" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="U19" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="20"/>
-      <c r="C20" s="20" t="s">
-        <v>107</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="3"/>
+      <c r="C20" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4" t="s">
@@ -3156,16 +3265,16 @@
       <c r="G20" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4" t="s">
-        <v>60</v>
-      </c>
+      <c r="H20" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I20" s="4"/>
       <c r="J20" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K20" s="4"/>
       <c r="L20" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
@@ -3183,36 +3292,38 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T20" s="4"/>
+      <c r="T20" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="U20" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="20">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="3">
         <v>4</v>
       </c>
-      <c r="C21" s="20"/>
+      <c r="C21" s="3"/>
       <c r="D21" s="11" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4" t="s">
-        <v>69</v>
-      </c>
+      <c r="H21" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I21" s="4"/>
       <c r="J21" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K21" s="4"/>
       <c r="L21" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
@@ -3230,36 +3341,38 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T21" s="4"/>
+      <c r="T21" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="U21" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="20">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="3">
         <v>5</v>
       </c>
-      <c r="C22" s="20"/>
+      <c r="C22" s="3"/>
       <c r="D22" s="10" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4" t="s">
-        <v>69</v>
-      </c>
+      <c r="H22" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I22" s="4"/>
       <c r="J22" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K22" s="4"/>
       <c r="L22" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
@@ -3277,34 +3390,38 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T22" s="4"/>
+      <c r="T22" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="U22" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="2:21" s="21" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="20"/>
-      <c r="C23" s="20" t="s">
-        <v>110</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="2:21" s="20" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
+      <c r="F23" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="G23" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4" t="s">
-        <v>69</v>
-      </c>
+      <c r="H23" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I23" s="4"/>
       <c r="J23" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K23" s="4"/>
       <c r="L23" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
@@ -3322,34 +3439,38 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T23" s="4"/>
+      <c r="T23" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="U23" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="2:21" s="21" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="20"/>
-      <c r="C24" s="20" t="s">
-        <v>111</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="2:21" s="20" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="3"/>
+      <c r="C24" s="3" t="s">
+        <v>102</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
+      <c r="F24" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="G24" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4" t="s">
-        <v>55</v>
-      </c>
+      <c r="H24" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I24" s="4"/>
       <c r="J24" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K24" s="4"/>
       <c r="L24" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
@@ -3367,34 +3488,38 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T24" s="4"/>
+      <c r="T24" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="U24" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="2:21" s="21" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="20"/>
-      <c r="C25" s="20" t="s">
-        <v>112</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="2:21" s="20" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="3"/>
+      <c r="C25" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
+      <c r="F25" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="G25" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4" t="s">
-        <v>55</v>
-      </c>
+      <c r="H25" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I25" s="4"/>
       <c r="J25" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K25" s="4"/>
       <c r="L25" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
@@ -3412,77 +3537,87 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T25" s="4"/>
+      <c r="T25" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="U25" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="2:21" s="39" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="35">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="2:21" s="27" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="3">
         <v>6</v>
       </c>
-      <c r="C26" s="35"/>
-      <c r="D26" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37" t="s">
+      <c r="C26" s="3"/>
+      <c r="D26" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="G26" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="H26" s="37"/>
-      <c r="I26" s="37" t="s">
-        <v>60</v>
-      </c>
-      <c r="J26" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="K26" s="37"/>
-      <c r="L26" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="M26" s="37"/>
-      <c r="N26" s="37"/>
-      <c r="O26" s="37"/>
-      <c r="P26" s="38">
+      <c r="H26" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I26" s="25"/>
+      <c r="J26" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="K26" s="25"/>
+      <c r="L26" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="M26" s="25"/>
+      <c r="N26" s="25"/>
+      <c r="O26" s="25"/>
+      <c r="P26" s="26">
         <v>43716</v>
       </c>
-      <c r="Q26" s="38">
+      <c r="Q26" s="26">
         <v>43716</v>
       </c>
-      <c r="R26" s="37" t="s">
+      <c r="R26" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="S26" s="37" t="str">
+      <c r="S26" s="25" t="str">
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T26" s="37"/>
-      <c r="U26" s="37" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
+      <c r="T26" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="U26" s="25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="3">
+        <v>7</v>
+      </c>
+      <c r="C27" s="3"/>
       <c r="D27" s="10" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
+      <c r="F27" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="G27" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4" t="s">
-        <v>55</v>
-      </c>
+      <c r="H27" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I27" s="4"/>
       <c r="J27" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K27" s="4"/>
       <c r="L27" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
@@ -3500,32 +3635,38 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T27" s="4"/>
+      <c r="T27" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="U27" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="21" t="s">
-        <v>76</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="3">
+        <v>8</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="20" t="s">
+        <v>70</v>
       </c>
       <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
+      <c r="F28" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="G28" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4" t="s">
-        <v>60</v>
-      </c>
+      <c r="H28" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I28" s="4"/>
       <c r="J28" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K28" s="4"/>
       <c r="L28" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
@@ -3543,32 +3684,38 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T28" s="4"/>
+      <c r="T28" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="U28" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="21" t="s">
-        <v>77</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="3"/>
+      <c r="C29" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D29" s="20" t="s">
+        <v>71</v>
       </c>
       <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
+      <c r="F29" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="G29" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4" t="s">
-        <v>57</v>
-      </c>
+      <c r="H29" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I29" s="4"/>
       <c r="J29" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K29" s="4"/>
       <c r="L29" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
@@ -3586,32 +3733,38 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T29" s="4"/>
+      <c r="T29" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="U29" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="30" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="3"/>
+      <c r="C30" s="3" t="s">
+        <v>106</v>
+      </c>
       <c r="D30" s="10" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
+      <c r="F30" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="G30" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4" t="s">
-        <v>57</v>
-      </c>
+      <c r="H30" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I30" s="4"/>
       <c r="J30" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K30" s="4"/>
       <c r="L30" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
@@ -3629,34 +3782,38 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T30" s="4"/>
+      <c r="T30" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="U30" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="31" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="3"/>
+      <c r="C31" s="3" t="s">
+        <v>114</v>
+      </c>
       <c r="D31" s="10" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4" t="s">
-        <v>108</v>
+        <v>42</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4" t="s">
-        <v>55</v>
-      </c>
+      <c r="H31" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I31" s="4"/>
       <c r="J31" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K31" s="4"/>
       <c r="L31" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M31" s="4"/>
       <c r="N31" s="4"/>
@@ -3674,32 +3831,38 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T31" s="4"/>
+      <c r="T31" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="U31" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="32" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="20"/>
-      <c r="C32" s="20"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="3">
+        <v>9</v>
+      </c>
+      <c r="C32" s="3"/>
       <c r="D32" s="10" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
+      <c r="F32" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="G32" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4" t="s">
-        <v>60</v>
-      </c>
+      <c r="H32" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I32" s="4"/>
       <c r="J32" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K32" s="4"/>
       <c r="L32" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
@@ -3717,32 +3880,38 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T32" s="4"/>
+      <c r="T32" s="44" t="s">
+        <v>124</v>
+      </c>
       <c r="U32" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="33" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="3">
+        <v>10</v>
+      </c>
+      <c r="C33" s="3"/>
       <c r="D33" s="10" t="s">
-        <v>81</v>
+        <v>121</v>
       </c>
       <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
+      <c r="F33" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="G33" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4" t="s">
-        <v>60</v>
-      </c>
+      <c r="H33" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I33" s="4"/>
       <c r="J33" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K33" s="4"/>
       <c r="L33" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
@@ -3760,32 +3929,38 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T33" s="4"/>
+      <c r="T33" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="U33" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="34" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="3"/>
+      <c r="C34" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="D34" s="10" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
+      <c r="F34" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="G34" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4" t="s">
-        <v>55</v>
-      </c>
+      <c r="H34" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I34" s="4"/>
       <c r="J34" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K34" s="4"/>
       <c r="L34" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
@@ -3803,32 +3978,38 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T34" s="4"/>
+      <c r="T34" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="U34" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="35" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="20"/>
-      <c r="C35" s="20"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="3"/>
+      <c r="C35" s="3" t="s">
+        <v>108</v>
+      </c>
       <c r="D35" s="10" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
+      <c r="F35" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="G35" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4" t="s">
-        <v>55</v>
-      </c>
+      <c r="H35" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I35" s="4"/>
       <c r="J35" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K35" s="4"/>
       <c r="L35" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M35" s="4"/>
       <c r="N35" s="4"/>
@@ -3846,38 +4027,44 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T35" s="4"/>
+      <c r="T35" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="U35" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="36" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="20"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="21" t="s">
-        <v>84</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="3"/>
+      <c r="C36" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>76</v>
       </c>
       <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
+      <c r="F36" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="G36" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4" t="s">
-        <v>60</v>
-      </c>
+      <c r="H36" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I36" s="4"/>
       <c r="J36" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K36" s="4"/>
       <c r="L36" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M36" s="4"/>
       <c r="N36" s="4"/>
       <c r="O36" s="4"/>
       <c r="P36" s="5">
-        <v>43714</v>
+        <v>43716</v>
       </c>
       <c r="Q36" s="5">
         <v>43716</v>
@@ -3887,44 +4074,75 @@
       </c>
       <c r="S36" s="4" t="str">
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
-        <v>Adequação ao escopo do projeto</v>
-      </c>
-      <c r="T36" s="4"/>
+        <v>N/A</v>
+      </c>
+      <c r="T36" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="U36" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="37" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="20"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="10"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="3"/>
+      <c r="C37" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>111</v>
+      </c>
       <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
+      <c r="F37" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
+      <c r="J37" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="K37" s="4"/>
-      <c r="L37" s="4"/>
+      <c r="L37" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="M37" s="4"/>
       <c r="N37" s="4"/>
       <c r="O37" s="4"/>
-      <c r="P37" s="5"/>
-      <c r="Q37" s="5"/>
-      <c r="R37" s="4"/>
-      <c r="S37" s="4"/>
-      <c r="T37" s="24"/>
-      <c r="U37" s="4"/>
-    </row>
-    <row r="38" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="20"/>
-      <c r="C38" s="20"/>
+      <c r="P37" s="5">
+        <v>43714</v>
+      </c>
+      <c r="Q37" s="5">
+        <v>43716</v>
+      </c>
+      <c r="R37" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="S37" s="4" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>Adequação ao escopo do projeto</v>
+      </c>
+      <c r="T37" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="U37" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="3"/>
+      <c r="C38" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="D38" s="10" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4" t="s">
-        <v>42</v>
+        <v>99</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>5</v>
@@ -3932,17 +4150,13 @@
       <c r="H38" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I38" s="4" t="s">
-        <v>60</v>
-      </c>
+      <c r="I38" s="4"/>
       <c r="J38" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="K38" s="4" t="s">
-        <v>46</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="K38" s="4"/>
       <c r="L38" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M38" s="4"/>
       <c r="N38" s="4"/>
@@ -3953,27 +4167,29 @@
       <c r="Q38" s="5">
         <v>43718</v>
       </c>
-      <c r="R38" s="4" t="s">
-        <v>46</v>
-      </c>
+      <c r="R38" s="4"/>
       <c r="S38" s="4" t="str">
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T38" s="24"/>
+      <c r="T38" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="U38" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="39" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="20"/>
-      <c r="C39" s="20"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="3"/>
+      <c r="C39" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="D39" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>5</v>
@@ -3981,17 +4197,13 @@
       <c r="H39" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I39" s="4" t="s">
-        <v>60</v>
-      </c>
+      <c r="I39" s="4"/>
       <c r="J39" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="K39" s="4" t="s">
-        <v>46</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="K39" s="4"/>
       <c r="L39" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M39" s="4"/>
       <c r="N39" s="4"/>
@@ -4002,37 +4214,43 @@
       <c r="Q39" s="5">
         <v>43718</v>
       </c>
-      <c r="R39" s="4" t="s">
-        <v>46</v>
-      </c>
+      <c r="R39" s="4"/>
       <c r="S39" s="4" t="str">
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T39" s="24"/>
+      <c r="T39" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="U39" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="3"/>
+      <c r="C40" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D40" s="10" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="40" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="20"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="10" t="s">
-        <v>89</v>
-      </c>
       <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
+      <c r="F40" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="G40" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H40" s="4"/>
+      <c r="H40" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="I40" s="4"/>
       <c r="J40" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K40" s="4"/>
       <c r="L40" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M40" s="4"/>
       <c r="N40" s="4"/>
@@ -4048,30 +4266,38 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T40" s="4"/>
+      <c r="T40" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="U40" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="41" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="20"/>
-      <c r="C41" s="20"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="3"/>
+      <c r="C41" s="3" t="s">
+        <v>118</v>
+      </c>
       <c r="D41" s="10" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
+      <c r="F41" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="G41" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H41" s="4"/>
+      <c r="H41" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="I41" s="4"/>
       <c r="J41" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K41" s="4"/>
       <c r="L41" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M41" s="4"/>
       <c r="N41" s="4"/>
@@ -4087,30 +4313,38 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T41" s="4"/>
+      <c r="T41" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="U41" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="42" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="20"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="10" t="s">
-        <v>91</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="3">
+        <v>11</v>
+      </c>
+      <c r="C42" s="3"/>
+      <c r="D42" s="11" t="s">
+        <v>77</v>
       </c>
       <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
+      <c r="F42" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="G42" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H42" s="4"/>
-      <c r="I42" s="4"/>
+      <c r="H42" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I42" s="30"/>
       <c r="J42" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K42" s="4"/>
       <c r="L42" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M42" s="4"/>
       <c r="N42" s="4"/>
@@ -4126,30 +4360,40 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T42" s="4"/>
-      <c r="U42" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="43" spans="2:21" s="21" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="20"/>
-      <c r="C43" s="20"/>
-      <c r="D43" s="10" t="s">
-        <v>92</v>
+      <c r="T42" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="U42" s="31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="43" spans="2:21" s="20" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="3">
+        <v>12</v>
+      </c>
+      <c r="C43" s="3"/>
+      <c r="D43" s="11" t="s">
+        <v>80</v>
       </c>
       <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
+      <c r="F43" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="G43" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4"/>
+      <c r="H43" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I43" s="30"/>
       <c r="J43" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K43" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="K43" s="4"/>
       <c r="L43" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M43" s="4"/>
       <c r="N43" s="4"/>
@@ -4160,35 +4404,47 @@
       <c r="Q43" s="5">
         <v>43718</v>
       </c>
-      <c r="R43" s="4"/>
+      <c r="R43" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="S43" s="4" t="str">
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T43" s="4"/>
-      <c r="U43" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="44" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
-      <c r="D44" s="10" t="s">
-        <v>93</v>
+      <c r="T43" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="U43" s="31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="2:21" s="20" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="3"/>
+      <c r="C44" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>112</v>
       </c>
       <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
+      <c r="F44" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="G44" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H44" s="4"/>
-      <c r="I44" s="4"/>
+      <c r="H44" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I44" s="30"/>
       <c r="J44" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K44" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="K44" s="4"/>
       <c r="L44" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M44" s="4"/>
       <c r="N44" s="4"/>
@@ -4199,35 +4455,43 @@
       <c r="Q44" s="5">
         <v>43718</v>
       </c>
-      <c r="R44" s="4"/>
+      <c r="R44" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="S44" s="4" t="str">
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T44" s="4"/>
-      <c r="U44" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="45" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="20"/>
-      <c r="C45" s="20"/>
+      <c r="T44" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="U44" s="31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="3">
+        <v>13</v>
+      </c>
+      <c r="C45" s="3"/>
       <c r="D45" s="10" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H45" s="4"/>
+      <c r="H45" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="I45" s="4"/>
       <c r="J45" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K45" s="4"/>
       <c r="L45" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M45" s="4"/>
       <c r="N45" s="4"/>
@@ -4243,30 +4507,36 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T45" s="4"/>
+      <c r="T45" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="U45" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="46" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="20"/>
-      <c r="C46" s="20"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="2:21" s="20" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="3">
+        <v>14</v>
+      </c>
+      <c r="C46" s="3"/>
       <c r="D46" s="10" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
       <c r="G46" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H46" s="4"/>
+      <c r="H46" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="I46" s="4"/>
       <c r="J46" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K46" s="4"/>
       <c r="L46" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M46" s="4"/>
       <c r="N46" s="4"/>
@@ -4282,30 +4552,38 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T46" s="4"/>
+      <c r="T46" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="U46" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="47" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="20"/>
-      <c r="C47" s="20"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="3">
+        <v>15</v>
+      </c>
+      <c r="C47" s="3"/>
       <c r="D47" s="10" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
+      <c r="F47" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="G47" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H47" s="4"/>
+      <c r="H47" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="I47" s="4"/>
       <c r="J47" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K47" s="4"/>
       <c r="L47" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M47" s="4"/>
       <c r="N47" s="4"/>
@@ -4321,59 +4599,44 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T47" s="4"/>
+      <c r="T47" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="U47" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="48" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="20"/>
-      <c r="C48" s="20"/>
-      <c r="D48" s="10" t="s">
-        <v>97</v>
-      </c>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="11"/>
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
-      <c r="G48" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="G48" s="4"/>
       <c r="H48" s="4"/>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="I48" s="30"/>
+      <c r="J48" s="4"/>
       <c r="K48" s="4"/>
-      <c r="L48" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="L48" s="4"/>
       <c r="M48" s="4"/>
       <c r="N48" s="4"/>
       <c r="O48" s="4"/>
-      <c r="P48" s="5">
-        <v>43718</v>
-      </c>
-      <c r="Q48" s="5">
-        <v>43718</v>
-      </c>
+      <c r="P48" s="5"/>
+      <c r="Q48" s="4"/>
       <c r="R48" s="4"/>
-      <c r="S48" s="4" t="str">
-        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
-        <v>N/A</v>
-      </c>
-      <c r="T48" s="4"/>
-      <c r="U48" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="49" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="20"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="10"/>
+      <c r="S48" s="4"/>
+      <c r="T48" s="10"/>
+      <c r="U48" s="31"/>
+    </row>
+    <row r="49" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="11"/>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
       <c r="H49" s="4"/>
-      <c r="I49" s="4"/>
+      <c r="I49" s="30"/>
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
       <c r="L49" s="4"/>
@@ -4384,18 +4647,18 @@
       <c r="Q49" s="4"/>
       <c r="R49" s="4"/>
       <c r="S49" s="4"/>
-      <c r="T49" s="4"/>
-      <c r="U49" s="4"/>
-    </row>
-    <row r="50" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="20"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="10"/>
+      <c r="T49" s="10"/>
+      <c r="U49" s="31"/>
+    </row>
+    <row r="50" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="11"/>
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
-      <c r="I50" s="4"/>
+      <c r="I50" s="30"/>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
       <c r="L50" s="4"/>
@@ -4406,18 +4669,18 @@
       <c r="Q50" s="4"/>
       <c r="R50" s="4"/>
       <c r="S50" s="4"/>
-      <c r="T50" s="4"/>
-      <c r="U50" s="4"/>
-    </row>
-    <row r="51" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="20"/>
-      <c r="C51" s="20"/>
-      <c r="D51" s="10"/>
+      <c r="T50" s="10"/>
+      <c r="U50" s="31"/>
+    </row>
+    <row r="51" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="11"/>
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
-      <c r="I51" s="4"/>
+      <c r="I51" s="30"/>
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
       <c r="L51" s="4"/>
@@ -4428,12 +4691,12 @@
       <c r="Q51" s="4"/>
       <c r="R51" s="4"/>
       <c r="S51" s="4"/>
-      <c r="T51" s="4"/>
-      <c r="U51" s="4"/>
-    </row>
-    <row r="52" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="20"/>
-      <c r="C52" s="20"/>
+      <c r="T51" s="10"/>
+      <c r="U51" s="31"/>
+    </row>
+    <row r="52" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
       <c r="D52" s="10"/>
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
@@ -4450,18 +4713,18 @@
       <c r="Q52" s="4"/>
       <c r="R52" s="4"/>
       <c r="S52" s="4"/>
-      <c r="T52" s="4"/>
+      <c r="T52" s="10"/>
       <c r="U52" s="4"/>
     </row>
-    <row r="53" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="20"/>
-      <c r="C53" s="20"/>
-      <c r="D53" s="10"/>
+    <row r="53" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="11"/>
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
-      <c r="I53" s="4"/>
+      <c r="I53" s="30"/>
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
@@ -4472,18 +4735,18 @@
       <c r="Q53" s="4"/>
       <c r="R53" s="4"/>
       <c r="S53" s="4"/>
-      <c r="T53" s="4"/>
-      <c r="U53" s="4"/>
-    </row>
-    <row r="54" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="20"/>
-      <c r="C54" s="20"/>
-      <c r="D54" s="10"/>
+      <c r="T53" s="10"/>
+      <c r="U53" s="31"/>
+    </row>
+    <row r="54" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="11"/>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
-      <c r="I54" s="4"/>
+      <c r="I54" s="30"/>
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
@@ -4494,18 +4757,18 @@
       <c r="Q54" s="4"/>
       <c r="R54" s="4"/>
       <c r="S54" s="4"/>
-      <c r="T54" s="4"/>
-      <c r="U54" s="4"/>
-    </row>
-    <row r="55" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="20"/>
-      <c r="C55" s="20"/>
-      <c r="D55" s="10"/>
+      <c r="T54" s="10"/>
+      <c r="U54" s="31"/>
+    </row>
+    <row r="55" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="11"/>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
-      <c r="I55" s="4"/>
+      <c r="I55" s="30"/>
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
       <c r="L55" s="4"/>
@@ -4516,12 +4779,12 @@
       <c r="Q55" s="4"/>
       <c r="R55" s="4"/>
       <c r="S55" s="4"/>
-      <c r="T55" s="4"/>
-      <c r="U55" s="4"/>
-    </row>
-    <row r="56" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="20"/>
-      <c r="C56" s="20"/>
+      <c r="T55" s="10"/>
+      <c r="U55" s="31"/>
+    </row>
+    <row r="56" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
       <c r="D56" s="10"/>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
@@ -4538,12 +4801,12 @@
       <c r="Q56" s="4"/>
       <c r="R56" s="4"/>
       <c r="S56" s="4"/>
-      <c r="T56" s="4"/>
+      <c r="T56" s="10"/>
       <c r="U56" s="4"/>
     </row>
-    <row r="57" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="20"/>
-      <c r="C57" s="20"/>
+    <row r="57" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
       <c r="D57" s="10"/>
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
@@ -4560,12 +4823,12 @@
       <c r="Q57" s="4"/>
       <c r="R57" s="4"/>
       <c r="S57" s="4"/>
-      <c r="T57" s="4"/>
+      <c r="T57" s="10"/>
       <c r="U57" s="4"/>
     </row>
-    <row r="58" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="20"/>
-      <c r="C58" s="20"/>
+    <row r="58" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
       <c r="D58" s="10"/>
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
@@ -4582,12 +4845,12 @@
       <c r="Q58" s="4"/>
       <c r="R58" s="4"/>
       <c r="S58" s="4"/>
-      <c r="T58" s="4"/>
+      <c r="T58" s="10"/>
       <c r="U58" s="4"/>
     </row>
-    <row r="59" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="20"/>
-      <c r="C59" s="20"/>
+    <row r="59" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
       <c r="D59" s="10"/>
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
@@ -4604,12 +4867,12 @@
       <c r="Q59" s="4"/>
       <c r="R59" s="4"/>
       <c r="S59" s="4"/>
-      <c r="T59" s="4"/>
+      <c r="T59" s="10"/>
       <c r="U59" s="4"/>
     </row>
-    <row r="60" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="20"/>
-      <c r="C60" s="20"/>
+    <row r="60" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
       <c r="D60" s="10"/>
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
@@ -4626,12 +4889,12 @@
       <c r="Q60" s="4"/>
       <c r="R60" s="4"/>
       <c r="S60" s="4"/>
-      <c r="T60" s="4"/>
+      <c r="T60" s="10"/>
       <c r="U60" s="4"/>
     </row>
-    <row r="61" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="20"/>
-      <c r="C61" s="20"/>
+    <row r="61" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
       <c r="D61" s="10"/>
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
@@ -4648,12 +4911,12 @@
       <c r="Q61" s="4"/>
       <c r="R61" s="4"/>
       <c r="S61" s="4"/>
-      <c r="T61" s="4"/>
+      <c r="T61" s="10"/>
       <c r="U61" s="4"/>
     </row>
-    <row r="62" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="20"/>
-      <c r="C62" s="20"/>
+    <row r="62" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
       <c r="D62" s="10"/>
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
@@ -4670,12 +4933,12 @@
       <c r="Q62" s="4"/>
       <c r="R62" s="4"/>
       <c r="S62" s="4"/>
-      <c r="T62" s="4"/>
+      <c r="T62" s="10"/>
       <c r="U62" s="4"/>
     </row>
-    <row r="63" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="20"/>
-      <c r="C63" s="20"/>
+    <row r="63" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
       <c r="D63" s="10"/>
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
@@ -4692,12 +4955,12 @@
       <c r="Q63" s="4"/>
       <c r="R63" s="4"/>
       <c r="S63" s="4"/>
-      <c r="T63" s="4"/>
+      <c r="T63" s="10"/>
       <c r="U63" s="4"/>
     </row>
-    <row r="64" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="20"/>
-      <c r="C64" s="20"/>
+    <row r="64" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
       <c r="D64" s="10"/>
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
@@ -4714,12 +4977,12 @@
       <c r="Q64" s="4"/>
       <c r="R64" s="4"/>
       <c r="S64" s="4"/>
-      <c r="T64" s="4"/>
+      <c r="T64" s="10"/>
       <c r="U64" s="4"/>
     </row>
-    <row r="65" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="20"/>
-      <c r="C65" s="20"/>
+    <row r="65" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
       <c r="D65" s="10"/>
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
@@ -4736,12 +4999,12 @@
       <c r="Q65" s="4"/>
       <c r="R65" s="4"/>
       <c r="S65" s="4"/>
-      <c r="T65" s="4"/>
+      <c r="T65" s="10"/>
       <c r="U65" s="4"/>
     </row>
-    <row r="66" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="20"/>
-      <c r="C66" s="20"/>
+    <row r="66" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
       <c r="D66" s="10"/>
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
@@ -4758,12 +5021,12 @@
       <c r="Q66" s="4"/>
       <c r="R66" s="4"/>
       <c r="S66" s="4"/>
-      <c r="T66" s="4"/>
+      <c r="T66" s="10"/>
       <c r="U66" s="4"/>
     </row>
-    <row r="67" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="20"/>
-      <c r="C67" s="20"/>
+    <row r="67" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
       <c r="D67" s="10"/>
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
@@ -4780,12 +5043,12 @@
       <c r="Q67" s="4"/>
       <c r="R67" s="4"/>
       <c r="S67" s="4"/>
-      <c r="T67" s="4"/>
+      <c r="T67" s="10"/>
       <c r="U67" s="4"/>
     </row>
-    <row r="68" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="20"/>
-      <c r="C68" s="20"/>
+    <row r="68" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
       <c r="D68" s="10"/>
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
@@ -4802,12 +5065,12 @@
       <c r="Q68" s="4"/>
       <c r="R68" s="4"/>
       <c r="S68" s="4"/>
-      <c r="T68" s="4"/>
+      <c r="T68" s="10"/>
       <c r="U68" s="4"/>
     </row>
-    <row r="69" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="20"/>
-      <c r="C69" s="20"/>
+    <row r="69" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
       <c r="D69" s="10"/>
       <c r="E69" s="4"/>
       <c r="F69" s="4"/>
@@ -4824,12 +5087,12 @@
       <c r="Q69" s="4"/>
       <c r="R69" s="4"/>
       <c r="S69" s="4"/>
-      <c r="T69" s="4"/>
+      <c r="T69" s="10"/>
       <c r="U69" s="4"/>
     </row>
-    <row r="70" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="20"/>
-      <c r="C70" s="20"/>
+    <row r="70" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
       <c r="D70" s="10"/>
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
@@ -4846,12 +5109,12 @@
       <c r="Q70" s="4"/>
       <c r="R70" s="4"/>
       <c r="S70" s="4"/>
-      <c r="T70" s="4"/>
+      <c r="T70" s="10"/>
       <c r="U70" s="4"/>
     </row>
-    <row r="71" spans="2:21" s="21" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="20"/>
-      <c r="C71" s="20"/>
+    <row r="71" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
       <c r="D71" s="10"/>
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
@@ -4868,11 +5131,11 @@
       <c r="Q71" s="4"/>
       <c r="R71" s="4"/>
       <c r="S71" s="4"/>
-      <c r="T71" s="4"/>
+      <c r="T71" s="10"/>
       <c r="U71" s="4"/>
     </row>
     <row r="72" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="N72" s="22"/>
+      <c r="N72" s="21"/>
     </row>
     <row r="73" spans="2:21" hidden="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -4889,47 +5152,41 @@
     <mergeCell ref="M2:M3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U5:U71">
+  <dataValidations disablePrompts="1" count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U56:U71 U5:U47 U52">
       <formula1>"Proposto,Aprovado,Projetado,Implementado,Verificado, Entregue, Eliminado, Rejeitado"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I71">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I56:I71 I5:I47 I52">
       <formula1>"Máxima,Alta,Média,Baixa,Mínima"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H71">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H56:H71 H5:H47 H52">
       <formula1>"Funcional,Não Funcional"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L40:L48 J5:J71">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J56:J71 L38:L41 L45:L47 J5:J47 J52">
       <formula1>"Gerson Santos,Célia Taniwaki,José Yoshihiro,Alex Barreira"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R5:R71 K5:K71">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R56:R71 K56:K71 R5:R47 R52 K5:K47 K52">
       <formula1>"Fernando Abreu,João Vinícius,Kessi Santana,Thalita Igwe,Vitoria Ferreira"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L49:L71 L5:L39">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L42:L44 L56:L71 L5:L37 L52">
       <formula1>"Gerson Santos,Fernando Abreu,João Vinícius,Kessi Santana,Thalita Igwe,Vitoria Ferreira,Célia Taniwaki,Alex Barreira,José Yoshihiro"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F71">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F56:F71 F5:F47 F52">
       <formula1>"Essencial,Importante,Desejável"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="T5" r:id="rId1"/>
+    <hyperlink ref="T10" r:id="rId2"/>
+    <hyperlink ref="T11" r:id="rId3"/>
+    <hyperlink ref="T32" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId5"/>
   <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId6"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Alteração requisitos e slides.
</commit_message>
<xml_diff>
--- a/documentacao/requisitos.xlsx
+++ b/documentacao/requisitos.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="130">
   <si>
     <t>Histórico de alterações do documento</t>
   </si>
@@ -480,12 +480,6 @@
     <t>10.6</t>
   </si>
   <si>
-    <t>10.7</t>
-  </si>
-  <si>
-    <t>10.8</t>
-  </si>
-  <si>
     <t>1.5</t>
   </si>
   <si>
@@ -508,13 +502,28 @@
   </si>
   <si>
     <t>USER PREMIUN E FREE</t>
+  </si>
+  <si>
+    <t>Baixa</t>
+  </si>
+  <si>
+    <t>Alta</t>
+  </si>
+  <si>
+    <t>Mínima</t>
+  </si>
+  <si>
+    <t>Máxima</t>
+  </si>
+  <si>
+    <t>Média</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -586,6 +595,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -767,7 +782,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -862,6 +877,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -892,17 +919,8 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -926,14 +944,12 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
           <color theme="0"/>
         </left>
-        <right style="medium">
-          <color theme="0"/>
-        </right>
+        <right/>
         <top style="medium">
           <color theme="0"/>
         </top>
@@ -958,12 +974,14 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
           <color theme="0"/>
         </left>
-        <right/>
+        <right style="medium">
+          <color theme="0"/>
+        </right>
         <top style="medium">
           <color theme="0"/>
         </top>
@@ -1784,8 +1802,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="requisitos" displayName="requisitos" ref="D4:U71" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18">
-  <autoFilter ref="D4:U71"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="requisitos" displayName="requisitos" ref="D4:U69" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18">
+  <autoFilter ref="D4:U69"/>
   <tableColumns count="18">
     <tableColumn id="1" name="Descrição do Requisito" dataDxfId="17"/>
     <tableColumn id="2" name="Objetivo / Estratégia de Negócio" dataDxfId="16"/>
@@ -1803,8 +1821,8 @@
     <tableColumn id="16" name="Data Última Alteração" dataDxfId="4"/>
     <tableColumn id="17" name="Responsável pela última alteração" dataDxfId="3"/>
     <tableColumn id="18" name="Motivo Última Alteração" dataDxfId="2"/>
-    <tableColumn id="19" name="Documentação de Apoio" dataDxfId="0"/>
-    <tableColumn id="20" name="Situação do Requisito" dataDxfId="1"/>
+    <tableColumn id="19" name="Documentação de Apoio" dataDxfId="1"/>
+    <tableColumn id="20" name="Situação do Requisito" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2101,7 +2119,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -2117,12 +2135,12 @@
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2"/>
     <row r="4" spans="2:5" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -2139,7 +2157,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
@@ -2153,7 +2171,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="7" t="s">
         <v>9</v>
       </c>
@@ -2167,7 +2185,7 @@
         <v>43533</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2181,7 +2199,7 @@
         <v>43594</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="7" t="s">
         <v>13</v>
       </c>
@@ -2195,7 +2213,7 @@
         <v>43625</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="7" t="s">
         <v>15</v>
       </c>
@@ -2209,9 +2227,9 @@
         <v>43686</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>14</v>
@@ -2223,96 +2241,96 @@
         <v>43747</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E11" s="8"/>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E12" s="8"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E13" s="8"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E14" s="8"/>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E15" s="8"/>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E16" s="8"/>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="5:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E17" s="8"/>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="5:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E18" s="8"/>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="5:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E19" s="8"/>
     </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="5:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E20" s="8"/>
     </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="5:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E21" s="8"/>
     </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="5:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E22" s="8"/>
     </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="5:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E23" s="8"/>
     </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="5:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E24" s="8"/>
     </row>
-    <row r="25" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="5:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E25" s="8"/>
     </row>
-    <row r="26" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="5:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E26" s="8"/>
     </row>
-    <row r="27" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="5:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E27" s="8"/>
     </row>
-    <row r="28" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="5:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E28" s="8"/>
     </row>
-    <row r="29" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="5:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E29" s="8"/>
     </row>
-    <row r="30" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="5:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E30" s="8"/>
     </row>
-    <row r="31" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="5:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E31" s="8"/>
     </row>
-    <row r="32" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="5:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E32" s="8"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2"/>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B34" s="33" t="s">
+      <c r="B34" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="33"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="33"/>
+      <c r="C34" s="37"/>
+      <c r="D34" s="37"/>
+      <c r="E34" s="37"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B35" s="33" t="s">
+      <c r="B35" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="C35" s="33"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
+      <c r="C35" s="37"/>
+      <c r="D35" s="37"/>
+      <c r="E35" s="37"/>
     </row>
     <row r="36" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="33" t="s">
+      <c r="B36" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="C36" s="33"/>
-      <c r="D36" s="33"/>
-      <c r="E36" s="33"/>
+      <c r="C36" s="37"/>
+      <c r="D36" s="37"/>
+      <c r="E36" s="37"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2"/>
     <row r="38" spans="2:5" hidden="1" x14ac:dyDescent="0.2"/>
@@ -2344,7 +2362,7 @@
   <dimension ref="A1:V73"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="L5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="P5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
       <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
@@ -2391,54 +2409,54 @@
       <c r="P1" s="14"/>
       <c r="Q1" s="17"/>
       <c r="R1" s="9"/>
-      <c r="T1" s="42"/>
+      <c r="T1" s="32"/>
       <c r="U1" s="17"/>
     </row>
     <row r="2" spans="2:21" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="28"/>
       <c r="C2" s="28"/>
-      <c r="D2" s="45" t="s">
-        <v>126</v>
-      </c>
-      <c r="E2" s="40"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34" t="s">
+      <c r="D2" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" s="44"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="36" t="s">
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="38">
+      <c r="P2" s="42">
         <f ca="1">TODAY()</f>
         <v>43719</v>
       </c>
       <c r="R2" s="18"/>
-      <c r="T2" s="42"/>
+      <c r="T2" s="32"/>
       <c r="U2" s="17"/>
     </row>
     <row r="3" spans="2:21" s="13" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="28"/>
       <c r="C3" s="28"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="39"/>
-      <c r="T3" s="42"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="41"/>
+      <c r="P3" s="43"/>
+      <c r="T3" s="32"/>
       <c r="U3" s="19"/>
     </row>
     <row r="4" spans="2:21" s="2" customFormat="1" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2521,7 +2539,9 @@
       <c r="H5" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I5" s="4"/>
+      <c r="I5" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="J5" s="4" t="s">
         <v>44</v>
       </c>
@@ -2549,8 +2569,8 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T5" s="43" t="s">
-        <v>120</v>
+      <c r="T5" s="33" t="s">
+        <v>118</v>
       </c>
       <c r="U5" s="4" t="s">
         <v>47</v>
@@ -2574,7 +2594,9 @@
       <c r="H6" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="I6" s="4"/>
+      <c r="I6" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="J6" s="4" t="s">
         <v>44</v>
       </c>
@@ -2601,7 +2623,7 @@
         <v>N/A</v>
       </c>
       <c r="T6" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U6" s="4" t="s">
         <v>47</v>
@@ -2625,7 +2647,9 @@
       <c r="H7" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="I7" s="4"/>
+      <c r="I7" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="J7" s="4" t="s">
         <v>44</v>
       </c>
@@ -2650,7 +2674,7 @@
         <v>Adequação ao escopo do projeto</v>
       </c>
       <c r="T7" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U7" s="4" t="s">
         <v>47</v>
@@ -2674,7 +2698,9 @@
       <c r="H8" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="I8" s="4"/>
+      <c r="I8" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="J8" s="4" t="s">
         <v>44</v>
       </c>
@@ -2701,7 +2727,7 @@
         <v>N/A</v>
       </c>
       <c r="T8" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U8" s="4" t="s">
         <v>47</v>
@@ -2725,7 +2751,9 @@
       <c r="H9" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="I9" s="4"/>
+      <c r="I9" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="J9" s="4" t="s">
         <v>44</v>
       </c>
@@ -2752,7 +2780,7 @@
         <v>N/A</v>
       </c>
       <c r="T9" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U9" s="4" t="s">
         <v>47</v>
@@ -2776,7 +2804,9 @@
       <c r="H10" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="I10" s="4"/>
+      <c r="I10" s="4" t="s">
+        <v>127</v>
+      </c>
       <c r="J10" s="4" t="s">
         <v>44</v>
       </c>
@@ -2800,8 +2830,8 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T10" s="43" t="s">
-        <v>122</v>
+      <c r="T10" s="33" t="s">
+        <v>120</v>
       </c>
       <c r="U10" s="4" t="s">
         <v>47</v>
@@ -2825,7 +2855,9 @@
       <c r="H11" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="I11" s="4"/>
+      <c r="I11" s="4" t="s">
+        <v>127</v>
+      </c>
       <c r="J11" s="4" t="s">
         <v>44</v>
       </c>
@@ -2849,8 +2881,8 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T11" s="44" t="s">
-        <v>123</v>
+      <c r="T11" s="34" t="s">
+        <v>121</v>
       </c>
       <c r="U11" s="4" t="s">
         <v>47</v>
@@ -2874,7 +2906,9 @@
       <c r="H12" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I12" s="4"/>
+      <c r="I12" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="J12" s="4" t="s">
         <v>44</v>
       </c>
@@ -2899,7 +2933,7 @@
         <v>N/A</v>
       </c>
       <c r="T12" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U12" s="4" t="s">
         <v>47</v>
@@ -2923,7 +2957,9 @@
       <c r="H13" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I13" s="4"/>
+      <c r="I13" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="J13" s="4" t="s">
         <v>44</v>
       </c>
@@ -2950,7 +2986,7 @@
         <v>N/A</v>
       </c>
       <c r="T13" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U13" s="4" t="s">
         <v>79</v>
@@ -2974,7 +3010,9 @@
       <c r="H14" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I14" s="4"/>
+      <c r="I14" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="J14" s="4" t="s">
         <v>44</v>
       </c>
@@ -2998,7 +3036,7 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T14" s="43" t="s">
+      <c r="T14" s="33" t="s">
         <v>78</v>
       </c>
       <c r="U14" s="4" t="s">
@@ -3023,7 +3061,9 @@
       <c r="H15" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I15" s="4"/>
+      <c r="I15" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="J15" s="4" t="s">
         <v>44</v>
       </c>
@@ -3048,7 +3088,7 @@
         <v>N/A</v>
       </c>
       <c r="T15" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U15" s="4" t="s">
         <v>47</v>
@@ -3072,7 +3112,9 @@
       <c r="H16" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I16" s="4"/>
+      <c r="I16" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="J16" s="4" t="s">
         <v>44</v>
       </c>
@@ -3097,7 +3139,7 @@
         <v>N/A</v>
       </c>
       <c r="T16" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U16" s="4" t="s">
         <v>47</v>
@@ -3121,7 +3163,9 @@
       <c r="H17" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I17" s="4"/>
+      <c r="I17" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="J17" s="4" t="s">
         <v>44</v>
       </c>
@@ -3146,7 +3190,7 @@
         <v>N/A</v>
       </c>
       <c r="T17" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U17" s="4" t="s">
         <v>47</v>
@@ -3170,7 +3214,9 @@
       <c r="H18" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I18" s="4"/>
+      <c r="I18" s="4" t="s">
+        <v>128</v>
+      </c>
       <c r="J18" s="4" t="s">
         <v>44</v>
       </c>
@@ -3195,7 +3241,7 @@
         <v>Adequação ao escopo do projeto</v>
       </c>
       <c r="T18" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U18" s="4" t="s">
         <v>47</v>
@@ -3219,7 +3265,9 @@
       <c r="H19" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I19" s="4"/>
+      <c r="I19" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="J19" s="4" t="s">
         <v>44</v>
       </c>
@@ -3244,7 +3292,7 @@
         <v>N/A</v>
       </c>
       <c r="T19" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U19" s="4" t="s">
         <v>47</v>
@@ -3268,7 +3316,9 @@
       <c r="H20" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I20" s="4"/>
+      <c r="I20" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="J20" s="4" t="s">
         <v>44</v>
       </c>
@@ -3293,7 +3343,7 @@
         <v>N/A</v>
       </c>
       <c r="T20" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U20" s="4" t="s">
         <v>47</v>
@@ -3317,7 +3367,9 @@
       <c r="H21" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I21" s="4"/>
+      <c r="I21" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="J21" s="4" t="s">
         <v>44</v>
       </c>
@@ -3342,7 +3394,7 @@
         <v>N/A</v>
       </c>
       <c r="T21" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U21" s="4" t="s">
         <v>47</v>
@@ -3366,7 +3418,9 @@
       <c r="H22" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I22" s="4"/>
+      <c r="I22" s="4" t="s">
+        <v>128</v>
+      </c>
       <c r="J22" s="4" t="s">
         <v>44</v>
       </c>
@@ -3391,7 +3445,7 @@
         <v>N/A</v>
       </c>
       <c r="T22" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U22" s="4" t="s">
         <v>47</v>
@@ -3415,7 +3469,9 @@
       <c r="H23" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I23" s="4"/>
+      <c r="I23" s="4" t="s">
+        <v>128</v>
+      </c>
       <c r="J23" s="4" t="s">
         <v>44</v>
       </c>
@@ -3440,7 +3496,7 @@
         <v>N/A</v>
       </c>
       <c r="T23" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U23" s="4" t="s">
         <v>47</v>
@@ -3464,7 +3520,9 @@
       <c r="H24" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I24" s="4"/>
+      <c r="I24" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="J24" s="4" t="s">
         <v>44</v>
       </c>
@@ -3489,7 +3547,7 @@
         <v>N/A</v>
       </c>
       <c r="T24" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U24" s="4" t="s">
         <v>47</v>
@@ -3513,7 +3571,9 @@
       <c r="H25" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I25" s="4"/>
+      <c r="I25" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="J25" s="4" t="s">
         <v>44</v>
       </c>
@@ -3538,7 +3598,7 @@
         <v>N/A</v>
       </c>
       <c r="T25" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U25" s="4" t="s">
         <v>47</v>
@@ -3562,7 +3622,9 @@
       <c r="H26" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="I26" s="25"/>
+      <c r="I26" s="25" t="s">
+        <v>129</v>
+      </c>
       <c r="J26" s="25" t="s">
         <v>44</v>
       </c>
@@ -3587,7 +3649,7 @@
         <v>N/A</v>
       </c>
       <c r="T26" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U26" s="25" t="s">
         <v>47</v>
@@ -3611,7 +3673,9 @@
       <c r="H27" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I27" s="4"/>
+      <c r="I27" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="J27" s="4" t="s">
         <v>44</v>
       </c>
@@ -3636,7 +3700,7 @@
         <v>N/A</v>
       </c>
       <c r="T27" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U27" s="4" t="s">
         <v>47</v>
@@ -3660,7 +3724,9 @@
       <c r="H28" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I28" s="4"/>
+      <c r="I28" s="4" t="s">
+        <v>129</v>
+      </c>
       <c r="J28" s="4" t="s">
         <v>44</v>
       </c>
@@ -3685,7 +3751,7 @@
         <v>N/A</v>
       </c>
       <c r="T28" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U28" s="4" t="s">
         <v>47</v>
@@ -3709,7 +3775,9 @@
       <c r="H29" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I29" s="4"/>
+      <c r="I29" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="J29" s="4" t="s">
         <v>44</v>
       </c>
@@ -3734,7 +3802,7 @@
         <v>N/A</v>
       </c>
       <c r="T29" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U29" s="4" t="s">
         <v>47</v>
@@ -3758,7 +3826,9 @@
       <c r="H30" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="I30" s="4"/>
+      <c r="I30" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="J30" s="4" t="s">
         <v>44</v>
       </c>
@@ -3783,7 +3853,7 @@
         <v>N/A</v>
       </c>
       <c r="T30" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U30" s="4" t="s">
         <v>47</v>
@@ -3807,7 +3877,9 @@
       <c r="H31" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I31" s="4"/>
+      <c r="I31" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="J31" s="4" t="s">
         <v>44</v>
       </c>
@@ -3832,7 +3904,7 @@
         <v>N/A</v>
       </c>
       <c r="T31" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U31" s="4" t="s">
         <v>47</v>
@@ -3856,7 +3928,9 @@
       <c r="H32" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I32" s="4"/>
+      <c r="I32" s="4" t="s">
+        <v>128</v>
+      </c>
       <c r="J32" s="4" t="s">
         <v>44</v>
       </c>
@@ -3880,8 +3954,8 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T32" s="44" t="s">
-        <v>124</v>
+      <c r="T32" s="34" t="s">
+        <v>122</v>
       </c>
       <c r="U32" s="4" t="s">
         <v>47</v>
@@ -3893,7 +3967,7 @@
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4" t="s">
@@ -3905,7 +3979,9 @@
       <c r="H33" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I33" s="4"/>
+      <c r="I33" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="J33" s="4" t="s">
         <v>44</v>
       </c>
@@ -3930,7 +4006,7 @@
         <v>N/A</v>
       </c>
       <c r="T33" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U33" s="4" t="s">
         <v>47</v>
@@ -3942,7 +4018,7 @@
         <v>107</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4" t="s">
@@ -3954,7 +4030,9 @@
       <c r="H34" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I34" s="4"/>
+      <c r="I34" s="4" t="s">
+        <v>129</v>
+      </c>
       <c r="J34" s="4" t="s">
         <v>44</v>
       </c>
@@ -3979,7 +4057,7 @@
         <v>N/A</v>
       </c>
       <c r="T34" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U34" s="4" t="s">
         <v>47</v>
@@ -3991,7 +4069,7 @@
         <v>108</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4" t="s">
@@ -4003,7 +4081,9 @@
       <c r="H35" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I35" s="4"/>
+      <c r="I35" s="4" t="s">
+        <v>129</v>
+      </c>
       <c r="J35" s="4" t="s">
         <v>44</v>
       </c>
@@ -4028,7 +4108,7 @@
         <v>N/A</v>
       </c>
       <c r="T35" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U35" s="4" t="s">
         <v>47</v>
@@ -4040,7 +4120,7 @@
         <v>109</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>76</v>
+        <v>111</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4" t="s">
@@ -4052,7 +4132,9 @@
       <c r="H36" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I36" s="4"/>
+      <c r="I36" s="4" t="s">
+        <v>129</v>
+      </c>
       <c r="J36" s="4" t="s">
         <v>44</v>
       </c>
@@ -4064,7 +4146,7 @@
       <c r="N36" s="4"/>
       <c r="O36" s="4"/>
       <c r="P36" s="5">
-        <v>43716</v>
+        <v>43714</v>
       </c>
       <c r="Q36" s="5">
         <v>43716</v>
@@ -4074,10 +4156,10 @@
       </c>
       <c r="S36" s="4" t="str">
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
-        <v>N/A</v>
+        <v>Adequação ao escopo do projeto</v>
       </c>
       <c r="T36" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U36" s="4" t="s">
         <v>47</v>
@@ -4089,7 +4171,7 @@
         <v>110</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>111</v>
+        <v>85</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4" t="s">
@@ -4101,7 +4183,9 @@
       <c r="H37" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I37" s="4"/>
+      <c r="I37" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="J37" s="4" t="s">
         <v>44</v>
       </c>
@@ -4113,20 +4197,20 @@
       <c r="N37" s="4"/>
       <c r="O37" s="4"/>
       <c r="P37" s="5">
-        <v>43714</v>
+        <v>43718</v>
       </c>
       <c r="Q37" s="5">
-        <v>43716</v>
+        <v>43718</v>
       </c>
       <c r="R37" s="4" t="s">
         <v>7</v>
       </c>
       <c r="S37" s="4" t="str">
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
-        <v>Adequação ao escopo do projeto</v>
+        <v>N/A</v>
       </c>
       <c r="T37" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U37" s="4" t="s">
         <v>47</v>
@@ -4138,7 +4222,7 @@
         <v>115</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4" t="s">
@@ -4150,7 +4234,9 @@
       <c r="H38" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I38" s="4"/>
+      <c r="I38" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="J38" s="4" t="s">
         <v>44</v>
       </c>
@@ -4167,13 +4253,15 @@
       <c r="Q38" s="5">
         <v>43718</v>
       </c>
-      <c r="R38" s="4"/>
+      <c r="R38" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="S38" s="4" t="str">
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
       <c r="T38" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U38" s="4" t="s">
         <v>47</v>
@@ -4185,11 +4273,11 @@
         <v>116</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>5</v>
@@ -4197,7 +4285,9 @@
       <c r="H39" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I39" s="4"/>
+      <c r="I39" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="J39" s="4" t="s">
         <v>44</v>
       </c>
@@ -4214,25 +4304,27 @@
       <c r="Q39" s="5">
         <v>43718</v>
       </c>
-      <c r="R39" s="4"/>
+      <c r="R39" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="S39" s="4" t="str">
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
       <c r="T39" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U39" s="4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="40" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="3"/>
-      <c r="C40" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D40" s="10" t="s">
-        <v>86</v>
+      <c r="B40" s="3">
+        <v>11</v>
+      </c>
+      <c r="C40" s="3"/>
+      <c r="D40" s="11" t="s">
+        <v>77</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4" t="s">
@@ -4244,7 +4336,9 @@
       <c r="H40" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I40" s="4"/>
+      <c r="I40" s="30" t="s">
+        <v>126</v>
+      </c>
       <c r="J40" s="4" t="s">
         <v>44</v>
       </c>
@@ -4261,29 +4355,31 @@
       <c r="Q40" s="5">
         <v>43718</v>
       </c>
-      <c r="R40" s="4"/>
+      <c r="R40" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="S40" s="4" t="str">
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
       <c r="T40" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="U40" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="U40" s="31" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="3"/>
-      <c r="C41" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D41" s="10" t="s">
-        <v>87</v>
+    <row r="41" spans="2:21" s="20" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="3">
+        <v>12</v>
+      </c>
+      <c r="C41" s="3"/>
+      <c r="D41" s="11" t="s">
+        <v>80</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4" t="s">
-        <v>99</v>
+        <v>42</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>5</v>
@@ -4291,11 +4387,15 @@
       <c r="H41" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I41" s="4"/>
+      <c r="I41" s="30" t="s">
+        <v>126</v>
+      </c>
       <c r="J41" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K41" s="4"/>
+      <c r="K41" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="L41" s="4" t="s">
         <v>44</v>
       </c>
@@ -4308,29 +4408,31 @@
       <c r="Q41" s="5">
         <v>43718</v>
       </c>
-      <c r="R41" s="4"/>
+      <c r="R41" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="S41" s="4" t="str">
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
       <c r="T41" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="U41" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="42" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="3">
-        <v>11</v>
-      </c>
-      <c r="C42" s="3"/>
+        <v>123</v>
+      </c>
+      <c r="U41" s="31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="42" spans="2:21" s="20" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="3"/>
+      <c r="C42" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="D42" s="11" t="s">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4" t="s">
-        <v>99</v>
+        <v>42</v>
       </c>
       <c r="G42" s="4" t="s">
         <v>5</v>
@@ -4338,11 +4440,15 @@
       <c r="H42" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I42" s="30"/>
+      <c r="I42" s="30" t="s">
+        <v>126</v>
+      </c>
       <c r="J42" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K42" s="4"/>
+      <c r="K42" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="L42" s="4" t="s">
         <v>44</v>
       </c>
@@ -4355,29 +4461,31 @@
       <c r="Q42" s="5">
         <v>43718</v>
       </c>
-      <c r="R42" s="4"/>
+      <c r="R42" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="S42" s="4" t="str">
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
       <c r="T42" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U42" s="31" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="43" spans="2:21" s="20" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="43" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B43" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C43" s="3"/>
-      <c r="D43" s="11" t="s">
-        <v>80</v>
+      <c r="D43" s="10" t="s">
+        <v>88</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>5</v>
@@ -4385,13 +4493,13 @@
       <c r="H43" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I43" s="30"/>
+      <c r="I43" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="J43" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K43" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="K43" s="4"/>
       <c r="L43" s="4" t="s">
         <v>44</v>
       </c>
@@ -4405,30 +4513,30 @@
         <v>43718</v>
       </c>
       <c r="R43" s="4" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="S43" s="4" t="str">
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
       <c r="T43" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="U43" s="31" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="44" spans="2:21" s="20" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="3"/>
-      <c r="C44" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D44" s="11" t="s">
-        <v>112</v>
+        <v>123</v>
+      </c>
+      <c r="U43" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="2:21" s="20" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="3">
+        <v>14</v>
+      </c>
+      <c r="C44" s="3"/>
+      <c r="D44" s="10" t="s">
+        <v>84</v>
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="4" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>5</v>
@@ -4436,13 +4544,13 @@
       <c r="H44" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I44" s="30"/>
+      <c r="I44" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="J44" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K44" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="K44" s="4"/>
       <c r="L44" s="4" t="s">
         <v>44</v>
       </c>
@@ -4456,36 +4564,40 @@
         <v>43718</v>
       </c>
       <c r="R44" s="4" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="S44" s="4" t="str">
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
       <c r="T44" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="U44" s="31" t="s">
-        <v>79</v>
+        <v>123</v>
+      </c>
+      <c r="U44" s="4" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="45" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B45" s="3">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="10" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
+      <c r="F45" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="G45" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H45" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I45" s="4"/>
+      <c r="I45" s="4" t="s">
+        <v>129</v>
+      </c>
       <c r="J45" s="4" t="s">
         <v>44</v>
       </c>
@@ -4502,35 +4614,39 @@
       <c r="Q45" s="5">
         <v>43718</v>
       </c>
-      <c r="R45" s="4"/>
+      <c r="R45" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="S45" s="4" t="str">
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
       <c r="T45" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U45" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="2:21" s="20" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="3">
-        <v>14</v>
-      </c>
+    <row r="46" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="3"/>
       <c r="C46" s="3"/>
-      <c r="D46" s="10" t="s">
-        <v>84</v>
+      <c r="D46" s="46" t="s">
+        <v>74</v>
       </c>
       <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
+      <c r="F46" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="G46" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H46" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I46" s="4"/>
+      <c r="I46" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="J46" s="4" t="s">
         <v>44</v>
       </c>
@@ -4542,30 +4658,30 @@
       <c r="N46" s="4"/>
       <c r="O46" s="4"/>
       <c r="P46" s="5">
-        <v>43718</v>
+        <v>43716</v>
       </c>
       <c r="Q46" s="5">
-        <v>43718</v>
-      </c>
-      <c r="R46" s="4"/>
+        <v>43716</v>
+      </c>
+      <c r="R46" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="S46" s="4" t="str">
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
       <c r="T46" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U46" s="4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="47" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="3">
-        <v>15</v>
-      </c>
+      <c r="B47" s="3"/>
       <c r="C47" s="3"/>
-      <c r="D47" s="10" t="s">
-        <v>83</v>
+      <c r="D47" s="46" t="s">
+        <v>82</v>
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="4" t="s">
@@ -4577,7 +4693,9 @@
       <c r="H47" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I47" s="4"/>
+      <c r="I47" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="J47" s="4" t="s">
         <v>44</v>
       </c>
@@ -4594,13 +4712,15 @@
       <c r="Q47" s="5">
         <v>43718</v>
       </c>
-      <c r="R47" s="4"/>
+      <c r="R47" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="S47" s="4" t="str">
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
       <c r="T47" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U47" s="4" t="s">
         <v>47</v>
@@ -4653,12 +4773,12 @@
     <row r="50" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
-      <c r="D50" s="11"/>
+      <c r="D50" s="10"/>
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
-      <c r="I50" s="30"/>
+      <c r="I50" s="4"/>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
       <c r="L50" s="4"/>
@@ -4670,7 +4790,7 @@
       <c r="R50" s="4"/>
       <c r="S50" s="4"/>
       <c r="T50" s="10"/>
-      <c r="U50" s="31"/>
+      <c r="U50" s="4"/>
     </row>
     <row r="51" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B51" s="3"/>
@@ -4697,12 +4817,12 @@
     <row r="52" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
-      <c r="D52" s="10"/>
+      <c r="D52" s="11"/>
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
-      <c r="I52" s="4"/>
+      <c r="I52" s="30"/>
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
@@ -4714,7 +4834,7 @@
       <c r="R52" s="4"/>
       <c r="S52" s="4"/>
       <c r="T52" s="10"/>
-      <c r="U52" s="4"/>
+      <c r="U52" s="31"/>
     </row>
     <row r="53" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B53" s="3"/>
@@ -4741,12 +4861,12 @@
     <row r="54" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
-      <c r="D54" s="11"/>
+      <c r="D54" s="10"/>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
-      <c r="I54" s="30"/>
+      <c r="I54" s="4"/>
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
@@ -4758,17 +4878,17 @@
       <c r="R54" s="4"/>
       <c r="S54" s="4"/>
       <c r="T54" s="10"/>
-      <c r="U54" s="31"/>
+      <c r="U54" s="4"/>
     </row>
     <row r="55" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
-      <c r="D55" s="11"/>
+      <c r="D55" s="10"/>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
-      <c r="I55" s="30"/>
+      <c r="I55" s="4"/>
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
       <c r="L55" s="4"/>
@@ -4780,7 +4900,7 @@
       <c r="R55" s="4"/>
       <c r="S55" s="4"/>
       <c r="T55" s="10"/>
-      <c r="U55" s="31"/>
+      <c r="U55" s="4"/>
     </row>
     <row r="56" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B56" s="3"/>
@@ -5090,54 +5210,12 @@
       <c r="T69" s="10"/>
       <c r="U69" s="4"/>
     </row>
-    <row r="70" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="3"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="10"/>
-      <c r="E70" s="4"/>
-      <c r="F70" s="4"/>
-      <c r="G70" s="4"/>
-      <c r="H70" s="4"/>
-      <c r="I70" s="4"/>
-      <c r="J70" s="4"/>
-      <c r="K70" s="4"/>
-      <c r="L70" s="4"/>
-      <c r="M70" s="4"/>
-      <c r="N70" s="4"/>
-      <c r="O70" s="4"/>
-      <c r="P70" s="5"/>
-      <c r="Q70" s="4"/>
-      <c r="R70" s="4"/>
-      <c r="S70" s="4"/>
-      <c r="T70" s="10"/>
-      <c r="U70" s="4"/>
-    </row>
-    <row r="71" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="3"/>
-      <c r="C71" s="3"/>
-      <c r="D71" s="10"/>
-      <c r="E71" s="4"/>
-      <c r="F71" s="4"/>
-      <c r="G71" s="4"/>
-      <c r="H71" s="4"/>
-      <c r="I71" s="4"/>
-      <c r="J71" s="4"/>
-      <c r="K71" s="4"/>
-      <c r="L71" s="4"/>
-      <c r="M71" s="4"/>
-      <c r="N71" s="4"/>
-      <c r="O71" s="4"/>
-      <c r="P71" s="5"/>
-      <c r="Q71" s="4"/>
-      <c r="R71" s="4"/>
-      <c r="S71" s="4"/>
-      <c r="T71" s="10"/>
-      <c r="U71" s="4"/>
-    </row>
-    <row r="72" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="N72" s="21"/>
-    </row>
-    <row r="73" spans="2:21" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="70" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="N70" s="21"/>
+    </row>
+    <row r="71" spans="2:21" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="72" spans="2:21" x14ac:dyDescent="0.2"/>
+    <row r="73" spans="2:21" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="H2:J3"/>
@@ -5152,26 +5230,26 @@
     <mergeCell ref="M2:M3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations disablePrompts="1" count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U56:U71 U5:U47 U52">
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U54:U69 U50 U5:U47">
       <formula1>"Proposto,Aprovado,Projetado,Implementado,Verificado, Entregue, Eliminado, Rejeitado"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I56:I71 I5:I47 I52">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I54:I69 I50 I5:I47">
       <formula1>"Máxima,Alta,Média,Baixa,Mínima"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H56:H71 H5:H47 H52">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H54:H69 H50 H5:H47">
       <formula1>"Funcional,Não Funcional"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J56:J71 L38:L41 L45:L47 J5:J47 J52">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J54:J69 L43:L45 J50 L47 J5:J47 L37:L39">
       <formula1>"Gerson Santos,Célia Taniwaki,José Yoshihiro,Alex Barreira"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R56:R71 K56:K71 R5:R47 R52 K5:K47 K52">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R54:R69 K54:K69 R50 K50 R5:R47 K5:K47">
       <formula1>"Fernando Abreu,João Vinícius,Kessi Santana,Thalita Igwe,Vitoria Ferreira"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L42:L44 L56:L71 L5:L37 L52">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L40:L42 L54:L69 L50 L46 L5:L36">
       <formula1>"Gerson Santos,Fernando Abreu,João Vinícius,Kessi Santana,Thalita Igwe,Vitoria Ferreira,Célia Taniwaki,Alex Barreira,José Yoshihiro"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F56:F71 F5:F47 F52">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F54:F69 F50 F5:F47">
       <formula1>"Essencial,Importante,Desejável"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Alteração requisito e inclusão do print do canvas.
</commit_message>
<xml_diff>
--- a/documentacao/requisitos.xlsx
+++ b/documentacao/requisitos.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Data-Source\documentacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aluno\Desktop\VITORIA\Data-Source\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156E6209-51DC-45EF-8181-6ED12D51807C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Histórico de Alterações" sheetId="4" r:id="rId1"/>
     <sheet name="Documentação e Matriz" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="146">
   <si>
     <t>Histórico de alterações do documento</t>
   </si>
@@ -267,9 +268,6 @@
     <t>Fernando Abreu</t>
   </si>
   <si>
-    <t>Exemplo executado em até 5 seg</t>
-  </si>
-  <si>
     <t>Proposto</t>
   </si>
   <si>
@@ -297,9 +295,6 @@
     <t>O cliente deverá ter o JRE instalado em seu computador</t>
   </si>
   <si>
-    <t>O sofware deverá ter um dashboard com as informações do hardware do device</t>
-  </si>
-  <si>
     <t>O software deverá coletar as informações de hardware do device</t>
   </si>
   <si>
@@ -339,18 +334,12 @@
     <t>O software deverá ter níveis de acesso</t>
   </si>
   <si>
-    <t>O software deverá ter autenticação de usuários para a entrada no sistema</t>
-  </si>
-  <si>
     <t>O software deverá ter uma tela de login</t>
   </si>
   <si>
     <t>O software deverá emitir um alerta visual, caso os dados de login sejam inválidos</t>
   </si>
   <si>
-    <t>O software deverá fazer integração com o PowerBI</t>
-  </si>
-  <si>
     <t>O software deverá permitir ao administrador a exibição de usuários em cada servidor</t>
   </si>
   <si>
@@ -369,9 +358,6 @@
     <t>Projetado</t>
   </si>
   <si>
-    <t>O software deverá uma tela com os dados do usuário e do seu device</t>
-  </si>
-  <si>
     <t>O software deverá permitir que o usuário encerre a sessão que está logado</t>
   </si>
   <si>
@@ -501,9 +487,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>USER PREMIUN E FREE</t>
-  </si>
-  <si>
     <t>Baixa</t>
   </si>
   <si>
@@ -517,13 +500,79 @@
   </si>
   <si>
     <t>Média</t>
+  </si>
+  <si>
+    <t>O software deverá ter autenticação de usuários</t>
+  </si>
+  <si>
+    <t>O sofware deverá ter um dashboard com as informações do hardware dos devices (servidores e máquina dos jogadores)</t>
+  </si>
+  <si>
+    <t>Deverá ter gráficos e tabelas que devem carregar em até 10 segundos</t>
+  </si>
+  <si>
+    <t>Não permitirá acesso ao sistema, caso o login não seja validado juntamento ao banco de dados</t>
+  </si>
+  <si>
+    <t>O software deverá uma tela detalhada com os dados do usuário e do seu device</t>
+  </si>
+  <si>
+    <t>Thalita Igwe</t>
+  </si>
+  <si>
+    <t>João Vinícius</t>
+  </si>
+  <si>
+    <t>Kessi Santana</t>
+  </si>
+  <si>
+    <t>Aprovado</t>
+  </si>
+  <si>
+    <t>6.1</t>
+  </si>
+  <si>
+    <t>1, 3.1, 3,2</t>
+  </si>
+  <si>
+    <t>O software permitirá ao usuário ter conta premium ou conta free</t>
+  </si>
+  <si>
+    <t>1, 6, 10.3</t>
+  </si>
+  <si>
+    <t>1, 6, 10.3, 8.3</t>
+  </si>
+  <si>
+    <t>9.1</t>
+  </si>
+  <si>
+    <t>O cliente (NOC) deverá ter licença do PowerBI Pro</t>
+  </si>
+  <si>
+    <t>O software deverá fazer integração com o PowerBI Pro para os relatórios</t>
+  </si>
+  <si>
+    <t>1, 6</t>
+  </si>
+  <si>
+    <t>1, 6, 10</t>
+  </si>
+  <si>
+    <t>1, 3, 3.2</t>
+  </si>
+  <si>
+    <t>1, 3, 6</t>
+  </si>
+  <si>
+    <t>Aumentar o desempenho dos devices para manter a maior quantidade possível de jogadores nas salas, evitando assim perdas financeiras a médio-longo prazo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="14" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -595,12 +644,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -782,7 +825,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -843,9 +886,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -919,8 +959,8 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1787,13 +1827,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B4:E32" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26">
-  <autoFilter ref="B4:E32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="B4:E32" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26">
+  <autoFilter ref="B4:E32" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Versão" dataDxfId="25"/>
-    <tableColumn id="2" name="Alteração efetuada" dataDxfId="24"/>
-    <tableColumn id="3" name="Responsável " dataDxfId="23"/>
-    <tableColumn id="4" name="Data " dataDxfId="22">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Versão" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Alteração efetuada" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Responsável " dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Data " dataDxfId="22">
       <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1802,27 +1842,27 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="requisitos" displayName="requisitos" ref="D4:U69" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18">
-  <autoFilter ref="D4:U69"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="requisitos" displayName="requisitos" ref="D4:U69" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18">
+  <autoFilter ref="D4:U69" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="18">
-    <tableColumn id="1" name="Descrição do Requisito" dataDxfId="17"/>
-    <tableColumn id="2" name="Objetivo / Estratégia de Negócio" dataDxfId="16"/>
-    <tableColumn id="3" name="Prioridade" dataDxfId="15"/>
-    <tableColumn id="4" name="Versão do Requisito" dataDxfId="14"/>
-    <tableColumn id="7" name="Tipo Requisito " dataDxfId="13"/>
-    <tableColumn id="8" name="Complexidade" dataDxfId="12"/>
-    <tableColumn id="9" name="Solicitante" dataDxfId="11"/>
-    <tableColumn id="10" name="Responsável" dataDxfId="10"/>
-    <tableColumn id="11" name="Validador" dataDxfId="9"/>
-    <tableColumn id="12" name="Critérios de Aceitação" dataDxfId="8"/>
-    <tableColumn id="13" name="Dependência Internas entre Requisitos  (Rastreabilidade)" dataDxfId="7"/>
-    <tableColumn id="14" name="Dependências Externas entre Requisitos (Rastreabilidade)" dataDxfId="6"/>
-    <tableColumn id="15" name="Data da Criação" dataDxfId="5"/>
-    <tableColumn id="16" name="Data Última Alteração" dataDxfId="4"/>
-    <tableColumn id="17" name="Responsável pela última alteração" dataDxfId="3"/>
-    <tableColumn id="18" name="Motivo Última Alteração" dataDxfId="2"/>
-    <tableColumn id="19" name="Documentação de Apoio" dataDxfId="1"/>
-    <tableColumn id="20" name="Situação do Requisito" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Descrição do Requisito" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Objetivo / Estratégia de Negócio" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Prioridade" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Versão do Requisito" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Tipo Requisito " dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Complexidade" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Solicitante" dataDxfId="11"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Responsável" dataDxfId="10"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Validador" dataDxfId="9"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Critérios de Aceitação" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Dependência Internas entre Requisitos  (Rastreabilidade)" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Dependências Externas entre Requisitos (Rastreabilidade)" dataDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="Data da Criação" dataDxfId="5"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="Data Última Alteração" dataDxfId="4"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="Responsável pela última alteração" dataDxfId="3"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="Motivo Última Alteração" dataDxfId="2"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="Documentação de Apoio" dataDxfId="1"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="Situação do Requisito" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1904,6 +1944,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1939,6 +1996,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2114,7 +2188,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2135,25 +2209,25 @@
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2"/>
     <row r="4" spans="2:5" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="21" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2229,7 +2303,7 @@
     </row>
     <row r="10" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="7" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>14</v>
@@ -2309,28 +2383,28 @@
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2"/>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B34" s="37" t="s">
+      <c r="B34" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="37"/>
-      <c r="D34" s="37"/>
-      <c r="E34" s="37"/>
+      <c r="C34" s="36"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="36"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B35" s="37" t="s">
+      <c r="B35" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C35" s="37"/>
-      <c r="D35" s="37"/>
-      <c r="E35" s="37"/>
+      <c r="C35" s="36"/>
+      <c r="D35" s="36"/>
+      <c r="E35" s="36"/>
     </row>
     <row r="36" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="37" t="s">
+      <c r="B36" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="C36" s="37"/>
-      <c r="D36" s="37"/>
-      <c r="E36" s="37"/>
+      <c r="C36" s="36"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="36"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2"/>
     <row r="38" spans="2:5" hidden="1" x14ac:dyDescent="0.2"/>
@@ -2345,7 +2419,7 @@
     <mergeCell ref="B36:E36"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D32" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Fernando Abreu,João Vinícius,Kessi Santana,Thalita Igwe,Vitoria Ferreira"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2358,11 +2432,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V73"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="P5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
       <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
@@ -2371,10 +2445,10 @@
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="3.85546875" style="29" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.85546875" style="28" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="28" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="49.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="21.28515625" style="1" customWidth="1"/>
     <col min="8" max="8" width="18.85546875" style="1" customWidth="1"/>
@@ -2389,15 +2463,15 @@
     <col min="17" max="17" width="14.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="17" style="1" customWidth="1"/>
-    <col min="20" max="20" width="16.140625" style="23" customWidth="1"/>
+    <col min="20" max="20" width="16.140625" style="22" customWidth="1"/>
     <col min="21" max="21" width="25.42578125" style="1" customWidth="1"/>
     <col min="22" max="22" width="3.7109375" style="1" customWidth="1"/>
     <col min="23" max="16384" width="9.140625" style="1" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:21" s="13" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
       <c r="J1" s="14"/>
@@ -2409,54 +2483,52 @@
       <c r="P1" s="14"/>
       <c r="Q1" s="17"/>
       <c r="R1" s="9"/>
-      <c r="T1" s="32"/>
+      <c r="T1" s="31"/>
       <c r="U1" s="17"/>
     </row>
     <row r="2" spans="2:21" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="35" t="s">
-        <v>124</v>
-      </c>
-      <c r="E2" s="44"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38" t="s">
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="40" t="s">
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="42">
+      <c r="P2" s="41">
         <f ca="1">TODAY()</f>
-        <v>43719</v>
+        <v>43720</v>
       </c>
       <c r="R2" s="18"/>
-      <c r="T2" s="32"/>
+      <c r="T2" s="31"/>
       <c r="U2" s="17"/>
     </row>
     <row r="3" spans="2:21" s="13" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="41"/>
-      <c r="P3" s="43"/>
-      <c r="T3" s="32"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="42"/>
+      <c r="T3" s="31"/>
       <c r="U3" s="19"/>
     </row>
     <row r="4" spans="2:21" s="2" customFormat="1" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2540,7 +2612,7 @@
         <v>43</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>44</v>
@@ -2552,7 +2624,7 @@
         <v>44</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>46</v>
+        <v>118</v>
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
@@ -2569,11 +2641,11 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T5" s="33" t="s">
-        <v>118</v>
+      <c r="T5" s="32" t="s">
+        <v>113</v>
       </c>
       <c r="U5" s="4" t="s">
-        <v>47</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2582,20 +2654,20 @@
         <v>9</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>44</v>
@@ -2606,7 +2678,9 @@
       <c r="L6" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M6" s="4"/>
+      <c r="M6" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
       <c r="P6" s="5">
@@ -2623,10 +2697,10 @@
         <v>N/A</v>
       </c>
       <c r="T6" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="U6" s="4" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2635,31 +2709,39 @@
         <v>11</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K7" s="4"/>
+      <c r="K7" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="L7" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
+      <c r="M7" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="N7" s="4">
+        <v>1</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="P7" s="5">
         <v>43707</v>
       </c>
@@ -2674,10 +2756,10 @@
         <v>Adequação ao escopo do projeto</v>
       </c>
       <c r="T7" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="U7" s="4" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2686,20 +2768,20 @@
         <v>13</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>44</v>
@@ -2710,7 +2792,9 @@
       <c r="L8" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M8" s="4"/>
+      <c r="M8" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
       <c r="P8" s="5">
@@ -2727,10 +2811,10 @@
         <v>N/A</v>
       </c>
       <c r="T8" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="U8" s="4" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2739,7 +2823,7 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4" t="s">
@@ -2749,10 +2833,10 @@
         <v>5</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>44</v>
@@ -2763,7 +2847,9 @@
       <c r="L9" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M9" s="4"/>
+      <c r="M9" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
       <c r="P9" s="5">
@@ -2780,19 +2866,19 @@
         <v>N/A</v>
       </c>
       <c r="T9" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="U9" s="4" t="s">
-        <v>47</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4" t="s">
@@ -2802,19 +2888,23 @@
         <v>5</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K10" s="4"/>
+      <c r="K10" s="4" t="s">
+        <v>129</v>
+      </c>
       <c r="L10" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M10" s="4"/>
+      <c r="M10" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
       <c r="P10" s="5">
@@ -2830,20 +2920,20 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T10" s="33" t="s">
-        <v>120</v>
+      <c r="T10" s="32" t="s">
+        <v>115</v>
       </c>
       <c r="U10" s="4" t="s">
-        <v>47</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4" t="s">
@@ -2853,19 +2943,23 @@
         <v>5</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K11" s="4"/>
+      <c r="K11" s="4" t="s">
+        <v>129</v>
+      </c>
       <c r="L11" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M11" s="4"/>
+      <c r="M11" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
       <c r="P11" s="5">
@@ -2881,20 +2975,20 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T11" s="34" t="s">
-        <v>121</v>
+      <c r="T11" s="33" t="s">
+        <v>116</v>
       </c>
       <c r="U11" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" s="20" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <v>3</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="10" t="s">
-        <v>56</v>
+        <v>125</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4" t="s">
@@ -2907,17 +3001,23 @@
         <v>43</v>
       </c>
       <c r="I12" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="M12" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="J12" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
+      <c r="N12" s="4" t="s">
+        <v>134</v>
+      </c>
       <c r="O12" s="4"/>
       <c r="P12" s="5">
         <v>43713</v>
@@ -2933,19 +3033,19 @@
         <v>N/A</v>
       </c>
       <c r="T12" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="U12" s="4" t="s">
-        <v>47</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
@@ -2958,7 +3058,7 @@
         <v>43</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>44</v>
@@ -2969,8 +3069,12 @@
       <c r="L13" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
+      <c r="M13" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="O13" s="4"/>
       <c r="P13" s="5">
         <v>43718</v>
@@ -2986,19 +3090,19 @@
         <v>N/A</v>
       </c>
       <c r="T13" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="U13" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4" t="s">
@@ -3011,16 +3115,20 @@
         <v>43</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K14" s="4"/>
+      <c r="K14" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="L14" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M14" s="4"/>
+      <c r="M14" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
       <c r="P14" s="5">
@@ -3036,20 +3144,20 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T14" s="33" t="s">
-        <v>78</v>
+      <c r="T14" s="32" t="s">
+        <v>74</v>
       </c>
       <c r="U14" s="4" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4" t="s">
@@ -3062,17 +3170,23 @@
         <v>43</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K15" s="4"/>
+      <c r="K15" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="L15" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
+      <c r="M15" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="O15" s="4"/>
       <c r="P15" s="5">
         <v>43711</v>
@@ -3088,19 +3202,19 @@
         <v>N/A</v>
       </c>
       <c r="T15" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="U15" s="4" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4" t="s">
@@ -3113,17 +3227,23 @@
         <v>43</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K16" s="4"/>
+      <c r="K16" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="L16" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
+      <c r="M16" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="O16" s="4"/>
       <c r="P16" s="5">
         <v>43711</v>
@@ -3139,19 +3259,19 @@
         <v>N/A</v>
       </c>
       <c r="T16" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="U16" s="4" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4" t="s">
@@ -3164,17 +3284,23 @@
         <v>43</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J17" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K17" s="4"/>
+      <c r="K17" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="L17" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
+      <c r="M17" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="O17" s="4"/>
       <c r="P17" s="5">
         <v>43711</v>
@@ -3190,23 +3316,23 @@
         <v>N/A</v>
       </c>
       <c r="T17" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="U17" s="4" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>5</v>
@@ -3215,16 +3341,20 @@
         <v>43</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="J18" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K18" s="4"/>
+      <c r="K18" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="L18" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M18" s="4"/>
+      <c r="M18" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
       <c r="P18" s="5">
@@ -3241,23 +3371,23 @@
         <v>Adequação ao escopo do projeto</v>
       </c>
       <c r="T18" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="U18" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
       <c r="C19" s="3" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>5</v>
@@ -3266,16 +3396,20 @@
         <v>43</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J19" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K19" s="4"/>
+      <c r="K19" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="L19" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M19" s="4"/>
+      <c r="M19" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
       <c r="P19" s="5">
@@ -3292,19 +3426,19 @@
         <v>N/A</v>
       </c>
       <c r="T19" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="U19" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4" t="s">
@@ -3317,17 +3451,23 @@
         <v>43</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K20" s="4"/>
+      <c r="K20" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="L20" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
+      <c r="M20" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="O20" s="4"/>
       <c r="P20" s="5">
         <v>43716</v>
@@ -3343,23 +3483,25 @@
         <v>N/A</v>
       </c>
       <c r="T20" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="U20" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="2:21" s="20" customFormat="1" ht="77.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <v>4</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="E21" s="4"/>
+        <v>62</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>145</v>
+      </c>
       <c r="F21" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>5</v>
@@ -3368,16 +3510,20 @@
         <v>43</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J21" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K21" s="4"/>
+      <c r="K21" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="L21" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M21" s="4"/>
+      <c r="M21" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
       <c r="P21" s="5">
@@ -3394,10 +3540,10 @@
         <v>N/A</v>
       </c>
       <c r="T21" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="U21" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3406,11 +3552,11 @@
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>5</v>
@@ -3419,17 +3565,23 @@
         <v>43</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="J22" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K22" s="4"/>
+      <c r="K22" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="L22" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
+      <c r="M22" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>96</v>
+      </c>
       <c r="O22" s="4"/>
       <c r="P22" s="5">
         <v>43716</v>
@@ -3445,23 +3597,23 @@
         <v>N/A</v>
       </c>
       <c r="T22" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="U22" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="2:21" s="20" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
       <c r="C23" s="3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>5</v>
@@ -3470,16 +3622,20 @@
         <v>43</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="J23" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K23" s="4"/>
+      <c r="K23" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="L23" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M23" s="4"/>
+      <c r="M23" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
       <c r="P23" s="5">
@@ -3496,23 +3652,23 @@
         <v>N/A</v>
       </c>
       <c r="T23" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="U23" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="2:21" s="20" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>5</v>
@@ -3521,16 +3677,20 @@
         <v>43</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J24" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K24" s="4"/>
+      <c r="K24" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="L24" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M24" s="4"/>
+      <c r="M24" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
       <c r="P24" s="5">
@@ -3547,23 +3707,23 @@
         <v>N/A</v>
       </c>
       <c r="T24" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="U24" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="2:21" s="20" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
       <c r="C25" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>5</v>
@@ -3572,16 +3732,20 @@
         <v>43</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J25" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K25" s="4"/>
+      <c r="K25" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="L25" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M25" s="4"/>
+      <c r="M25" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
       <c r="P25" s="5">
@@ -3598,125 +3762,134 @@
         <v>N/A</v>
       </c>
       <c r="T25" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="U25" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" spans="2:21" s="27" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="2:21" s="26" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <v>6</v>
       </c>
       <c r="C26" s="3"/>
-      <c r="D26" s="24" t="s">
-        <v>104</v>
-      </c>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25" t="s">
+      <c r="D26" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="G26" s="25" t="s">
+      <c r="G26" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="H26" s="25" t="s">
+      <c r="H26" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="I26" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="J26" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="K26" s="25"/>
-      <c r="L26" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="M26" s="25"/>
-      <c r="N26" s="25"/>
-      <c r="O26" s="25"/>
-      <c r="P26" s="26">
+      <c r="I26" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="J26" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="K26" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="L26" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="M26" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="N26" s="24"/>
+      <c r="O26" s="24"/>
+      <c r="P26" s="25">
         <v>43716</v>
       </c>
-      <c r="Q26" s="26">
+      <c r="Q26" s="25">
         <v>43716</v>
       </c>
-      <c r="R26" s="25" t="s">
+      <c r="R26" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="S26" s="25" t="str">
+      <c r="S26" s="24" t="str">
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
       <c r="T26" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="U26" s="24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="3"/>
+      <c r="C27" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="F27" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="G27" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="H27" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="I27" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="U26" s="25" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="3">
+      <c r="J27" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="K27" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="L27" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="M27" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="N27" s="24">
+        <v>6</v>
+      </c>
+      <c r="O27" s="24"/>
+      <c r="P27" s="25">
+        <v>43720</v>
+      </c>
+      <c r="Q27" s="25">
+        <v>43720</v>
+      </c>
+      <c r="R27" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="I27" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
-      <c r="P27" s="5">
-        <v>43716</v>
-      </c>
-      <c r="Q27" s="5">
-        <v>43716</v>
-      </c>
-      <c r="R27" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="S27" s="4" t="str">
+      <c r="S27" s="24" t="str">
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
       <c r="T27" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="U27" s="4" t="s">
-        <v>47</v>
+        <v>118</v>
+      </c>
+      <c r="U27" s="24" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C28" s="3"/>
-      <c r="D28" s="20" t="s">
-        <v>70</v>
+      <c r="D28" s="10" t="s">
+        <v>67</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>5</v>
@@ -3725,16 +3898,20 @@
         <v>43</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="J28" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K28" s="4"/>
+      <c r="K28" s="4" t="s">
+        <v>131</v>
+      </c>
       <c r="L28" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M28" s="4"/>
+      <c r="M28" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
       <c r="P28" s="5">
@@ -3751,19 +3928,19 @@
         <v>N/A</v>
       </c>
       <c r="T28" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="U28" s="4" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="3"/>
-      <c r="C29" s="3" t="s">
-        <v>105</v>
-      </c>
+      <c r="B29" s="3">
+        <v>8</v>
+      </c>
+      <c r="C29" s="3"/>
       <c r="D29" s="20" t="s">
-        <v>71</v>
+        <v>124</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4" t="s">
@@ -3776,17 +3953,23 @@
         <v>43</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J29" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K29" s="4"/>
+      <c r="K29" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="L29" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
+      <c r="M29" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="N29" s="4" t="s">
+        <v>137</v>
+      </c>
       <c r="O29" s="4"/>
       <c r="P29" s="5">
         <v>43716</v>
@@ -3802,42 +3985,48 @@
         <v>N/A</v>
       </c>
       <c r="T29" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="U29" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="30" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="2:21" s="20" customFormat="1" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" s="3"/>
       <c r="C30" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>72</v>
+        <v>100</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>68</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="J30" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K30" s="4"/>
+      <c r="K30" s="4" t="s">
+        <v>129</v>
+      </c>
       <c r="L30" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M30" s="4"/>
-      <c r="N30" s="4"/>
+      <c r="M30" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="N30" s="4" t="s">
+        <v>136</v>
+      </c>
       <c r="O30" s="4"/>
       <c r="P30" s="5">
         <v>43716</v>
@@ -3853,42 +4042,48 @@
         <v>N/A</v>
       </c>
       <c r="T30" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="U30" s="4" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B31" s="3"/>
       <c r="C31" s="3" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="J31" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K31" s="4"/>
+      <c r="K31" s="4" t="s">
+        <v>129</v>
+      </c>
       <c r="L31" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
+      <c r="M31" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="N31" s="4" t="s">
+        <v>136</v>
+      </c>
       <c r="O31" s="4"/>
       <c r="P31" s="5">
         <v>43716</v>
@@ -3904,23 +4099,23 @@
         <v>N/A</v>
       </c>
       <c r="T31" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="U31" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="3">
-        <v>9</v>
-      </c>
-      <c r="C32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3" t="s">
+        <v>109</v>
+      </c>
       <c r="D32" s="10" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4" t="s">
-        <v>99</v>
+        <v>42</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>5</v>
@@ -3929,17 +4124,23 @@
         <v>43</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="J32" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K32" s="4"/>
+      <c r="K32" s="4" t="s">
+        <v>129</v>
+      </c>
       <c r="L32" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
+      <c r="M32" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="N32" s="4" t="s">
+        <v>136</v>
+      </c>
       <c r="O32" s="4"/>
       <c r="P32" s="5">
         <v>43716</v>
@@ -3954,24 +4155,24 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T32" s="34" t="s">
-        <v>122</v>
+      <c r="T32" s="4" t="s">
+        <v>118</v>
       </c>
       <c r="U32" s="4" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B33" s="3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="10" t="s">
-        <v>119</v>
+        <v>140</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4" t="s">
-        <v>49</v>
+        <v>94</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>5</v>
@@ -3980,17 +4181,23 @@
         <v>43</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="J33" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K33" s="4"/>
+      <c r="K33" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="L33" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
+      <c r="M33" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="N33" s="4">
+        <v>2</v>
+      </c>
       <c r="O33" s="4"/>
       <c r="P33" s="5">
         <v>43716</v>
@@ -4005,24 +4212,24 @@
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="T33" s="4" t="s">
-        <v>123</v>
+      <c r="T33" s="33" t="s">
+        <v>117</v>
       </c>
       <c r="U33" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B34" s="3"/>
       <c r="C34" s="3" t="s">
-        <v>107</v>
+        <v>138</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>75</v>
+        <v>139</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>5</v>
@@ -4031,18 +4238,24 @@
         <v>43</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="J34" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K34" s="4"/>
+      <c r="K34" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="L34" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M34" s="4"/>
+      <c r="M34" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="N34" s="4"/>
-      <c r="O34" s="4"/>
+      <c r="O34" s="4">
+        <v>9</v>
+      </c>
       <c r="P34" s="5">
         <v>43716</v>
       </c>
@@ -4057,23 +4270,23 @@
         <v>N/A</v>
       </c>
       <c r="T34" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="U34" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="3"/>
-      <c r="C35" s="3" t="s">
-        <v>108</v>
-      </c>
+      <c r="B35" s="3">
+        <v>10</v>
+      </c>
+      <c r="C35" s="3"/>
       <c r="D35" s="10" t="s">
-        <v>76</v>
+        <v>114</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>5</v>
@@ -4082,17 +4295,23 @@
         <v>43</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="J35" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K35" s="4"/>
+      <c r="K35" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="L35" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M35" s="4"/>
-      <c r="N35" s="4"/>
+      <c r="M35" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="N35" s="4" t="s">
+        <v>141</v>
+      </c>
       <c r="O35" s="4"/>
       <c r="P35" s="5">
         <v>43716</v>
@@ -4108,23 +4327,23 @@
         <v>N/A</v>
       </c>
       <c r="T35" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="U35" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B36" s="3"/>
       <c r="C36" s="3" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>111</v>
+        <v>71</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>5</v>
@@ -4133,20 +4352,26 @@
         <v>43</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="J36" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K36" s="4"/>
+      <c r="K36" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="L36" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M36" s="4"/>
-      <c r="N36" s="4"/>
+      <c r="M36" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="N36" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="O36" s="4"/>
       <c r="P36" s="5">
-        <v>43714</v>
+        <v>43716</v>
       </c>
       <c r="Q36" s="5">
         <v>43716</v>
@@ -4156,26 +4381,26 @@
       </c>
       <c r="S36" s="4" t="str">
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
-        <v>Adequação ao escopo do projeto</v>
+        <v>N/A</v>
       </c>
       <c r="T36" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="U36" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B37" s="3"/>
       <c r="C37" s="3" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>5</v>
@@ -4184,23 +4409,29 @@
         <v>43</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="J37" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K37" s="4"/>
+      <c r="K37" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="L37" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M37" s="4"/>
-      <c r="N37" s="4"/>
+      <c r="M37" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="N37" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="O37" s="4"/>
       <c r="P37" s="5">
-        <v>43718</v>
+        <v>43716</v>
       </c>
       <c r="Q37" s="5">
-        <v>43718</v>
+        <v>43716</v>
       </c>
       <c r="R37" s="4" t="s">
         <v>7</v>
@@ -4210,23 +4441,23 @@
         <v>N/A</v>
       </c>
       <c r="T37" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="U37" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B38" s="3"/>
       <c r="C38" s="3" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4" t="s">
-        <v>99</v>
+        <v>48</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>5</v>
@@ -4235,49 +4466,55 @@
         <v>43</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="J38" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K38" s="4"/>
+      <c r="K38" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="L38" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M38" s="4"/>
-      <c r="N38" s="4"/>
+      <c r="M38" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="N38" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="O38" s="4"/>
       <c r="P38" s="5">
-        <v>43718</v>
+        <v>43714</v>
       </c>
       <c r="Q38" s="5">
-        <v>43718</v>
+        <v>43716</v>
       </c>
       <c r="R38" s="4" t="s">
         <v>7</v>
       </c>
       <c r="S38" s="4" t="str">
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
-        <v>N/A</v>
+        <v>Adequação ao escopo do projeto</v>
       </c>
       <c r="T38" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="U38" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B39" s="3"/>
       <c r="C39" s="3" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4" t="s">
-        <v>99</v>
+        <v>48</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>5</v>
@@ -4286,17 +4523,23 @@
         <v>43</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J39" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K39" s="4"/>
+      <c r="K39" s="4" t="s">
+        <v>129</v>
+      </c>
       <c r="L39" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M39" s="4"/>
-      <c r="N39" s="4"/>
+      <c r="M39" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="N39" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="O39" s="4"/>
       <c r="P39" s="5">
         <v>43718</v>
@@ -4312,23 +4555,23 @@
         <v>N/A</v>
       </c>
       <c r="T39" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="U39" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="40" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="3">
-        <v>11</v>
-      </c>
-      <c r="C40" s="3"/>
-      <c r="D40" s="11" t="s">
-        <v>77</v>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>81</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>5</v>
@@ -4336,18 +4579,24 @@
       <c r="H40" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I40" s="30" t="s">
-        <v>126</v>
+      <c r="I40" s="4" t="s">
+        <v>120</v>
       </c>
       <c r="J40" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K40" s="4"/>
+      <c r="K40" s="4" t="s">
+        <v>129</v>
+      </c>
       <c r="L40" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M40" s="4"/>
-      <c r="N40" s="4"/>
+      <c r="M40" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="N40" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="O40" s="4"/>
       <c r="P40" s="5">
         <v>43718</v>
@@ -4363,23 +4612,23 @@
         <v>N/A</v>
       </c>
       <c r="T40" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="U40" s="31" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="41" spans="2:21" s="20" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="3">
-        <v>12</v>
-      </c>
-      <c r="C41" s="3"/>
-      <c r="D41" s="11" t="s">
-        <v>80</v>
+        <v>118</v>
+      </c>
+      <c r="U40" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="3"/>
+      <c r="C41" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>82</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4" t="s">
-        <v>42</v>
+        <v>94</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>5</v>
@@ -4387,20 +4636,24 @@
       <c r="H41" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I41" s="30" t="s">
-        <v>126</v>
+      <c r="I41" s="4" t="s">
+        <v>120</v>
       </c>
       <c r="J41" s="4" t="s">
         <v>44</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>45</v>
+        <v>129</v>
       </c>
       <c r="L41" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M41" s="4"/>
-      <c r="N41" s="4"/>
+      <c r="M41" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="N41" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="O41" s="4"/>
       <c r="P41" s="5">
         <v>43718</v>
@@ -4409,30 +4662,30 @@
         <v>43718</v>
       </c>
       <c r="R41" s="4" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="S41" s="4" t="str">
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
       <c r="T41" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="U41" s="31" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="42" spans="2:21" s="20" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="3"/>
-      <c r="C42" s="3" t="s">
-        <v>113</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="U41" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="3">
+        <v>11</v>
+      </c>
+      <c r="C42" s="3"/>
       <c r="D42" s="11" t="s">
-        <v>112</v>
+        <v>73</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4" t="s">
-        <v>42</v>
+        <v>94</v>
       </c>
       <c r="G42" s="4" t="s">
         <v>5</v>
@@ -4440,20 +4693,24 @@
       <c r="H42" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I42" s="30" t="s">
-        <v>126</v>
+      <c r="I42" s="29" t="s">
+        <v>120</v>
       </c>
       <c r="J42" s="4" t="s">
         <v>44</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>45</v>
+        <v>131</v>
       </c>
       <c r="L42" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M42" s="4"/>
-      <c r="N42" s="4"/>
+      <c r="M42" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="N42" s="4">
+        <v>1</v>
+      </c>
       <c r="O42" s="4"/>
       <c r="P42" s="5">
         <v>43718</v>
@@ -4462,30 +4719,30 @@
         <v>43718</v>
       </c>
       <c r="R42" s="4" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="S42" s="4" t="str">
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
       <c r="T42" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="U42" s="31" t="s">
-        <v>79</v>
+        <v>118</v>
+      </c>
+      <c r="U42" s="30" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B43" s="3">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C43" s="3"/>
-      <c r="D43" s="10" t="s">
-        <v>88</v>
+      <c r="D43" s="11" t="s">
+        <v>128</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>5</v>
@@ -4493,18 +4750,24 @@
       <c r="H43" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I43" s="4" t="s">
-        <v>126</v>
+      <c r="I43" s="29" t="s">
+        <v>120</v>
       </c>
       <c r="J43" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K43" s="4"/>
+      <c r="K43" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="L43" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M43" s="4"/>
-      <c r="N43" s="4"/>
+      <c r="M43" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="N43" s="4" t="s">
+        <v>143</v>
+      </c>
       <c r="O43" s="4"/>
       <c r="P43" s="5">
         <v>43718</v>
@@ -4513,30 +4776,30 @@
         <v>43718</v>
       </c>
       <c r="R43" s="4" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="S43" s="4" t="str">
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
       <c r="T43" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="U43" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="44" spans="2:21" s="20" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="3">
-        <v>14</v>
-      </c>
-      <c r="C44" s="3"/>
-      <c r="D44" s="10" t="s">
-        <v>84</v>
+        <v>118</v>
+      </c>
+      <c r="U43" s="30" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="44" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="3"/>
+      <c r="C44" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>107</v>
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="4" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>5</v>
@@ -4544,17 +4807,21 @@
       <c r="H44" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I44" s="4" t="s">
-        <v>126</v>
+      <c r="I44" s="29" t="s">
+        <v>120</v>
       </c>
       <c r="J44" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K44" s="4"/>
+      <c r="K44" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="L44" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M44" s="4"/>
+      <c r="M44" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="N44" s="4"/>
       <c r="O44" s="4"/>
       <c r="P44" s="5">
@@ -4564,22 +4831,22 @@
         <v>43718</v>
       </c>
       <c r="R44" s="4" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="S44" s="4" t="str">
         <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
         <v>N/A</v>
       </c>
       <c r="T44" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="U44" s="4" t="s">
-        <v>47</v>
+        <v>118</v>
+      </c>
+      <c r="U44" s="30" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="45" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B45" s="3">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="10" t="s">
@@ -4587,7 +4854,7 @@
       </c>
       <c r="E45" s="4"/>
       <c r="F45" s="4" t="s">
-        <v>99</v>
+        <v>48</v>
       </c>
       <c r="G45" s="4" t="s">
         <v>5</v>
@@ -4596,16 +4863,20 @@
         <v>43</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="J45" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K45" s="4"/>
+      <c r="K45" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="L45" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M45" s="4"/>
+      <c r="M45" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="N45" s="4"/>
       <c r="O45" s="4"/>
       <c r="P45" s="5">
@@ -4622,21 +4893,23 @@
         <v>N/A</v>
       </c>
       <c r="T45" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="U45" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="46" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="3"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="46" spans="2:21" s="26" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="3">
+        <v>14</v>
+      </c>
       <c r="C46" s="3"/>
-      <c r="D46" s="46" t="s">
-        <v>74</v>
+      <c r="D46" s="10" t="s">
+        <v>79</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G46" s="4" t="s">
         <v>5</v>
@@ -4645,23 +4918,29 @@
         <v>43</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J46" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K46" s="4"/>
+      <c r="K46" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="L46" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M46" s="4"/>
-      <c r="N46" s="4"/>
+      <c r="M46" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="N46" s="4">
+        <v>14</v>
+      </c>
       <c r="O46" s="4"/>
       <c r="P46" s="5">
-        <v>43716</v>
+        <v>43718</v>
       </c>
       <c r="Q46" s="5">
-        <v>43716</v>
+        <v>43718</v>
       </c>
       <c r="R46" s="4" t="s">
         <v>7</v>
@@ -4671,21 +4950,23 @@
         <v>N/A</v>
       </c>
       <c r="T46" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="U46" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="47" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="3"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="2:21" s="26" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="3">
+        <v>15</v>
+      </c>
       <c r="C47" s="3"/>
-      <c r="D47" s="46" t="s">
-        <v>82</v>
+      <c r="D47" s="10" t="s">
+        <v>78</v>
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="4" t="s">
-        <v>99</v>
+        <v>48</v>
       </c>
       <c r="G47" s="4" t="s">
         <v>5</v>
@@ -4694,17 +4975,23 @@
         <v>43</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="J47" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K47" s="4"/>
+      <c r="K47" s="4" t="s">
+        <v>131</v>
+      </c>
       <c r="L47" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M47" s="4"/>
-      <c r="N47" s="4"/>
+      <c r="M47" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="N47" s="4" t="s">
+        <v>144</v>
+      </c>
       <c r="O47" s="4"/>
       <c r="P47" s="5">
         <v>43718</v>
@@ -4720,55 +5007,125 @@
         <v>N/A</v>
       </c>
       <c r="T47" s="4" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="U47" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="3"/>
+      <c r="B48" s="3">
+        <v>16</v>
+      </c>
       <c r="C48" s="3"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
-      <c r="I48" s="30"/>
-      <c r="J48" s="4"/>
-      <c r="K48" s="4"/>
-      <c r="L48" s="4"/>
-      <c r="M48" s="4"/>
-      <c r="N48" s="4"/>
-      <c r="O48" s="4"/>
-      <c r="P48" s="5"/>
-      <c r="Q48" s="4"/>
-      <c r="R48" s="4"/>
-      <c r="S48" s="4"/>
-      <c r="T48" s="10"/>
-      <c r="U48" s="31"/>
+      <c r="D48" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="E48" s="24"/>
+      <c r="F48" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="G48" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="H48" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="I48" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="J48" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="K48" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="L48" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="M48" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="N48" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="O48" s="24"/>
+      <c r="P48" s="25">
+        <v>43716</v>
+      </c>
+      <c r="Q48" s="25">
+        <v>43716</v>
+      </c>
+      <c r="R48" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="S48" s="24" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
+      <c r="T48" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="U48" s="24" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="49" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="3"/>
+      <c r="B49" s="3">
+        <v>17</v>
+      </c>
       <c r="C49" s="3"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
-      <c r="H49" s="4"/>
-      <c r="I49" s="30"/>
-      <c r="J49" s="4"/>
-      <c r="K49" s="4"/>
-      <c r="L49" s="4"/>
-      <c r="M49" s="4"/>
-      <c r="N49" s="4"/>
-      <c r="O49" s="4"/>
-      <c r="P49" s="5"/>
-      <c r="Q49" s="4"/>
-      <c r="R49" s="4"/>
-      <c r="S49" s="4"/>
-      <c r="T49" s="10"/>
-      <c r="U49" s="31"/>
+      <c r="D49" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="E49" s="24"/>
+      <c r="F49" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="G49" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="H49" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="I49" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="J49" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="K49" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="L49" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="M49" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="N49" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="O49" s="24"/>
+      <c r="P49" s="25">
+        <v>43718</v>
+      </c>
+      <c r="Q49" s="25">
+        <v>43718</v>
+      </c>
+      <c r="R49" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="S49" s="24" t="str">
+        <f>IF(requisitos[[#This Row],[Data da Criação]]&lt;&gt;requisitos[[#This Row],[Data Última Alteração]],"Adequação ao escopo do projeto","N/A")</f>
+        <v>N/A</v>
+      </c>
+      <c r="T49" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="U49" s="24" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="50" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B50" s="3"/>
@@ -4800,7 +5157,7 @@
       <c r="F51" s="4"/>
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
-      <c r="I51" s="30"/>
+      <c r="I51" s="29"/>
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
       <c r="L51" s="4"/>
@@ -4812,7 +5169,7 @@
       <c r="R51" s="4"/>
       <c r="S51" s="4"/>
       <c r="T51" s="10"/>
-      <c r="U51" s="31"/>
+      <c r="U51" s="30"/>
     </row>
     <row r="52" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B52" s="3"/>
@@ -4822,7 +5179,7 @@
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
-      <c r="I52" s="30"/>
+      <c r="I52" s="29"/>
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
@@ -4834,7 +5191,7 @@
       <c r="R52" s="4"/>
       <c r="S52" s="4"/>
       <c r="T52" s="10"/>
-      <c r="U52" s="31"/>
+      <c r="U52" s="30"/>
     </row>
     <row r="53" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B53" s="3"/>
@@ -4844,7 +5201,7 @@
       <c r="F53" s="4"/>
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
-      <c r="I53" s="30"/>
+      <c r="I53" s="29"/>
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
@@ -4856,7 +5213,7 @@
       <c r="R53" s="4"/>
       <c r="S53" s="4"/>
       <c r="T53" s="10"/>
-      <c r="U53" s="31"/>
+      <c r="U53" s="30"/>
     </row>
     <row r="54" spans="2:21" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B54" s="3"/>
@@ -5210,10 +5567,8 @@
       <c r="T69" s="10"/>
       <c r="U69" s="4"/>
     </row>
-    <row r="70" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="N70" s="21"/>
-    </row>
-    <row r="71" spans="2:21" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="70" spans="2:21" x14ac:dyDescent="0.2"/>
+    <row r="71" spans="2:21" x14ac:dyDescent="0.2"/>
     <row r="72" spans="2:21" x14ac:dyDescent="0.2"/>
     <row r="73" spans="2:21" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -5231,37 +5586,40 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U54:U69 U50 U5:U47">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U54:U69 U5:U50" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Proposto,Aprovado,Projetado,Implementado,Verificado, Entregue, Eliminado, Rejeitado"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I54:I69 I50 I5:I47">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I54:I69 I5:I50" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Máxima,Alta,Média,Baixa,Mínima"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H54:H69 H50 H5:H47">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H54:H69 H5:H50" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"Funcional,Não Funcional"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J54:J69 L43:L45 J50 L47 J5:J47 L37:L39">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J54:J69 J5:J50 L45:L47 L49 L39:L41" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>"Gerson Santos,Célia Taniwaki,José Yoshihiro,Alex Barreira"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R54:R69 K54:K69 R50 K50 R5:R47 K5:K47">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R54:R69 K54:K69 R5:R50 K5:K50" xr:uid="{00000000-0002-0000-0100-000004000000}">
       <formula1>"Fernando Abreu,João Vinícius,Kessi Santana,Thalita Igwe,Vitoria Ferreira"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L40:L42 L54:L69 L50 L46 L5:L36">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5:L38 L54:L69 L50 L42:L44 L48" xr:uid="{00000000-0002-0000-0100-000005000000}">
       <formula1>"Gerson Santos,Fernando Abreu,João Vinícius,Kessi Santana,Thalita Igwe,Vitoria Ferreira,Célia Taniwaki,Alex Barreira,José Yoshihiro"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F54:F69 F50 F5:F47">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F54:F69 F5:F26 F28:F50" xr:uid="{00000000-0002-0000-0100-000006000000}">
       <formula1>"Essencial,Importante,Desejável"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="T5" r:id="rId1"/>
-    <hyperlink ref="T10" r:id="rId2"/>
-    <hyperlink ref="T11" r:id="rId3"/>
-    <hyperlink ref="T32" r:id="rId4"/>
+    <hyperlink ref="T5" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="T10" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="T11" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="T33" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId5"/>
   <headerFooter alignWithMargins="0"/>
+  <ignoredErrors>
+    <ignoredError sqref="N36:N41 N47:N49" twoDigitTextYear="1"/>
+  </ignoredErrors>
   <drawing r:id="rId6"/>
   <tableParts count="1">
     <tablePart r:id="rId7"/>

</xml_diff>